<commit_message>
[Douglas Giordano] - Atualização planilha de priorização de casos de uso, incrementos e responsabilidades.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -4,17 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Requisitos" sheetId="1" r:id="rId1"/>
+    <sheet name="Incremento 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Incremento 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Incremento 3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="138">
   <si>
     <t>ID</t>
   </si>
@@ -358,15 +361,6 @@
     <t>Priorização</t>
   </si>
   <si>
-    <t>Em Aberto</t>
-  </si>
-  <si>
-    <t>Realizado no Ciclo X</t>
-  </si>
-  <si>
-    <t>Em Implementação</t>
-  </si>
-  <si>
     <t>Responsável</t>
   </si>
   <si>
@@ -401,13 +395,49 @@
   </si>
   <si>
     <t>Finalizada</t>
+  </si>
+  <si>
+    <t>Parcialmente Finalizada</t>
+  </si>
+  <si>
+    <t>Pendente</t>
+  </si>
+  <si>
+    <t>Em Andamento</t>
+  </si>
+  <si>
+    <t>1+1</t>
+  </si>
+  <si>
+    <t>4.10</t>
+  </si>
+  <si>
+    <t>Horas Planejadas</t>
+  </si>
+  <si>
+    <t>Horas Realizadas</t>
+  </si>
+  <si>
+    <t>Recursos</t>
+  </si>
+  <si>
+    <t>Recurso</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Criar ata de julgamento da prova escrita</t>
+  </si>
+  <si>
+    <t>Casos de Uso Atrasados</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,6 +462,22 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -463,7 +509,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -592,11 +638,157 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -619,9 +811,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -660,6 +849,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -669,10 +876,99 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -977,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,161 +1285,173 @@
     <col min="2" max="2" width="73.140625" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="4" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.85546875" customWidth="1"/>
     <col min="9" max="9" width="28.85546875" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="H1" s="28" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="H1" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="28"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="I1" s="34"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="F2" s="20" t="s">
+      <c r="E2" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C3" s="18">
-        <v>4</v>
-      </c>
-      <c r="D3" s="18">
-        <v>1</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="H3" s="11">
-        <v>1</v>
-      </c>
-      <c r="I3" s="13">
+        <v>115</v>
+      </c>
+      <c r="C3" s="17">
+        <v>4</v>
+      </c>
+      <c r="D3" s="17">
+        <v>1</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3" s="10">
+        <v>1</v>
+      </c>
+      <c r="I3" s="12">
         <v>42019</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C4" s="18">
-        <v>4</v>
-      </c>
-      <c r="D4" s="18">
-        <v>1</v>
-      </c>
-      <c r="E4" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="17">
+        <v>4</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F4" s="29"/>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <v>2</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="12">
         <v>42026</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
-        <v>1</v>
-      </c>
-      <c r="B5" s="17" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="20">
+        <v>1</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="18">
-        <v>4</v>
-      </c>
-      <c r="D5" s="18">
-        <v>1</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F5" s="29"/>
-      <c r="H5" s="11">
+      <c r="C5" s="17">
+        <v>4</v>
+      </c>
+      <c r="D5" s="17">
+        <v>1</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="H5" s="10">
         <v>3</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="12">
         <v>42033</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
         <v>2</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="15">
-        <v>4</v>
-      </c>
-      <c r="D6" s="15">
-        <v>1</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="F6" s="16"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="14">
+        <v>4</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="26">
-        <v>4</v>
-      </c>
-      <c r="D7" s="26">
-        <v>1</v>
-      </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="27"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="B7" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="31">
+        <v>4</v>
+      </c>
+      <c r="D7" s="31">
+        <v>1</v>
+      </c>
+      <c r="E7" s="31"/>
+      <c r="F7" s="32"/>
+      <c r="H7" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="I7" s="34"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1156,14 +1464,22 @@
         <v>1</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1172,16 +1488,26 @@
       <c r="C9" s="4">
         <v>4</v>
       </c>
-      <c r="D9" s="4">
-        <v>1</v>
+      <c r="D9" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="I9" s="10">
+        <v>4</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1190,16 +1516,26 @@
       <c r="C10" s="4">
         <v>4</v>
       </c>
-      <c r="D10" s="4">
-        <v>1</v>
+      <c r="D10" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="I10" s="10">
+        <v>3</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1208,16 +1544,26 @@
       <c r="C11" s="4">
         <v>4</v>
       </c>
-      <c r="D11" s="4">
-        <v>1</v>
+      <c r="D11" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="I11" s="10">
+        <v>2</v>
+      </c>
+      <c r="J11" s="24"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1230,12 +1576,20 @@
         <v>1</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I12" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1244,16 +1598,20 @@
       <c r="C13" s="4">
         <v>4</v>
       </c>
-      <c r="D13" s="4">
-        <v>1</v>
+      <c r="D13" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1266,16 +1624,15 @@
         <v>1</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="H14" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="I14" s="28"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1284,40 +1641,32 @@
       <c r="C15" s="4">
         <v>4</v>
       </c>
-      <c r="D15" s="4">
-        <v>1</v>
+      <c r="D15" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F15" s="7"/>
-      <c r="H15" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="27"/>
-      <c r="H16" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="I16" s="11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1327,19 +1676,18 @@
         <v>4</v>
       </c>
       <c r="D17" s="4">
-        <v>1</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="7"/>
-      <c r="H17" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="I17" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1349,19 +1697,18 @@
         <v>4</v>
       </c>
       <c r="D18" s="4">
-        <v>1</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="7"/>
-      <c r="H18" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="I18" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
+      <c r="E18" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1371,19 +1718,18 @@
         <v>4</v>
       </c>
       <c r="D19" s="4">
-        <v>1</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="7"/>
-      <c r="H19" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="I19" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1393,13 +1739,18 @@
         <v>4</v>
       </c>
       <c r="D20" s="4">
-        <v>1</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1409,17 +1760,18 @@
         <v>4</v>
       </c>
       <c r="D21" s="4">
-        <v>1</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="7"/>
-      <c r="H21" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="I21" s="28"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1431,17 +1783,15 @@
       <c r="D22" s="4">
         <v>2</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="7"/>
-      <c r="H22" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
+      <c r="E22" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1453,17 +1803,15 @@
       <c r="D23" s="4">
         <v>2</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="7"/>
-      <c r="H23" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="I23" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
+      <c r="E23" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -1475,71 +1823,71 @@
       <c r="D24" s="4">
         <v>2</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="7"/>
-      <c r="H24" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="I24" s="11">
+      <c r="E24" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" s="27">
+        <v>4</v>
+      </c>
+      <c r="D25" s="27">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="E25" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="4">
-        <v>4</v>
-      </c>
-      <c r="D25" s="4">
+      <c r="C26" s="4">
+        <v>4</v>
+      </c>
+      <c r="D26" s="4">
         <v>2</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="7"/>
-      <c r="H25" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="I25" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
+      <c r="E26" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B27" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="27"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="32"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="C27" s="4">
-        <v>4</v>
-      </c>
-      <c r="D27" s="4">
-        <v>2</v>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="C28" s="4">
         <v>4</v>
@@ -1548,14 +1896,16 @@
         <v>2</v>
       </c>
       <c r="E28" s="4"/>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
-        <v>44</v>
+      <c r="F28" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>42</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C29" s="4">
         <v>4</v>
@@ -1564,294 +1914,298 @@
         <v>2</v>
       </c>
       <c r="E29" s="4"/>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
+      <c r="F29" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="4">
+        <v>4</v>
+      </c>
+      <c r="D30" s="4">
+        <v>2</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B31" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="27"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="32"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="4">
-        <v>4</v>
-      </c>
-      <c r="D31" s="4">
-        <v>2</v>
-      </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="C32" s="4">
         <v>4</v>
       </c>
       <c r="D32" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="7"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="23" t="s">
-        <v>49</v>
+      <c r="A33" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" s="4">
         <v>4</v>
       </c>
-      <c r="D33" s="4">
-        <v>2</v>
+      <c r="D33" s="27">
+        <v>0</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
-        <v>50</v>
+      <c r="A34" s="22" t="s">
+        <v>49</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" s="4">
         <v>4</v>
       </c>
-      <c r="D34" s="4">
-        <v>2</v>
+      <c r="D34" s="27">
+        <v>0</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="7"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
-        <v>51</v>
+      <c r="A35" s="22" t="s">
+        <v>50</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C35" s="4">
         <v>4</v>
       </c>
-      <c r="D35" s="4">
-        <v>2</v>
+      <c r="D35" s="27">
+        <v>0</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
-        <v>52</v>
+      <c r="A36" s="22" t="s">
+        <v>51</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C36" s="4">
         <v>4</v>
       </c>
-      <c r="D36" s="4">
-        <v>2</v>
+      <c r="D36" s="27">
+        <v>0</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="23" t="s">
-        <v>53</v>
+      <c r="A37" s="22" t="s">
+        <v>52</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C37" s="4">
         <v>4</v>
       </c>
-      <c r="D37" s="4">
-        <v>2</v>
+      <c r="D37" s="27">
+        <v>0</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="7"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
-        <v>54</v>
+      <c r="A38" s="22" t="s">
+        <v>53</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C38" s="4">
         <v>4</v>
       </c>
-      <c r="D38" s="4">
-        <v>2</v>
+      <c r="D38" s="27">
+        <v>0</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="7"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="23" t="s">
-        <v>55</v>
+      <c r="A39" s="22" t="s">
+        <v>54</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C39" s="4">
         <v>4</v>
       </c>
-      <c r="D39" s="4">
-        <v>2</v>
+      <c r="D39" s="27">
+        <v>0</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="7"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="23" t="s">
-        <v>56</v>
+      <c r="A40" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C40" s="4">
         <v>4</v>
       </c>
-      <c r="D40" s="4">
-        <v>2</v>
+      <c r="D40" s="27">
+        <v>0</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="7"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
-        <v>57</v>
+      <c r="A41" s="22" t="s">
+        <v>56</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C41" s="4">
         <v>4</v>
       </c>
-      <c r="D41" s="4">
-        <v>2</v>
+      <c r="D41" s="27">
+        <v>0</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="7"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="23" t="s">
-        <v>58</v>
+      <c r="A42" s="22" t="s">
+        <v>57</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C42" s="4">
         <v>4</v>
       </c>
-      <c r="D42" s="4">
-        <v>2</v>
+      <c r="D42" s="27">
+        <v>0</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="7"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="23" t="s">
-        <v>59</v>
+      <c r="A43" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" s="4">
         <v>4</v>
       </c>
-      <c r="D43" s="4">
-        <v>3</v>
+      <c r="D43" s="27">
+        <v>0</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="7"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="23" t="s">
-        <v>75</v>
+      <c r="A44" s="22" t="s">
+        <v>59</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C44" s="4">
         <v>4</v>
       </c>
-      <c r="D44" s="4">
-        <v>3</v>
+      <c r="D44" s="27">
+        <v>0</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="7"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="23" t="s">
-        <v>76</v>
+      <c r="A45" s="22" t="s">
+        <v>75</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C45" s="4">
         <v>4</v>
       </c>
-      <c r="D45" s="4">
-        <v>3</v>
+      <c r="D45" s="27">
+        <v>0</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="7"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="9">
+      <c r="A46" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46" s="4">
+        <v>4</v>
+      </c>
+      <c r="D46" s="27">
+        <v>0</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B46" s="25" t="s">
+      <c r="B47" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="27"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="23" t="s">
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="32"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="C47" s="4">
-        <v>4</v>
-      </c>
-      <c r="D47" s="4">
-        <v>3</v>
-      </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="7"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="C48" s="4">
         <v>4</v>
@@ -1863,11 +2217,11 @@
       <c r="F48" s="7"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="23" t="s">
-        <v>87</v>
+      <c r="A49" s="22" t="s">
+        <v>86</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C49" s="4">
         <v>4</v>
@@ -1879,11 +2233,11 @@
       <c r="F49" s="7"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="23" t="s">
-        <v>88</v>
+      <c r="A50" s="22" t="s">
+        <v>87</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C50" s="4">
         <v>4</v>
@@ -1895,11 +2249,11 @@
       <c r="F50" s="7"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="23" t="s">
-        <v>89</v>
+      <c r="A51" s="22" t="s">
+        <v>88</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C51" s="4">
         <v>4</v>
@@ -1911,11 +2265,11 @@
       <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="23" t="s">
-        <v>90</v>
+      <c r="A52" s="22" t="s">
+        <v>89</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C52" s="4">
         <v>4</v>
@@ -1927,11 +2281,11 @@
       <c r="F52" s="7"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="23" t="s">
-        <v>91</v>
+      <c r="A53" s="22" t="s">
+        <v>90</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C53" s="4">
         <v>4</v>
@@ -1943,39 +2297,39 @@
       <c r="F53" s="7"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="9">
+      <c r="A54" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C54" s="4">
+        <v>4</v>
+      </c>
+      <c r="D54" s="4">
+        <v>3</v>
+      </c>
+      <c r="E54" s="4"/>
+      <c r="F54" s="7"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B54" s="25" t="s">
+      <c r="B55" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="27"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="23" t="s">
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="32"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B56" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="C55" s="4">
-        <v>4</v>
-      </c>
-      <c r="D55" s="4">
-        <v>3</v>
-      </c>
-      <c r="E55" s="4"/>
-      <c r="F55" s="7"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="C56" s="4">
         <v>4</v>
@@ -1987,11 +2341,11 @@
       <c r="F56" s="7"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="23" t="s">
-        <v>99</v>
+      <c r="A57" s="22" t="s">
+        <v>98</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C57" s="4">
         <v>4</v>
@@ -2003,35 +2357,1272 @@
       <c r="F57" s="7"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="24" t="s">
+      <c r="A58" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C58" s="4">
+        <v>4</v>
+      </c>
+      <c r="D58" s="4">
+        <v>3</v>
+      </c>
+      <c r="E58" s="4"/>
+      <c r="F58" s="7"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B59" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="6">
-        <v>4</v>
-      </c>
-      <c r="D58" s="6">
+      <c r="C59" s="6">
+        <v>4</v>
+      </c>
+      <c r="D59" s="6">
         <v>3</v>
       </c>
-      <c r="E58" s="6"/>
-      <c r="F58" s="8"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="A1:F1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H7:I7"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="68.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="40"/>
+      <c r="I1" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="43">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="17">
+        <v>4</v>
+      </c>
+      <c r="D3" s="17">
+        <v>1</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" s="44">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="J3" s="25">
+        <v>8</v>
+      </c>
+      <c r="K3" s="25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="43">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="17">
+        <v>4</v>
+      </c>
+      <c r="D4" s="17">
+        <v>1</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="45">
+        <v>0.25</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="J4" s="25">
+        <v>12</v>
+      </c>
+      <c r="K4" s="25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="46">
+        <v>1</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="17">
+        <v>4</v>
+      </c>
+      <c r="D5" s="17">
+        <v>1</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G5" s="45">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="J5" s="25">
+        <v>8</v>
+      </c>
+      <c r="K5" s="25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="47">
+        <v>2</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="14">
+        <v>4</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="G6" s="48">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="J6" s="25">
+        <v>8</v>
+      </c>
+      <c r="K6" s="25">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="49">
+        <v>3</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="31">
+        <v>4</v>
+      </c>
+      <c r="D7" s="31">
+        <v>1</v>
+      </c>
+      <c r="E7" s="31"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="50"/>
+      <c r="I7" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="J7" s="25">
+        <v>8</v>
+      </c>
+      <c r="K7" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="27">
+        <v>4</v>
+      </c>
+      <c r="D8" s="27">
+        <v>1</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G8" s="45">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="J8" s="25">
+        <v>8</v>
+      </c>
+      <c r="K8" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="27">
+        <v>4</v>
+      </c>
+      <c r="D9" s="27">
+        <v>1</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="45">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="J9" s="25">
+        <v>6</v>
+      </c>
+      <c r="K9" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="27">
+        <v>4</v>
+      </c>
+      <c r="D10" s="27">
+        <v>1</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" s="45">
+        <v>0.3125</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="J10" s="25">
+        <v>10</v>
+      </c>
+      <c r="K10" s="25">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="27">
+        <v>4</v>
+      </c>
+      <c r="D11" s="27">
+        <v>1</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G11" s="45">
+        <v>0.125</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="J11" s="28">
+        <f>SUM(J3:J10)</f>
+        <v>68</v>
+      </c>
+      <c r="K11" s="28">
+        <f>SUM(K3:K10)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="27">
+        <v>4</v>
+      </c>
+      <c r="D12" s="27">
+        <v>1</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" s="45">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="27">
+        <v>4</v>
+      </c>
+      <c r="D13" s="27">
+        <v>1</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G13" s="45">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="J13" s="25"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="27">
+        <v>4</v>
+      </c>
+      <c r="D14" s="27">
+        <v>1</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G14" s="45">
+        <v>0</v>
+      </c>
+      <c r="I14" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="53">
+        <v>4</v>
+      </c>
+      <c r="D15" s="53">
+        <v>1</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="F15" s="54" t="s">
+        <v>128</v>
+      </c>
+      <c r="G15" s="55">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="J15" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="K15" s="25"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D16" s="14"/>
+      <c r="I16" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="J16" s="25">
+        <v>5</v>
+      </c>
+      <c r="K16" s="25"/>
+    </row>
+    <row r="17" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I17" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="J17" s="25">
+        <v>3</v>
+      </c>
+      <c r="K17" s="25"/>
+    </row>
+    <row r="18" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I18" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="J18" s="25">
+        <v>3</v>
+      </c>
+      <c r="K18" s="25"/>
+    </row>
+    <row r="19" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I19" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="J19" s="25">
+        <v>1</v>
+      </c>
+      <c r="K19" s="25"/>
+    </row>
+    <row r="20" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I20" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="J20" s="28">
+        <f>SUM(J16:J19)</f>
+        <v>12</v>
+      </c>
+      <c r="K20" s="28"/>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="WyV5OP1vdJ+VpaEHlVcyqGqxbvUgHqbmYqQTvlIwjIpyt6jDn4JOk/CVVGzQtywhsZxv3DB7EClluZWRoYEn9Q==" saltValue="NNQmqwKB65TUdkDPEPfL2w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I14:K14"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="40"/>
+      <c r="I1" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="49">
+        <v>4</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="64"/>
+      <c r="I3" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="J3" s="25">
+        <v>8</v>
+      </c>
+      <c r="K3" s="25"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="27">
+        <v>4</v>
+      </c>
+      <c r="D4" s="27">
+        <v>2</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" s="58"/>
+      <c r="I4" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="J4" s="25">
+        <v>12</v>
+      </c>
+      <c r="K4" s="25"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="27">
+        <v>4</v>
+      </c>
+      <c r="D5" s="27">
+        <v>2</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G5" s="58"/>
+      <c r="I5" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="J5" s="25">
+        <v>8</v>
+      </c>
+      <c r="K5" s="25"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="27">
+        <v>4</v>
+      </c>
+      <c r="D6" s="27">
+        <v>2</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G6" s="59"/>
+      <c r="I6" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="J6" s="25">
+        <v>8</v>
+      </c>
+      <c r="K6" s="25"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="27">
+        <v>4</v>
+      </c>
+      <c r="D7" s="27">
+        <v>2</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G7" s="59"/>
+      <c r="I7" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="J7" s="25">
+        <v>8</v>
+      </c>
+      <c r="K7" s="25"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="27">
+        <v>4</v>
+      </c>
+      <c r="D8" s="27">
+        <v>2</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G8" s="58"/>
+      <c r="I8" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="J8" s="25">
+        <v>8</v>
+      </c>
+      <c r="K8" s="25"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="27">
+        <v>4</v>
+      </c>
+      <c r="D9" s="27">
+        <v>2</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G9" s="58"/>
+      <c r="I9" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="J9" s="25">
+        <v>6</v>
+      </c>
+      <c r="K9" s="25"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="27">
+        <v>4</v>
+      </c>
+      <c r="D10" s="27">
+        <v>2</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G10" s="58"/>
+      <c r="I10" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="J10" s="25">
+        <v>10</v>
+      </c>
+      <c r="K10" s="25"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="27">
+        <v>4</v>
+      </c>
+      <c r="D11" s="27">
+        <v>2</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G11" s="58"/>
+      <c r="I11" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="J11" s="28">
+        <f>SUM(J3:J10)</f>
+        <v>68</v>
+      </c>
+      <c r="K11" s="28">
+        <f>SUM(K3:K10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="27">
+        <v>4</v>
+      </c>
+      <c r="D12" s="27">
+        <v>2</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G12" s="58"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="27">
+        <v>4</v>
+      </c>
+      <c r="D13" s="27">
+        <v>2</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G13" s="58"/>
+      <c r="J13" s="25"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>5</v>
+      </c>
+      <c r="B14" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="I14" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="27">
+        <v>4</v>
+      </c>
+      <c r="D15" s="27">
+        <v>2</v>
+      </c>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G15" s="58"/>
+      <c r="I15" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="J15" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="K15" s="25"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="27">
+        <v>4</v>
+      </c>
+      <c r="D16" s="27">
+        <v>2</v>
+      </c>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G16" s="60"/>
+      <c r="I16" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="J16" s="25">
+        <v>0</v>
+      </c>
+      <c r="K16" s="25"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="53">
+        <v>4</v>
+      </c>
+      <c r="D17" s="53">
+        <v>2</v>
+      </c>
+      <c r="E17" s="53"/>
+      <c r="F17" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G17" s="61"/>
+      <c r="I17" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="J17" s="25">
+        <v>3</v>
+      </c>
+      <c r="K17" s="25"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I18" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="J18" s="25">
+        <v>3</v>
+      </c>
+      <c r="K18" s="25"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="40"/>
+      <c r="I19" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="J19" s="25">
+        <v>14</v>
+      </c>
+      <c r="K19" s="25"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="J20" s="28">
+        <f>SUM(J16:J19)</f>
+        <v>20</v>
+      </c>
+      <c r="K20" s="28"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="43">
+        <v>0</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="17">
+        <v>4</v>
+      </c>
+      <c r="D21" s="17">
+        <v>1</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G21" s="45"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="49">
+        <v>3</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="31">
+        <v>4</v>
+      </c>
+      <c r="D22" s="31">
+        <v>1</v>
+      </c>
+      <c r="E22" s="31"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="50"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="27">
+        <v>4</v>
+      </c>
+      <c r="D23" s="27">
+        <v>1</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G23" s="45"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="27">
+        <v>4</v>
+      </c>
+      <c r="D24" s="27">
+        <v>1</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G24" s="45"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="27">
+        <v>4</v>
+      </c>
+      <c r="D25" s="27">
+        <v>1</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G25" s="45"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="27">
+        <v>4</v>
+      </c>
+      <c r="D26" s="27">
+        <v>1</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G26" s="45"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="27">
+        <v>4</v>
+      </c>
+      <c r="D27" s="27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G27" s="45"/>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="53">
+        <v>4</v>
+      </c>
+      <c r="D28" s="53">
+        <v>1</v>
+      </c>
+      <c r="E28" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="F28" s="54" t="s">
+        <v>128</v>
+      </c>
+      <c r="G28" s="55"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I14:K14"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Pedro Silva] - Escolhendo o meu incremento.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="138">
   <si>
     <t>ID</t>
   </si>
@@ -864,9 +864,66 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -882,81 +939,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -964,9 +967,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1293,18 +1293,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="H1" s="34" t="s">
+      <c r="A1" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="H1" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="34"/>
+      <c r="I1" s="55"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1434,21 +1434,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="31">
-        <v>4</v>
-      </c>
-      <c r="D7" s="31">
-        <v>1</v>
-      </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="32"/>
-      <c r="H7" s="34" t="s">
+      <c r="B7" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="52">
+        <v>4</v>
+      </c>
+      <c r="D7" s="52">
+        <v>1</v>
+      </c>
+      <c r="E7" s="52"/>
+      <c r="F7" s="53"/>
+      <c r="H7" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="34"/>
+      <c r="I7" s="55"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1607,8 +1607,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="56"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1656,13 +1656,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="53"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1874,13 +1874,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="32"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="53"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -1940,13 +1940,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="32"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="53"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2192,13 +2192,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="30" t="s">
+      <c r="B47" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="32"/>
+      <c r="C47" s="52"/>
+      <c r="D47" s="52"/>
+      <c r="E47" s="52"/>
+      <c r="F47" s="53"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2316,13 +2316,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="30" t="s">
+      <c r="B55" s="51" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="31"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="31"/>
-      <c r="F55" s="32"/>
+      <c r="C55" s="52"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="52"/>
+      <c r="F55" s="53"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2390,6 +2390,9 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B31:F31"/>
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B55:F55"/>
     <mergeCell ref="A1:F1"/>
@@ -2397,9 +2400,6 @@
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B7:F7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2428,23 +2428,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="40"/>
-      <c r="I1" s="35" t="s">
+      <c r="A1" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="30"/>
+      <c r="I1" s="59" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -2462,7 +2462,7 @@
       <c r="F2" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="32" t="s">
         <v>132</v>
       </c>
       <c r="I2" s="28" t="s">
@@ -2476,7 +2476,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="43">
+      <c r="A3" s="33">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -2494,7 +2494,7 @@
       <c r="F3" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="G3" s="44">
+      <c r="G3" s="34">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="I3" s="25" t="s">
@@ -2508,7 +2508,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="43">
+      <c r="A4" s="33">
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -2526,7 +2526,7 @@
       <c r="F4" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G4" s="45">
+      <c r="G4" s="35">
         <v>0.25</v>
       </c>
       <c r="I4" s="25" t="s">
@@ -2540,7 +2540,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="46">
+      <c r="A5" s="36">
         <v>1</v>
       </c>
       <c r="B5" s="16" t="s">
@@ -2558,7 +2558,7 @@
       <c r="F5" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="G5" s="45">
+      <c r="G5" s="35">
         <v>0.16666666666666666</v>
       </c>
       <c r="I5" s="25" t="s">
@@ -2572,7 +2572,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="47">
+      <c r="A6" s="37">
         <v>2</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -2590,7 +2590,7 @@
       <c r="F6" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="G6" s="48">
+      <c r="G6" s="38">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I6" s="25" t="s">
@@ -2604,21 +2604,21 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="49">
+      <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="31">
-        <v>4</v>
-      </c>
-      <c r="D7" s="31">
-        <v>1</v>
-      </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="50"/>
+      <c r="B7" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="52">
+        <v>4</v>
+      </c>
+      <c r="D7" s="52">
+        <v>1</v>
+      </c>
+      <c r="E7" s="52"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
       </c>
@@ -2630,7 +2630,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="33" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -2648,7 +2648,7 @@
       <c r="F8" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="G8" s="45">
+      <c r="G8" s="35">
         <v>0.16666666666666666</v>
       </c>
       <c r="I8" s="25" t="s">
@@ -2662,7 +2662,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="33" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2680,7 +2680,7 @@
       <c r="F9" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G9" s="45">
+      <c r="G9" s="35">
         <v>0.22916666666666666</v>
       </c>
       <c r="I9" s="25" t="s">
@@ -2694,7 +2694,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -2712,7 +2712,7 @@
       <c r="F10" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G10" s="45">
+      <c r="G10" s="35">
         <v>0.3125</v>
       </c>
       <c r="I10" s="25" t="s">
@@ -2726,7 +2726,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="33" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2744,7 +2744,7 @@
       <c r="F11" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="G11" s="45">
+      <c r="G11" s="35">
         <v>0.125</v>
       </c>
       <c r="I11" s="28" t="s">
@@ -2760,7 +2760,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="33" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -2778,12 +2778,12 @@
       <c r="F12" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="G12" s="45">
+      <c r="G12" s="35">
         <v>0.125</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="33" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -2801,13 +2801,13 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="G13" s="45">
+      <c r="G13" s="35">
         <v>0.16666666666666666</v>
       </c>
       <c r="J13" s="25"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="33" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -2825,35 +2825,35 @@
       <c r="F14" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="G14" s="45">
+      <c r="G14" s="35">
         <v>0</v>
       </c>
-      <c r="I14" s="35" t="s">
+      <c r="I14" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="53">
-        <v>4</v>
-      </c>
-      <c r="D15" s="53">
-        <v>1</v>
-      </c>
-      <c r="E15" s="53" t="s">
+      <c r="C15" s="43">
+        <v>4</v>
+      </c>
+      <c r="D15" s="43">
+        <v>1</v>
+      </c>
+      <c r="E15" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="F15" s="54" t="s">
+      <c r="F15" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="G15" s="55">
+      <c r="G15" s="45">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="I15" s="25" t="s">
@@ -2893,7 +2893,7 @@
       <c r="K18" s="25"/>
     </row>
     <row r="19" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I19" s="37" t="s">
+      <c r="I19" s="29" t="s">
         <v>127</v>
       </c>
       <c r="J19" s="25">
@@ -2928,8 +2928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2945,23 +2945,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="40"/>
-      <c r="I1" s="35" t="s">
+      <c r="A1" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="30"/>
+      <c r="I1" s="59" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -2976,10 +2976,10 @@
       <c r="E2" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="32" t="s">
         <v>132</v>
       </c>
       <c r="I2" s="28" t="s">
@@ -2993,17 +2993,17 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="49">
-        <v>4</v>
-      </c>
-      <c r="B3" s="62" t="s">
+      <c r="A3" s="39">
+        <v>4</v>
+      </c>
+      <c r="B3" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="65"/>
       <c r="I3" s="25" t="s">
         <v>118</v>
       </c>
@@ -3013,7 +3013,7 @@
       <c r="K3" s="25"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="33" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -3031,7 +3031,7 @@
       <c r="F4" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G4" s="58"/>
+      <c r="G4" s="47"/>
       <c r="I4" s="25" t="s">
         <v>117</v>
       </c>
@@ -3041,7 +3041,7 @@
       <c r="K4" s="25"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="33" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -3059,7 +3059,7 @@
       <c r="F5" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G5" s="58"/>
+      <c r="G5" s="47"/>
       <c r="I5" s="25" t="s">
         <v>123</v>
       </c>
@@ -3069,7 +3069,7 @@
       <c r="K5" s="25"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="33" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -3087,7 +3087,7 @@
       <c r="F6" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G6" s="59"/>
+      <c r="G6" s="48"/>
       <c r="I6" s="25" t="s">
         <v>121</v>
       </c>
@@ -3097,7 +3097,7 @@
       <c r="K6" s="25"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="33" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -3115,7 +3115,7 @@
       <c r="F7" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G7" s="59"/>
+      <c r="G7" s="48"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
       </c>
@@ -3125,7 +3125,7 @@
       <c r="K7" s="25"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="33" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -3143,7 +3143,7 @@
       <c r="F8" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G8" s="58"/>
+      <c r="G8" s="47"/>
       <c r="I8" s="25" t="s">
         <v>124</v>
       </c>
@@ -3153,7 +3153,7 @@
       <c r="K8" s="25"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="33" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -3171,7 +3171,7 @@
       <c r="F9" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G9" s="58"/>
+      <c r="G9" s="47"/>
       <c r="I9" s="25" t="s">
         <v>119</v>
       </c>
@@ -3181,7 +3181,7 @@
       <c r="K9" s="25"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="33" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -3199,7 +3199,7 @@
       <c r="F10" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G10" s="58"/>
+      <c r="G10" s="47"/>
       <c r="I10" s="25" t="s">
         <v>120</v>
       </c>
@@ -3209,7 +3209,7 @@
       <c r="K10" s="25"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="33" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -3227,7 +3227,7 @@
       <c r="F11" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G11" s="58"/>
+      <c r="G11" s="47"/>
       <c r="I11" s="28" t="s">
         <v>135</v>
       </c>
@@ -3241,7 +3241,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="33" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -3259,10 +3259,10 @@
       <c r="F12" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G12" s="58"/>
+      <c r="G12" s="47"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="33" t="s">
         <v>130</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -3280,29 +3280,29 @@
       <c r="F13" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G13" s="58"/>
+      <c r="G13" s="47"/>
       <c r="J13" s="25"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>5</v>
       </c>
-      <c r="B14" s="65" t="s">
+      <c r="B14" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="I14" s="35" t="s">
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="I14" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="33" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -3314,11 +3314,13 @@
       <c r="D15" s="27">
         <v>2</v>
       </c>
-      <c r="E15" s="27"/>
+      <c r="E15" s="27" t="s">
+        <v>120</v>
+      </c>
       <c r="F15" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G15" s="58"/>
+      <c r="G15" s="47"/>
       <c r="I15" s="25" t="s">
         <v>103</v>
       </c>
@@ -3328,7 +3330,7 @@
       <c r="K15" s="25"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="33" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -3344,7 +3346,7 @@
       <c r="F16" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G16" s="60"/>
+      <c r="G16" s="49"/>
       <c r="I16" s="25" t="s">
         <v>125</v>
       </c>
@@ -3354,23 +3356,23 @@
       <c r="K16" s="25"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="53">
-        <v>4</v>
-      </c>
-      <c r="D17" s="53">
+      <c r="C17" s="43">
+        <v>4</v>
+      </c>
+      <c r="D17" s="43">
         <v>2</v>
       </c>
-      <c r="E17" s="53"/>
+      <c r="E17" s="43"/>
       <c r="F17" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G17" s="61"/>
+      <c r="G17" s="50"/>
       <c r="I17" s="25" t="s">
         <v>126</v>
       </c>
@@ -3389,16 +3391,16 @@
       <c r="K18" s="25"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="40"/>
-      <c r="I19" s="37" t="s">
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="30"/>
+      <c r="I19" s="29" t="s">
         <v>127</v>
       </c>
       <c r="J19" s="25">
@@ -3407,7 +3409,7 @@
       <c r="K19" s="25"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="19" t="s">
@@ -3425,7 +3427,7 @@
       <c r="F20" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="G20" s="42" t="s">
+      <c r="G20" s="32" t="s">
         <v>132</v>
       </c>
       <c r="I20" s="28" t="s">
@@ -3438,7 +3440,7 @@
       <c r="K20" s="28"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="43">
+      <c r="A21" s="33">
         <v>0</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -3456,27 +3458,27 @@
       <c r="F21" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G21" s="45"/>
+      <c r="G21" s="35"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="49">
+      <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="31">
-        <v>4</v>
-      </c>
-      <c r="D22" s="31">
-        <v>1</v>
-      </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="50"/>
+      <c r="B22" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="52">
+        <v>4</v>
+      </c>
+      <c r="D22" s="52">
+        <v>1</v>
+      </c>
+      <c r="E22" s="52"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="40"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="33" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -3494,10 +3496,10 @@
       <c r="F23" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G23" s="45"/>
+      <c r="G23" s="35"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -3515,10 +3517,10 @@
       <c r="F24" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G24" s="45"/>
+      <c r="G24" s="35"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="33" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -3536,10 +3538,10 @@
       <c r="F25" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="G25" s="45"/>
+      <c r="G25" s="35"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="33" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -3557,10 +3559,10 @@
       <c r="F26" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="G26" s="45"/>
+      <c r="G26" s="35"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="33" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -3578,38 +3580,38 @@
       <c r="F27" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="G27" s="45"/>
+      <c r="G27" s="35"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="52" t="s">
+      <c r="B28" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="53">
-        <v>4</v>
-      </c>
-      <c r="D28" s="53">
-        <v>1</v>
-      </c>
-      <c r="E28" s="53" t="s">
+      <c r="C28" s="43">
+        <v>4</v>
+      </c>
+      <c r="D28" s="43">
+        <v>1</v>
+      </c>
+      <c r="E28" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="F28" s="54" t="s">
+      <c r="F28" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="G28" s="55"/>
+      <c r="G28" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I14:K14"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B14:G14"/>
     <mergeCell ref="B3:G3"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I14:K14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
[Alex Becker] - Horas planejadas dos meus casos de uso do incremento II.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="139">
   <si>
     <t>ID</t>
   </si>
@@ -431,6 +431,9 @@
   </si>
   <si>
     <t>Casos de Uso Atrasados</t>
+  </si>
+  <si>
+    <t>Horas Disponíveis</t>
   </si>
 </sst>
 </file>
@@ -770,25 +773,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <left/>
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -913,9 +910,6 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -924,6 +918,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -939,9 +936,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -967,6 +961,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1276,7 +1279,7 @@
   <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,8 +1610,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="56"/>
-      <c r="K13" s="56"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -2390,16 +2393,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B7:F7"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B55:F55"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2410,8 +2413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2428,20 +2431,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
+      <c r="A1" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
       <c r="G1" s="30"/>
-      <c r="I1" s="59" t="s">
+      <c r="I1" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -2828,11 +2831,11 @@
       <c r="G14" s="35">
         <v>0</v>
       </c>
-      <c r="I14" s="59" t="s">
+      <c r="I14" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="41" t="s">
@@ -2926,10 +2929,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2938,29 +2941,31 @@
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="30"/>
-      <c r="I1" s="59" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="30"/>
+      <c r="J1" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
@@ -2976,43 +2981,47 @@
       <c r="E2" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="67" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="J2" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="J2" s="28" t="s">
-        <v>131</v>
-      </c>
       <c r="K2" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="L2" s="28" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="39">
         <v>4</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="65"/>
-      <c r="I3" s="25" t="s">
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="J3" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="J3" s="25">
+      <c r="K3" s="25">
         <v>8</v>
       </c>
-      <c r="K3" s="25"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="25"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>21</v>
       </c>
@@ -3031,16 +3040,17 @@
       <c r="F4" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G4" s="47"/>
-      <c r="I4" s="25" t="s">
+      <c r="G4" s="27"/>
+      <c r="H4" s="46"/>
+      <c r="J4" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="J4" s="25">
+      <c r="K4" s="25">
         <v>12</v>
       </c>
-      <c r="K4" s="25"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="25"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>22</v>
       </c>
@@ -3059,16 +3069,17 @@
       <c r="F5" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G5" s="47"/>
-      <c r="I5" s="25" t="s">
+      <c r="G5" s="27"/>
+      <c r="H5" s="46"/>
+      <c r="J5" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="J5" s="25">
+      <c r="K5" s="25">
         <v>8</v>
       </c>
-      <c r="K5" s="25"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="25"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>25</v>
       </c>
@@ -3087,16 +3098,17 @@
       <c r="F6" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G6" s="48"/>
-      <c r="I6" s="25" t="s">
+      <c r="G6" s="27"/>
+      <c r="H6" s="47"/>
+      <c r="J6" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="J6" s="25">
+      <c r="K6" s="25">
         <v>8</v>
       </c>
-      <c r="K6" s="25"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="25"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>27</v>
       </c>
@@ -3115,16 +3127,17 @@
       <c r="F7" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G7" s="48"/>
-      <c r="I7" s="25" t="s">
+      <c r="G7" s="27"/>
+      <c r="H7" s="47"/>
+      <c r="J7" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="J7" s="25">
+      <c r="K7" s="25">
         <v>8</v>
       </c>
-      <c r="K7" s="25"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="25"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>29</v>
       </c>
@@ -3143,16 +3156,17 @@
       <c r="F8" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G8" s="47"/>
-      <c r="I8" s="25" t="s">
+      <c r="G8" s="27"/>
+      <c r="H8" s="46"/>
+      <c r="J8" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="J8" s="25">
+      <c r="K8" s="25">
         <v>8</v>
       </c>
-      <c r="K8" s="25"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="25"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>31</v>
       </c>
@@ -3166,21 +3180,22 @@
         <v>2</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F9" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G9" s="47"/>
-      <c r="I9" s="25" t="s">
+      <c r="G9" s="27"/>
+      <c r="H9" s="46"/>
+      <c r="J9" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="J9" s="25">
+      <c r="K9" s="25">
         <v>6</v>
       </c>
-      <c r="K9" s="25"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="25"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>33</v>
       </c>
@@ -3199,16 +3214,17 @@
       <c r="F10" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G10" s="47"/>
-      <c r="I10" s="25" t="s">
+      <c r="G10" s="27"/>
+      <c r="H10" s="46"/>
+      <c r="J10" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="J10" s="25">
+      <c r="K10" s="25">
         <v>10</v>
       </c>
-      <c r="K10" s="25"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="25"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>35</v>
       </c>
@@ -3227,20 +3243,21 @@
       <c r="F11" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G11" s="47"/>
-      <c r="I11" s="28" t="s">
+      <c r="G11" s="27"/>
+      <c r="H11" s="46"/>
+      <c r="J11" s="28" t="s">
         <v>135</v>
-      </c>
-      <c r="J11" s="28">
-        <f>SUM(J3:J10)</f>
-        <v>68</v>
       </c>
       <c r="K11" s="28">
         <f>SUM(K3:K10)</f>
+        <v>68</v>
+      </c>
+      <c r="L11" s="28">
+        <f>SUM(L3:L10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
         <v>37</v>
       </c>
@@ -3259,9 +3276,12 @@
       <c r="F12" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G12" s="47"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G12" s="27">
+        <v>4</v>
+      </c>
+      <c r="H12" s="46"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>130</v>
       </c>
@@ -3275,33 +3295,37 @@
         <v>2</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F13" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G13" s="47"/>
-      <c r="J13" s="25"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G13" s="27">
+        <v>4</v>
+      </c>
+      <c r="H13" s="46"/>
+      <c r="K13" s="25"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>5</v>
       </c>
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="I14" s="59" t="s">
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="J14" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
         <v>40</v>
       </c>
@@ -3320,16 +3344,17 @@
       <c r="F15" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G15" s="47"/>
-      <c r="I15" s="25" t="s">
+      <c r="G15" s="27"/>
+      <c r="H15" s="46"/>
+      <c r="J15" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="J15" s="25" t="s">
+      <c r="K15" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K15" s="25"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="25"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>42</v>
       </c>
@@ -3346,16 +3371,17 @@
       <c r="F16" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G16" s="49"/>
-      <c r="I16" s="25" t="s">
+      <c r="G16" s="27"/>
+      <c r="H16" s="48"/>
+      <c r="J16" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="J16" s="25">
+      <c r="K16" s="25">
         <v>0</v>
       </c>
-      <c r="K16" s="25"/>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L16" s="25"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="41" t="s">
         <v>44</v>
       </c>
@@ -3369,46 +3395,48 @@
         <v>2</v>
       </c>
       <c r="E17" s="43"/>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="G17" s="50"/>
-      <c r="I17" s="25" t="s">
+      <c r="G17" s="6"/>
+      <c r="H17" s="49"/>
+      <c r="J17" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="J17" s="25">
+      <c r="K17" s="25">
         <v>3</v>
       </c>
-      <c r="K17" s="25"/>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I18" s="25" t="s">
+      <c r="L17" s="25"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="J18" s="25">
+      <c r="K18" s="25">
         <v>3</v>
       </c>
-      <c r="K18" s="25"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="57" t="s">
+      <c r="L18" s="25"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="30"/>
-      <c r="I19" s="29" t="s">
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="30"/>
+      <c r="J19" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="J19" s="25">
+      <c r="K19" s="25">
         <v>14</v>
       </c>
-      <c r="K19" s="25"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="25"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>0</v>
       </c>
@@ -3427,19 +3455,22 @@
       <c r="F20" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="G20" s="32" t="s">
+      <c r="G20" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="H20" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="I20" s="28" t="s">
+      <c r="J20" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="J20" s="28">
-        <f>SUM(J16:J19)</f>
+      <c r="K20" s="28">
+        <f>SUM(K16:K19)</f>
         <v>20</v>
       </c>
-      <c r="K20" s="28"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="28"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="33">
         <v>0</v>
       </c>
@@ -3458,9 +3489,10 @@
       <c r="F21" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G21" s="35"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G21" s="27"/>
+      <c r="H21" s="35"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="39">
         <v>3</v>
       </c>
@@ -3475,9 +3507,10 @@
       </c>
       <c r="E22" s="52"/>
       <c r="F22" s="53"/>
-      <c r="G22" s="40"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G22" s="51"/>
+      <c r="H22" s="52"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
         <v>7</v>
       </c>
@@ -3496,9 +3529,10 @@
       <c r="F23" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G23" s="35"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G23" s="27"/>
+      <c r="H23" s="35"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
         <v>9</v>
       </c>
@@ -3517,9 +3551,10 @@
       <c r="F24" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G24" s="35"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G24" s="27"/>
+      <c r="H24" s="35"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
         <v>11</v>
       </c>
@@ -3538,9 +3573,10 @@
       <c r="F25" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="G25" s="35"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G25" s="27"/>
+      <c r="H25" s="35"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
         <v>13</v>
       </c>
@@ -3559,9 +3595,10 @@
       <c r="F26" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="G26" s="35"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G26" s="27"/>
+      <c r="H26" s="35"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
         <v>16</v>
       </c>
@@ -3580,9 +3617,10 @@
       <c r="F27" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="G27" s="35"/>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G27" s="27"/>
+      <c r="H27" s="35"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="41" t="s">
         <v>18</v>
       </c>
@@ -3601,17 +3639,19 @@
       <c r="F28" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="G28" s="45"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I14:K14"/>
+  <mergeCells count="8">
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J14:L14"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="G22:H22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
[Pedro Silva] - Minhas horas planejadas preechidas
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -918,7 +918,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -930,10 +942,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -961,15 +970,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1296,18 +1296,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="H1" s="55" t="s">
+      <c r="A1" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="H1" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="55"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1437,21 +1437,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="52">
-        <v>4</v>
-      </c>
-      <c r="D7" s="52">
-        <v>1</v>
-      </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="53"/>
-      <c r="H7" s="55" t="s">
+      <c r="B7" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="56">
+        <v>4</v>
+      </c>
+      <c r="D7" s="56">
+        <v>1</v>
+      </c>
+      <c r="E7" s="56"/>
+      <c r="F7" s="57"/>
+      <c r="H7" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="55"/>
+      <c r="I7" s="54"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1610,8 +1610,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="50"/>
-      <c r="K13" s="50"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1659,13 +1659,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="53"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="57"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1877,13 +1877,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="53"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="57"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -1943,13 +1943,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="51" t="s">
+      <c r="B31" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="53"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="57"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2195,13 +2195,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="51" t="s">
+      <c r="B47" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="52"/>
-      <c r="D47" s="52"/>
-      <c r="E47" s="52"/>
-      <c r="F47" s="53"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="57"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2319,13 +2319,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="51" t="s">
+      <c r="B55" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="52"/>
-      <c r="D55" s="52"/>
-      <c r="E55" s="52"/>
-      <c r="F55" s="53"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="56"/>
+      <c r="F55" s="57"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2393,16 +2393,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B55:F55"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B7:F7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B55:F55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2431,20 +2431,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
+      <c r="A1" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
       <c r="G1" s="30"/>
-      <c r="I1" s="58" t="s">
+      <c r="I1" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -2610,17 +2610,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="52">
-        <v>4</v>
-      </c>
-      <c r="D7" s="52">
-        <v>1</v>
-      </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="53"/>
+      <c r="B7" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="56">
+        <v>4</v>
+      </c>
+      <c r="D7" s="56">
+        <v>1</v>
+      </c>
+      <c r="E7" s="56"/>
+      <c r="F7" s="57"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -2831,11 +2831,11 @@
       <c r="G14" s="35">
         <v>0</v>
       </c>
-      <c r="I14" s="58" t="s">
+      <c r="I14" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="59"/>
-      <c r="K14" s="59"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="62"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="41" t="s">
@@ -2932,7 +2932,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2949,21 +2949,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="65"/>
+      <c r="A1" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="50"/>
       <c r="H1" s="30"/>
-      <c r="J1" s="58" t="s">
+      <c r="J1" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -2981,7 +2981,7 @@
       <c r="E2" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="67" t="s">
+      <c r="F2" s="52" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="19" t="s">
@@ -3004,15 +3004,15 @@
       <c r="A3" s="39">
         <v>4</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
       <c r="J3" s="25" t="s">
         <v>118</v>
       </c>
@@ -3310,20 +3310,20 @@
       <c r="A14" s="9">
         <v>5</v>
       </c>
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="J14" s="58" t="s">
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="64"/>
+      <c r="J14" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="K14" s="59"/>
-      <c r="L14" s="59"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="62"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
@@ -3344,7 +3344,9 @@
       <c r="F15" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G15" s="27"/>
+      <c r="G15" s="27">
+        <v>7</v>
+      </c>
       <c r="H15" s="46"/>
       <c r="J15" s="25" t="s">
         <v>103</v>
@@ -3418,15 +3420,15 @@
       <c r="L18" s="25"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="66"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="51"/>
       <c r="H19" s="30"/>
       <c r="J19" s="29" t="s">
         <v>127</v>
@@ -3496,19 +3498,19 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="52">
-        <v>4</v>
-      </c>
-      <c r="D22" s="52">
-        <v>1</v>
-      </c>
-      <c r="E22" s="52"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="52"/>
+      <c r="B22" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="56">
+        <v>4</v>
+      </c>
+      <c r="D22" s="56">
+        <v>1</v>
+      </c>
+      <c r="E22" s="56"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="56"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -3551,7 +3553,9 @@
       <c r="F24" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G24" s="27"/>
+      <c r="G24" s="27">
+        <v>3</v>
+      </c>
       <c r="H24" s="35"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Edison Moura] Documento de controle de horas de trabalho alimentado.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="140">
   <si>
     <t>ID</t>
   </si>
@@ -434,6 +434,9 @@
   </si>
   <si>
     <t>Horas Disponíveis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 01:00:00</t>
   </si>
 </sst>
 </file>
@@ -785,7 +788,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -927,10 +930,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -942,7 +942,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -970,6 +973,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1296,18 +1302,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="H1" s="54" t="s">
+      <c r="A1" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="H1" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="54"/>
+      <c r="I1" s="58"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1437,21 +1443,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="56">
-        <v>4</v>
-      </c>
-      <c r="D7" s="56">
-        <v>1</v>
-      </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="57"/>
-      <c r="H7" s="54" t="s">
+      <c r="B7" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="55">
+        <v>4</v>
+      </c>
+      <c r="D7" s="55">
+        <v>1</v>
+      </c>
+      <c r="E7" s="55"/>
+      <c r="F7" s="56"/>
+      <c r="H7" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="54"/>
+      <c r="I7" s="58"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1610,8 +1616,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="58"/>
-      <c r="K13" s="58"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1659,13 +1665,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="57"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="56"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1877,13 +1883,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="57"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="56"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -1943,13 +1949,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="55" t="s">
+      <c r="B31" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="57"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="56"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2195,13 +2201,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="55" t="s">
+      <c r="B47" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="56"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="57"/>
+      <c r="C47" s="55"/>
+      <c r="D47" s="55"/>
+      <c r="E47" s="55"/>
+      <c r="F47" s="56"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2319,13 +2325,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="55" t="s">
+      <c r="B55" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="56"/>
-      <c r="D55" s="56"/>
-      <c r="E55" s="56"/>
-      <c r="F55" s="57"/>
+      <c r="C55" s="55"/>
+      <c r="D55" s="55"/>
+      <c r="E55" s="55"/>
+      <c r="F55" s="56"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2393,16 +2399,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B7:F7"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B55:F55"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2414,7 +2420,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2610,17 +2616,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="56">
-        <v>4</v>
-      </c>
-      <c r="D7" s="56">
-        <v>1</v>
-      </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="57"/>
+      <c r="B7" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="55">
+        <v>4</v>
+      </c>
+      <c r="D7" s="55">
+        <v>1</v>
+      </c>
+      <c r="E7" s="55"/>
+      <c r="F7" s="56"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -2931,8 +2937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3193,7 +3199,9 @@
       <c r="K9" s="25">
         <v>6</v>
       </c>
-      <c r="L9" s="25"/>
+      <c r="L9" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
@@ -3254,7 +3262,7 @@
       </c>
       <c r="L11" s="28">
         <f>SUM(L3:L10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3498,19 +3506,19 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="56">
-        <v>4</v>
-      </c>
-      <c r="D22" s="56">
-        <v>1</v>
-      </c>
-      <c r="E22" s="56"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="56"/>
+      <c r="B22" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="55">
+        <v>4</v>
+      </c>
+      <c r="D22" s="55">
+        <v>1</v>
+      </c>
+      <c r="E22" s="55"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="55"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -3597,10 +3605,14 @@
         <v>119</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G26" s="27"/>
-      <c r="H26" s="35"/>
+        <v>126</v>
+      </c>
+      <c r="G26" s="27">
+        <v>3</v>
+      </c>
+      <c r="H26" s="68" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">

</xml_diff>

<commit_message>
[Douglas Giordano] - Atualização documento de controle de horas.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Requisitos" sheetId="1" r:id="rId1"/>
@@ -930,7 +930,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -942,10 +948,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -973,9 +976,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1284,7 +1284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -1302,18 +1302,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="H1" s="58" t="s">
+      <c r="A1" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="H1" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="58"/>
+      <c r="I1" s="55"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1443,21 +1443,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="55">
-        <v>4</v>
-      </c>
-      <c r="D7" s="55">
-        <v>1</v>
-      </c>
-      <c r="E7" s="55"/>
-      <c r="F7" s="56"/>
-      <c r="H7" s="58" t="s">
+      <c r="B7" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="57">
+        <v>4</v>
+      </c>
+      <c r="D7" s="57">
+        <v>1</v>
+      </c>
+      <c r="E7" s="57"/>
+      <c r="F7" s="58"/>
+      <c r="H7" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="58"/>
+      <c r="I7" s="55"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1616,8 +1616,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1665,13 +1665,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="56"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="58"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1883,13 +1883,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="54" t="s">
+      <c r="B27" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="56"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="58"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -1949,13 +1949,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="54" t="s">
+      <c r="B31" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="56"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="58"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2201,13 +2201,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="54" t="s">
+      <c r="B47" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="55"/>
-      <c r="D47" s="55"/>
-      <c r="E47" s="55"/>
-      <c r="F47" s="56"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="58"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2325,13 +2325,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="54" t="s">
+      <c r="B55" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="55"/>
-      <c r="D55" s="55"/>
-      <c r="E55" s="55"/>
-      <c r="F55" s="56"/>
+      <c r="C55" s="57"/>
+      <c r="D55" s="57"/>
+      <c r="E55" s="57"/>
+      <c r="F55" s="58"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2399,16 +2399,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B55:F55"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B7:F7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B55:F55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2437,20 +2437,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
+      <c r="A1" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
       <c r="G1" s="30"/>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -2616,17 +2616,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="55">
-        <v>4</v>
-      </c>
-      <c r="D7" s="55">
-        <v>1</v>
-      </c>
-      <c r="E7" s="55"/>
-      <c r="F7" s="56"/>
+      <c r="B7" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="57">
+        <v>4</v>
+      </c>
+      <c r="D7" s="57">
+        <v>1</v>
+      </c>
+      <c r="E7" s="57"/>
+      <c r="F7" s="58"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -2837,11 +2837,11 @@
       <c r="G14" s="35">
         <v>0</v>
       </c>
-      <c r="I14" s="61" t="s">
+      <c r="I14" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="62"/>
-      <c r="K14" s="62"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="41" t="s">
@@ -2937,8 +2937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2955,21 +2955,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="63"/>
+      <c r="A1" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="64"/>
       <c r="G1" s="50"/>
       <c r="H1" s="30"/>
-      <c r="J1" s="61" t="s">
+      <c r="J1" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -3010,15 +3010,15 @@
       <c r="A3" s="39">
         <v>4</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="68"/>
       <c r="J3" s="25" t="s">
         <v>118</v>
       </c>
@@ -3222,7 +3222,9 @@
       <c r="F10" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G10" s="27"/>
+      <c r="G10" s="27">
+        <v>4</v>
+      </c>
       <c r="H10" s="46"/>
       <c r="J10" s="25" t="s">
         <v>120</v>
@@ -3251,7 +3253,9 @@
       <c r="F11" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G11" s="27"/>
+      <c r="G11" s="27">
+        <v>5</v>
+      </c>
       <c r="H11" s="46"/>
       <c r="J11" s="28" t="s">
         <v>135</v>
@@ -3318,20 +3322,20 @@
       <c r="A14" s="9">
         <v>5</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="J14" s="61" t="s">
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="J14" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="K14" s="62"/>
-      <c r="L14" s="62"/>
+      <c r="K14" s="63"/>
+      <c r="L14" s="63"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
@@ -3428,14 +3432,14 @@
       <c r="L18" s="25"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="59" t="s">
+      <c r="A19" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
       <c r="G19" s="51"/>
       <c r="H19" s="30"/>
       <c r="J19" s="29" t="s">
@@ -3506,19 +3510,19 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="55">
-        <v>4</v>
-      </c>
-      <c r="D22" s="55">
-        <v>1</v>
-      </c>
-      <c r="E22" s="55"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="55"/>
+      <c r="B22" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="57">
+        <v>4</v>
+      </c>
+      <c r="D22" s="57">
+        <v>1</v>
+      </c>
+      <c r="E22" s="57"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="57"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -3610,7 +3614,7 @@
       <c r="G26" s="27">
         <v>3</v>
       </c>
-      <c r="H26" s="68" t="s">
+      <c r="H26" s="53" t="s">
         <v>139</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Douglas Giordano] - Atualização documento de responsábilidades.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requisitos" sheetId="1" r:id="rId1"/>
@@ -933,10 +933,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -948,7 +945,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1284,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,18 +1302,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="H1" s="55" t="s">
+      <c r="A1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="H1" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="55"/>
+      <c r="I1" s="59"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1443,21 +1443,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="56" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="57">
-        <v>4</v>
-      </c>
-      <c r="D7" s="57">
-        <v>1</v>
-      </c>
-      <c r="E7" s="57"/>
-      <c r="F7" s="58"/>
-      <c r="H7" s="55" t="s">
+      <c r="B7" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="56">
+        <v>4</v>
+      </c>
+      <c r="D7" s="56">
+        <v>1</v>
+      </c>
+      <c r="E7" s="56"/>
+      <c r="F7" s="57"/>
+      <c r="H7" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="55"/>
+      <c r="I7" s="59"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1616,8 +1616,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1665,13 +1665,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="58"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="57"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1816,7 +1816,7 @@
         <v>117</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1883,13 +1883,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="56" t="s">
+      <c r="B27" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="58"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="57"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -1949,13 +1949,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="58"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="57"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2201,13 +2201,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="57"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="57"/>
-      <c r="F47" s="58"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="57"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2325,13 +2325,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="56" t="s">
+      <c r="B55" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="57"/>
-      <c r="D55" s="57"/>
-      <c r="E55" s="57"/>
-      <c r="F55" s="58"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="56"/>
+      <c r="F55" s="57"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2399,16 +2399,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B7:F7"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B55:F55"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2616,17 +2616,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="56" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="57">
-        <v>4</v>
-      </c>
-      <c r="D7" s="57">
-        <v>1</v>
-      </c>
-      <c r="E7" s="57"/>
-      <c r="F7" s="58"/>
+      <c r="B7" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="56">
+        <v>4</v>
+      </c>
+      <c r="D7" s="56">
+        <v>1</v>
+      </c>
+      <c r="E7" s="56"/>
+      <c r="F7" s="57"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -2937,8 +2937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3054,7 +3054,9 @@
       <c r="K4" s="25">
         <v>12</v>
       </c>
-      <c r="L4" s="25"/>
+      <c r="L4" s="25">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
@@ -3220,12 +3222,14 @@
         <v>117</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G10" s="27">
         <v>4</v>
       </c>
-      <c r="H10" s="46"/>
+      <c r="H10" s="46">
+        <v>0.1875</v>
+      </c>
       <c r="J10" s="25" t="s">
         <v>120</v>
       </c>
@@ -3266,7 +3270,7 @@
       </c>
       <c r="L11" s="28">
         <f>SUM(L3:L10)</f>
-        <v>1</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3391,7 +3395,7 @@
         <v>125</v>
       </c>
       <c r="K16" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" s="25"/>
     </row>
@@ -3446,7 +3450,7 @@
         <v>127</v>
       </c>
       <c r="K19" s="25">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L19" s="25"/>
     </row>
@@ -3510,19 +3514,19 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="56" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="57">
-        <v>4</v>
-      </c>
-      <c r="D22" s="57">
-        <v>1</v>
-      </c>
-      <c r="E22" s="57"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="57"/>
+      <c r="B22" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="56">
+        <v>4</v>
+      </c>
+      <c r="D22" s="56">
+        <v>1</v>
+      </c>
+      <c r="E22" s="56"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="56"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">

</xml_diff>

<commit_message>
[Miguel Zinelli] - Atualização da Planilha
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -933,7 +933,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -945,10 +948,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1302,18 +1302,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="H1" s="59" t="s">
+      <c r="A1" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="H1" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="59"/>
+      <c r="I1" s="55"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1443,21 +1443,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="56">
-        <v>4</v>
-      </c>
-      <c r="D7" s="56">
-        <v>1</v>
-      </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="57"/>
-      <c r="H7" s="59" t="s">
+      <c r="B7" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="57">
+        <v>4</v>
+      </c>
+      <c r="D7" s="57">
+        <v>1</v>
+      </c>
+      <c r="E7" s="57"/>
+      <c r="F7" s="58"/>
+      <c r="H7" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="59"/>
+      <c r="I7" s="55"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1616,8 +1616,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1665,13 +1665,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="58"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1883,13 +1883,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="57"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="58"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -1949,13 +1949,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="55" t="s">
+      <c r="B31" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="57"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="58"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2201,13 +2201,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="55" t="s">
+      <c r="B47" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="56"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="57"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="58"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2325,13 +2325,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="55" t="s">
+      <c r="B55" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="56"/>
-      <c r="D55" s="56"/>
-      <c r="E55" s="56"/>
-      <c r="F55" s="57"/>
+      <c r="C55" s="57"/>
+      <c r="D55" s="57"/>
+      <c r="E55" s="57"/>
+      <c r="F55" s="58"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2399,16 +2399,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B55:F55"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B7:F7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B55:F55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2616,17 +2616,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="56">
-        <v>4</v>
-      </c>
-      <c r="D7" s="56">
-        <v>1</v>
-      </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="57"/>
+      <c r="B7" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="57">
+        <v>4</v>
+      </c>
+      <c r="D7" s="57">
+        <v>1</v>
+      </c>
+      <c r="E7" s="57"/>
+      <c r="F7" s="58"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -2937,8 +2937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3106,7 +3106,9 @@
       <c r="F6" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G6" s="27"/>
+      <c r="G6" s="27">
+        <v>4</v>
+      </c>
       <c r="H6" s="47"/>
       <c r="J6" s="25" t="s">
         <v>121</v>
@@ -3135,7 +3137,9 @@
       <c r="F7" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G7" s="27"/>
+      <c r="G7" s="27">
+        <v>4</v>
+      </c>
       <c r="H7" s="47"/>
       <c r="J7" s="25" t="s">
         <v>122</v>
@@ -3514,19 +3518,19 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="56">
-        <v>4</v>
-      </c>
-      <c r="D22" s="56">
-        <v>1</v>
-      </c>
-      <c r="E22" s="56"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="56"/>
+      <c r="B22" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="57">
+        <v>4</v>
+      </c>
+      <c r="D22" s="57">
+        <v>1</v>
+      </c>
+      <c r="E22" s="57"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="57"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -3545,7 +3549,7 @@
         <v>121</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G23" s="27"/>
       <c r="H23" s="35"/>

</xml_diff>

<commit_message>
[Pedro Silva] - Integrando minha parte ao develop.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="140">
   <si>
     <t>ID</t>
   </si>
@@ -431,6 +431,12 @@
   </si>
   <si>
     <t>Casos de Uso Atrasados</t>
+  </si>
+  <si>
+    <t>Horas Disponíveis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 01:00:00</t>
   </si>
 </sst>
 </file>
@@ -770,25 +776,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <left/>
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -913,9 +913,6 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -924,6 +921,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -937,9 +949,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1275,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,18 +1302,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="H1" s="55" t="s">
+      <c r="A1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="H1" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="55"/>
+      <c r="I1" s="59"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1434,21 +1443,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="52">
-        <v>4</v>
-      </c>
-      <c r="D7" s="52">
-        <v>1</v>
-      </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="53"/>
-      <c r="H7" s="55" t="s">
+      <c r="B7" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="56">
+        <v>4</v>
+      </c>
+      <c r="D7" s="56">
+        <v>1</v>
+      </c>
+      <c r="E7" s="56"/>
+      <c r="F7" s="57"/>
+      <c r="H7" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="55"/>
+      <c r="I7" s="59"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1607,8 +1616,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="56"/>
-      <c r="K13" s="56"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1656,13 +1665,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="53"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="57"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1807,7 +1816,7 @@
         <v>117</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1874,13 +1883,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="53"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="57"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -1940,13 +1949,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="51" t="s">
+      <c r="B31" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="53"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="57"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2192,13 +2201,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="51" t="s">
+      <c r="B47" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="52"/>
-      <c r="D47" s="52"/>
-      <c r="E47" s="52"/>
-      <c r="F47" s="53"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="57"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2316,13 +2325,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="51" t="s">
+      <c r="B55" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="52"/>
-      <c r="D55" s="52"/>
-      <c r="E55" s="52"/>
-      <c r="F55" s="53"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="56"/>
+      <c r="F55" s="57"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2390,16 +2399,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B7:F7"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B55:F55"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2410,8 +2419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2428,20 +2437,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
+      <c r="A1" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
       <c r="G1" s="30"/>
-      <c r="I1" s="59" t="s">
+      <c r="I1" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -2607,17 +2616,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="52">
-        <v>4</v>
-      </c>
-      <c r="D7" s="52">
-        <v>1</v>
-      </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="53"/>
+      <c r="B7" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="56">
+        <v>4</v>
+      </c>
+      <c r="D7" s="56">
+        <v>1</v>
+      </c>
+      <c r="E7" s="56"/>
+      <c r="F7" s="57"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -2828,11 +2837,11 @@
       <c r="G14" s="35">
         <v>0</v>
       </c>
-      <c r="I14" s="59" t="s">
+      <c r="I14" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="41" t="s">
@@ -2926,10 +2935,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2938,29 +2947,31 @@
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="30"/>
-      <c r="I1" s="59" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="30"/>
+      <c r="J1" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
@@ -2976,43 +2987,47 @@
       <c r="E2" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="J2" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="J2" s="28" t="s">
-        <v>131</v>
-      </c>
       <c r="K2" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="L2" s="28" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="39">
         <v>4</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="65"/>
-      <c r="I3" s="25" t="s">
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="68"/>
+      <c r="J3" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="J3" s="25">
+      <c r="K3" s="25">
         <v>8</v>
       </c>
-      <c r="K3" s="25"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="25"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>21</v>
       </c>
@@ -3031,16 +3046,19 @@
       <c r="F4" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G4" s="47"/>
-      <c r="I4" s="25" t="s">
+      <c r="G4" s="27"/>
+      <c r="H4" s="46"/>
+      <c r="J4" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="J4" s="25">
+      <c r="K4" s="25">
         <v>12</v>
       </c>
-      <c r="K4" s="25"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="25">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>22</v>
       </c>
@@ -3059,16 +3077,17 @@
       <c r="F5" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G5" s="47"/>
-      <c r="I5" s="25" t="s">
+      <c r="G5" s="27"/>
+      <c r="H5" s="46"/>
+      <c r="J5" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="J5" s="25">
+      <c r="K5" s="25">
         <v>8</v>
       </c>
-      <c r="K5" s="25"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="25"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>25</v>
       </c>
@@ -3087,16 +3106,17 @@
       <c r="F6" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G6" s="48"/>
-      <c r="I6" s="25" t="s">
+      <c r="G6" s="27"/>
+      <c r="H6" s="47"/>
+      <c r="J6" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="J6" s="25">
+      <c r="K6" s="25">
         <v>8</v>
       </c>
-      <c r="K6" s="25"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="25"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>27</v>
       </c>
@@ -3115,16 +3135,17 @@
       <c r="F7" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G7" s="48"/>
-      <c r="I7" s="25" t="s">
+      <c r="G7" s="27"/>
+      <c r="H7" s="47"/>
+      <c r="J7" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="J7" s="25">
+      <c r="K7" s="25">
         <v>8</v>
       </c>
-      <c r="K7" s="25"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="25"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>29</v>
       </c>
@@ -3143,16 +3164,17 @@
       <c r="F8" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G8" s="47"/>
-      <c r="I8" s="25" t="s">
+      <c r="G8" s="27"/>
+      <c r="H8" s="46"/>
+      <c r="J8" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="J8" s="25">
+      <c r="K8" s="25">
         <v>8</v>
       </c>
-      <c r="K8" s="25"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="25"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>31</v>
       </c>
@@ -3166,21 +3188,24 @@
         <v>2</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F9" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G9" s="47"/>
-      <c r="I9" s="25" t="s">
+      <c r="G9" s="27"/>
+      <c r="H9" s="46"/>
+      <c r="J9" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="J9" s="25">
+      <c r="K9" s="25">
         <v>6</v>
       </c>
-      <c r="K9" s="25"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>33</v>
       </c>
@@ -3197,18 +3222,23 @@
         <v>117</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="G10" s="47"/>
-      <c r="I10" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="G10" s="27">
+        <v>4</v>
+      </c>
+      <c r="H10" s="46">
+        <v>0.1875</v>
+      </c>
+      <c r="J10" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="J10" s="25">
+      <c r="K10" s="25">
         <v>10</v>
       </c>
-      <c r="K10" s="25"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="25"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>35</v>
       </c>
@@ -3227,20 +3257,23 @@
       <c r="F11" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G11" s="47"/>
-      <c r="I11" s="28" t="s">
+      <c r="G11" s="27">
+        <v>5</v>
+      </c>
+      <c r="H11" s="46"/>
+      <c r="J11" s="28" t="s">
         <v>135</v>
-      </c>
-      <c r="J11" s="28">
-        <f>SUM(J3:J10)</f>
-        <v>68</v>
       </c>
       <c r="K11" s="28">
         <f>SUM(K3:K10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="L11" s="28">
+        <f>SUM(L3:L10)</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
         <v>37</v>
       </c>
@@ -3259,9 +3292,12 @@
       <c r="F12" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G12" s="47"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G12" s="27">
+        <v>4</v>
+      </c>
+      <c r="H12" s="46"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>130</v>
       </c>
@@ -3275,33 +3311,37 @@
         <v>2</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F13" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G13" s="47"/>
-      <c r="J13" s="25"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G13" s="27">
+        <v>4</v>
+      </c>
+      <c r="H13" s="46"/>
+      <c r="K13" s="25"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>5</v>
       </c>
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="I14" s="59" t="s">
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="J14" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="63"/>
+      <c r="L14" s="63"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
         <v>40</v>
       </c>
@@ -3320,16 +3360,19 @@
       <c r="F15" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G15" s="47"/>
-      <c r="I15" s="25" t="s">
+      <c r="G15" s="27">
+        <v>7</v>
+      </c>
+      <c r="H15" s="46"/>
+      <c r="J15" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="J15" s="25" t="s">
+      <c r="K15" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K15" s="25"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="25"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>42</v>
       </c>
@@ -3346,16 +3389,17 @@
       <c r="F16" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G16" s="49"/>
-      <c r="I16" s="25" t="s">
+      <c r="G16" s="27"/>
+      <c r="H16" s="48"/>
+      <c r="J16" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="J16" s="25">
-        <v>0</v>
-      </c>
-      <c r="K16" s="25"/>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K16" s="25">
+        <v>1</v>
+      </c>
+      <c r="L16" s="25"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="41" t="s">
         <v>44</v>
       </c>
@@ -3369,46 +3413,48 @@
         <v>2</v>
       </c>
       <c r="E17" s="43"/>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="G17" s="50"/>
-      <c r="I17" s="25" t="s">
+      <c r="G17" s="6"/>
+      <c r="H17" s="49"/>
+      <c r="J17" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="J17" s="25">
+      <c r="K17" s="25">
         <v>3</v>
       </c>
-      <c r="K17" s="25"/>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I18" s="25" t="s">
+      <c r="L17" s="25"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="J18" s="25">
+      <c r="K18" s="25">
         <v>3</v>
       </c>
-      <c r="K18" s="25"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="57" t="s">
+      <c r="L18" s="25"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="30"/>
-      <c r="I19" s="29" t="s">
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="30"/>
+      <c r="J19" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="J19" s="25">
-        <v>14</v>
-      </c>
-      <c r="K19" s="25"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="25">
+        <v>13</v>
+      </c>
+      <c r="L19" s="25"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>0</v>
       </c>
@@ -3427,19 +3473,22 @@
       <c r="F20" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="G20" s="32" t="s">
+      <c r="G20" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="H20" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="I20" s="28" t="s">
+      <c r="J20" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="J20" s="28">
-        <f>SUM(J16:J19)</f>
+      <c r="K20" s="28">
+        <f>SUM(K16:K19)</f>
         <v>20</v>
       </c>
-      <c r="K20" s="28"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="28"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="33">
         <v>0</v>
       </c>
@@ -3458,26 +3507,28 @@
       <c r="F21" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G21" s="35"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G21" s="27"/>
+      <c r="H21" s="35"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="52">
-        <v>4</v>
-      </c>
-      <c r="D22" s="52">
-        <v>1</v>
-      </c>
-      <c r="E22" s="52"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="40"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="56">
+        <v>4</v>
+      </c>
+      <c r="D22" s="56">
+        <v>1</v>
+      </c>
+      <c r="E22" s="56"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="56"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
         <v>7</v>
       </c>
@@ -3496,9 +3547,10 @@
       <c r="F23" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G23" s="35"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G23" s="27"/>
+      <c r="H23" s="35"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
         <v>9</v>
       </c>
@@ -3517,9 +3569,12 @@
       <c r="F24" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G24" s="35"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G24" s="27">
+        <v>3</v>
+      </c>
+      <c r="H24" s="35"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
         <v>11</v>
       </c>
@@ -3538,9 +3593,10 @@
       <c r="F25" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="G25" s="35"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G25" s="27"/>
+      <c r="H25" s="35"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
         <v>13</v>
       </c>
@@ -3557,11 +3613,16 @@
         <v>119</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G26" s="35"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="G26" s="27">
+        <v>3</v>
+      </c>
+      <c r="H26" s="53" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
         <v>16</v>
       </c>
@@ -3580,9 +3641,10 @@
       <c r="F27" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="G27" s="35"/>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G27" s="27"/>
+      <c r="H27" s="35"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="41" t="s">
         <v>18</v>
       </c>
@@ -3601,17 +3663,19 @@
       <c r="F28" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="G28" s="45"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I14:K14"/>
+  <mergeCells count="8">
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J14:L14"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="G22:H22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
[Alex Becker] - Atualizado planilhas com as horas trabalhadas.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -933,10 +933,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -948,7 +945,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1302,18 +1302,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="H1" s="55" t="s">
+      <c r="A1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="H1" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="55"/>
+      <c r="I1" s="59"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1443,21 +1443,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="56" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="57">
-        <v>4</v>
-      </c>
-      <c r="D7" s="57">
-        <v>1</v>
-      </c>
-      <c r="E7" s="57"/>
-      <c r="F7" s="58"/>
-      <c r="H7" s="55" t="s">
+      <c r="B7" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="56">
+        <v>4</v>
+      </c>
+      <c r="D7" s="56">
+        <v>1</v>
+      </c>
+      <c r="E7" s="56"/>
+      <c r="F7" s="57"/>
+      <c r="H7" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="55"/>
+      <c r="I7" s="59"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1616,8 +1616,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1665,13 +1665,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="58"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="57"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1883,13 +1883,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="56" t="s">
+      <c r="B27" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="58"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="57"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -1949,13 +1949,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="58"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="57"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2201,13 +2201,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="57"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="57"/>
-      <c r="F47" s="58"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="57"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2325,13 +2325,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="56" t="s">
+      <c r="B55" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="57"/>
-      <c r="D55" s="57"/>
-      <c r="E55" s="57"/>
-      <c r="F55" s="58"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="56"/>
+      <c r="F55" s="57"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2399,16 +2399,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B7:F7"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B55:F55"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2616,17 +2616,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="56" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="57">
-        <v>4</v>
-      </c>
-      <c r="D7" s="57">
-        <v>1</v>
-      </c>
-      <c r="E7" s="57"/>
-      <c r="F7" s="58"/>
+      <c r="B7" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="56">
+        <v>4</v>
+      </c>
+      <c r="D7" s="56">
+        <v>1</v>
+      </c>
+      <c r="E7" s="56"/>
+      <c r="F7" s="57"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -2937,8 +2937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3025,7 +3025,9 @@
       <c r="K3" s="25">
         <v>8</v>
       </c>
-      <c r="L3" s="25"/>
+      <c r="L3" s="25">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -3274,7 +3276,7 @@
       </c>
       <c r="L11" s="28">
         <f>SUM(L3:L10)</f>
-        <v>5.5</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3299,7 +3301,9 @@
       <c r="G12" s="27">
         <v>4</v>
       </c>
-      <c r="H12" s="46"/>
+      <c r="H12" s="46">
+        <v>0.16666666666666666</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
@@ -3323,7 +3327,9 @@
       <c r="G13" s="27">
         <v>4</v>
       </c>
-      <c r="H13" s="46"/>
+      <c r="H13" s="46">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="K13" s="25"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -3518,19 +3524,19 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="56" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="57">
-        <v>4</v>
-      </c>
-      <c r="D22" s="57">
-        <v>1</v>
-      </c>
-      <c r="E22" s="57"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="57"/>
+      <c r="B22" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="56">
+        <v>4</v>
+      </c>
+      <c r="D22" s="56">
+        <v>1</v>
+      </c>
+      <c r="E22" s="56"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="56"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">

</xml_diff>

<commit_message>
[Gean Pereira] - Atualização da gerencia de tempo das atividades listadas nos incrementos do processo de evolução de software
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
@@ -12,7 +12,7 @@
     <sheet name="Incremento 2" sheetId="3" r:id="rId3"/>
     <sheet name="Incremento 3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -933,7 +933,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -945,10 +948,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1038,7 +1038,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1073,7 +1073,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1302,18 +1302,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="H1" s="59" t="s">
+      <c r="A1" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="H1" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="59"/>
+      <c r="I1" s="55"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1443,21 +1443,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="56">
-        <v>4</v>
-      </c>
-      <c r="D7" s="56">
-        <v>1</v>
-      </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="57"/>
-      <c r="H7" s="59" t="s">
+      <c r="B7" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="57">
+        <v>4</v>
+      </c>
+      <c r="D7" s="57">
+        <v>1</v>
+      </c>
+      <c r="E7" s="57"/>
+      <c r="F7" s="58"/>
+      <c r="H7" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="59"/>
+      <c r="I7" s="55"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1616,8 +1616,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1665,13 +1665,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="58"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1883,13 +1883,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="57"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="58"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -1949,13 +1949,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="55" t="s">
+      <c r="B31" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="57"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="58"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2201,13 +2201,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="55" t="s">
+      <c r="B47" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="56"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="57"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="58"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2325,13 +2325,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="55" t="s">
+      <c r="B55" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="56"/>
-      <c r="D55" s="56"/>
-      <c r="E55" s="56"/>
-      <c r="F55" s="57"/>
+      <c r="C55" s="57"/>
+      <c r="D55" s="57"/>
+      <c r="E55" s="57"/>
+      <c r="F55" s="58"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2399,16 +2399,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B55:F55"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B7:F7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B55:F55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2616,17 +2616,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="56">
-        <v>4</v>
-      </c>
-      <c r="D7" s="56">
-        <v>1</v>
-      </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="57"/>
+      <c r="B7" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="57">
+        <v>4</v>
+      </c>
+      <c r="D7" s="57">
+        <v>1</v>
+      </c>
+      <c r="E7" s="57"/>
+      <c r="F7" s="58"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -2937,8 +2937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3170,7 +3170,9 @@
       <c r="F8" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G8" s="27"/>
+      <c r="G8" s="27">
+        <v>2</v>
+      </c>
       <c r="H8" s="46"/>
       <c r="J8" s="25" t="s">
         <v>124</v>
@@ -3515,28 +3517,32 @@
         <v>123</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="G21" s="27"/>
-      <c r="H21" s="35"/>
+        <v>125</v>
+      </c>
+      <c r="G21" s="27">
+        <v>4</v>
+      </c>
+      <c r="H21" s="46">
+        <v>0.20833333333333334</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="56">
-        <v>4</v>
-      </c>
-      <c r="D22" s="56">
-        <v>1</v>
-      </c>
-      <c r="E22" s="56"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="56"/>
+      <c r="B22" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="57">
+        <v>4</v>
+      </c>
+      <c r="D22" s="57">
+        <v>1</v>
+      </c>
+      <c r="E22" s="57"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="57"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -3649,9 +3655,11 @@
         <v>123</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="G27" s="27"/>
+        <v>128</v>
+      </c>
+      <c r="G27" s="27">
+        <v>2</v>
+      </c>
       <c r="H27" s="35"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[Pedro Silva] - Colocando as horas trabalhadas.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
@@ -12,7 +12,7 @@
     <sheet name="Incremento 2" sheetId="3" r:id="rId3"/>
     <sheet name="Incremento 3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -788,7 +788,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -933,10 +933,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -948,7 +945,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -976,6 +976,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1038,7 +1041,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1073,7 +1076,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1302,18 +1305,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="H1" s="55" t="s">
+      <c r="A1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="H1" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="55"/>
+      <c r="I1" s="59"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1443,21 +1446,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="56" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="57">
-        <v>4</v>
-      </c>
-      <c r="D7" s="57">
-        <v>1</v>
-      </c>
-      <c r="E7" s="57"/>
-      <c r="F7" s="58"/>
-      <c r="H7" s="55" t="s">
+      <c r="B7" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="56">
+        <v>4</v>
+      </c>
+      <c r="D7" s="56">
+        <v>1</v>
+      </c>
+      <c r="E7" s="56"/>
+      <c r="F7" s="57"/>
+      <c r="H7" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="55"/>
+      <c r="I7" s="59"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1616,8 +1619,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1665,13 +1668,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="58"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="57"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1883,13 +1886,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="56" t="s">
+      <c r="B27" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="58"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="57"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -1949,13 +1952,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="58"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="57"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2201,13 +2204,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="57"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="57"/>
-      <c r="F47" s="58"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="57"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2325,13 +2328,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="56" t="s">
+      <c r="B55" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="57"/>
-      <c r="D55" s="57"/>
-      <c r="E55" s="57"/>
-      <c r="F55" s="58"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="56"/>
+      <c r="F55" s="57"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2399,16 +2402,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B7:F7"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B55:F55"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2616,17 +2619,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="56" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="57">
-        <v>4</v>
-      </c>
-      <c r="D7" s="57">
-        <v>1</v>
-      </c>
-      <c r="E7" s="57"/>
-      <c r="F7" s="58"/>
+      <c r="B7" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="56">
+        <v>4</v>
+      </c>
+      <c r="D7" s="56">
+        <v>1</v>
+      </c>
+      <c r="E7" s="56"/>
+      <c r="F7" s="57"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -2937,8 +2940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3244,7 +3247,9 @@
       <c r="K10" s="25">
         <v>10</v>
       </c>
-      <c r="L10" s="25"/>
+      <c r="L10" s="69">
+        <v>10.5</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
@@ -3278,7 +3283,7 @@
       </c>
       <c r="L11" s="28">
         <f>SUM(L3:L10)</f>
-        <v>14.5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3370,12 +3375,14 @@
         <v>120</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G15" s="27">
         <v>7</v>
       </c>
-      <c r="H15" s="46"/>
+      <c r="H15" s="46">
+        <v>0.25</v>
+      </c>
       <c r="J15" s="25" t="s">
         <v>103</v>
       </c>
@@ -3530,19 +3537,19 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="56" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="57">
-        <v>4</v>
-      </c>
-      <c r="D22" s="57">
-        <v>1</v>
-      </c>
-      <c r="E22" s="57"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="57"/>
+      <c r="B22" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="56">
+        <v>4</v>
+      </c>
+      <c r="D22" s="56">
+        <v>1</v>
+      </c>
+      <c r="E22" s="56"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="56"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -3583,12 +3590,14 @@
         <v>120</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G24" s="27">
         <v>3</v>
       </c>
-      <c r="H24" s="35"/>
+      <c r="H24" s="35">
+        <v>0.1875</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">

</xml_diff>

<commit_message>
[Edison Moura] Atualizando planilha de atividades e horas trabalhadas na semana.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Incremento 2" sheetId="3" r:id="rId3"/>
     <sheet name="Incremento 3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -436,7 +436,7 @@
     <t>Horas Disponíveis</t>
   </si>
   <si>
-    <t xml:space="preserve"> 01:00:00</t>
+    <t xml:space="preserve"> 02:30:00</t>
   </si>
 </sst>
 </file>
@@ -933,7 +933,13 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -945,10 +951,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -976,9 +979,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1305,18 +1305,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="H1" s="59" t="s">
+      <c r="A1" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="H1" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="59"/>
+      <c r="I1" s="56"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1446,21 +1446,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="56">
-        <v>4</v>
-      </c>
-      <c r="D7" s="56">
-        <v>1</v>
-      </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="57"/>
-      <c r="H7" s="59" t="s">
+      <c r="B7" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="58">
+        <v>4</v>
+      </c>
+      <c r="D7" s="58">
+        <v>1</v>
+      </c>
+      <c r="E7" s="58"/>
+      <c r="F7" s="59"/>
+      <c r="H7" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="59"/>
+      <c r="I7" s="56"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1619,8 +1619,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="60"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1668,13 +1668,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="57"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="59"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1886,13 +1886,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="57"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="59"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -1952,13 +1952,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="55" t="s">
+      <c r="B31" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="57"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="59"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2204,13 +2204,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="55" t="s">
+      <c r="B47" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="56"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="57"/>
+      <c r="C47" s="58"/>
+      <c r="D47" s="58"/>
+      <c r="E47" s="58"/>
+      <c r="F47" s="59"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2328,13 +2328,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="55" t="s">
+      <c r="B55" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="56"/>
-      <c r="D55" s="56"/>
-      <c r="E55" s="56"/>
-      <c r="F55" s="57"/>
+      <c r="C55" s="58"/>
+      <c r="D55" s="58"/>
+      <c r="E55" s="58"/>
+      <c r="F55" s="59"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2402,16 +2402,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B55:F55"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B7:F7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B55:F55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2422,7 +2422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -2440,20 +2440,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
+      <c r="A1" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
       <c r="G1" s="30"/>
-      <c r="I1" s="62" t="s">
+      <c r="I1" s="63" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -2619,17 +2619,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="56">
-        <v>4</v>
-      </c>
-      <c r="D7" s="56">
-        <v>1</v>
-      </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="57"/>
+      <c r="B7" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="58">
+        <v>4</v>
+      </c>
+      <c r="D7" s="58">
+        <v>1</v>
+      </c>
+      <c r="E7" s="58"/>
+      <c r="F7" s="59"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -2840,11 +2840,11 @@
       <c r="G14" s="35">
         <v>0</v>
       </c>
-      <c r="I14" s="62" t="s">
+      <c r="I14" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="63"/>
-      <c r="K14" s="63"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="64"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="41" t="s">
@@ -2941,7 +2941,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2958,21 +2958,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="64"/>
+      <c r="A1" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="65"/>
       <c r="G1" s="50"/>
       <c r="H1" s="30"/>
-      <c r="J1" s="62" t="s">
+      <c r="J1" s="63" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -3013,15 +3013,15 @@
       <c r="A3" s="39">
         <v>4</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="69"/>
       <c r="J3" s="25" t="s">
         <v>118</v>
       </c>
@@ -3049,10 +3049,14 @@
         <v>119</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="46"/>
+        <v>128</v>
+      </c>
+      <c r="G4" s="27">
+        <v>2</v>
+      </c>
+      <c r="H4" s="46">
+        <v>3.125E-2</v>
+      </c>
       <c r="J4" s="25" t="s">
         <v>117</v>
       </c>
@@ -3247,7 +3251,7 @@
       <c r="K10" s="25">
         <v>10</v>
       </c>
-      <c r="L10" s="69">
+      <c r="L10" s="54">
         <v>10.5</v>
       </c>
     </row>
@@ -3343,20 +3347,20 @@
       <c r="A14" s="9">
         <v>5</v>
       </c>
-      <c r="B14" s="65" t="s">
+      <c r="B14" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="J14" s="62" t="s">
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="66"/>
+      <c r="J14" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="K14" s="63"/>
-      <c r="L14" s="63"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="64"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
@@ -3455,14 +3459,14 @@
       <c r="L18" s="25"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="61"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
       <c r="G19" s="51"/>
       <c r="H19" s="30"/>
       <c r="J19" s="29" t="s">
@@ -3537,19 +3541,19 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="56">
-        <v>4</v>
-      </c>
-      <c r="D22" s="56">
-        <v>1</v>
-      </c>
-      <c r="E22" s="56"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="56"/>
+      <c r="B22" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="58">
+        <v>4</v>
+      </c>
+      <c r="D22" s="58">
+        <v>1</v>
+      </c>
+      <c r="E22" s="58"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="58"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -3638,7 +3642,7 @@
         <v>119</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G26" s="27">
         <v>3</v>

</xml_diff>

<commit_message>
[Alex Becker] - Encerramento da planilha no ciclo 2.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="143">
   <si>
     <t>ID</t>
   </si>
@@ -437,13 +437,22 @@
   </si>
   <si>
     <t xml:space="preserve"> 02:30:00</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>Status Interface</t>
+  </si>
+  <si>
+    <t>Status Validação</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,6 +497,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -515,7 +531,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -784,11 +800,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -930,16 +959,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -951,7 +974,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -979,6 +1005,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1305,18 +1350,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="H1" s="56" t="s">
+      <c r="A1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="H1" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="56"/>
+      <c r="I1" s="59"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1446,21 +1491,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="57" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="58">
-        <v>4</v>
-      </c>
-      <c r="D7" s="58">
-        <v>1</v>
-      </c>
-      <c r="E7" s="58"/>
-      <c r="F7" s="59"/>
-      <c r="H7" s="56" t="s">
+      <c r="B7" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="56">
+        <v>4</v>
+      </c>
+      <c r="D7" s="56">
+        <v>1</v>
+      </c>
+      <c r="E7" s="56"/>
+      <c r="F7" s="57"/>
+      <c r="H7" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="56"/>
+      <c r="I7" s="59"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1619,8 +1664,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1668,13 +1713,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="59"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="57"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1886,13 +1931,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="57" t="s">
+      <c r="B27" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="59"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="57"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -1952,13 +1997,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="57" t="s">
+      <c r="B31" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="58"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="59"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="57"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2204,13 +2249,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="57" t="s">
+      <c r="B47" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="58"/>
-      <c r="D47" s="58"/>
-      <c r="E47" s="58"/>
-      <c r="F47" s="59"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="57"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2328,13 +2373,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="57" t="s">
+      <c r="B55" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="58"/>
-      <c r="D55" s="58"/>
-      <c r="E55" s="58"/>
-      <c r="F55" s="59"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="56"/>
+      <c r="F55" s="57"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2402,16 +2447,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B7:F7"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B55:F55"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2423,7 +2468,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2440,20 +2485,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
+      <c r="A1" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
       <c r="G1" s="30"/>
-      <c r="I1" s="63" t="s">
+      <c r="I1" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -2619,17 +2664,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="57" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="58">
-        <v>4</v>
-      </c>
-      <c r="D7" s="58">
-        <v>1</v>
-      </c>
-      <c r="E7" s="58"/>
-      <c r="F7" s="59"/>
+      <c r="B7" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="56">
+        <v>4</v>
+      </c>
+      <c r="D7" s="56">
+        <v>1</v>
+      </c>
+      <c r="E7" s="56"/>
+      <c r="F7" s="57"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -2840,11 +2885,11 @@
       <c r="G14" s="35">
         <v>0</v>
       </c>
-      <c r="I14" s="63" t="s">
+      <c r="I14" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="64"/>
-      <c r="K14" s="64"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="41" t="s">
@@ -2938,10 +2983,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2949,32 +2994,36 @@
     <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="30"/>
-      <c r="J1" s="63" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="30"/>
+      <c r="L1" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
@@ -2991,83 +3040,93 @@
         <v>114</v>
       </c>
       <c r="F2" s="52" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="I2" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="J2" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="L2" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="M2" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="N2" s="28" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="39">
         <v>4</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="69"/>
-      <c r="J3" s="25" t="s">
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="68"/>
+      <c r="L3" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="K3" s="25">
+      <c r="M3" s="25">
         <v>8</v>
       </c>
-      <c r="L3" s="25">
+      <c r="N3" s="25">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="27">
-        <v>4</v>
-      </c>
-      <c r="D4" s="27">
+      <c r="C4" s="72">
+        <v>4</v>
+      </c>
+      <c r="D4" s="72">
         <v>2</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="72" t="s">
         <v>119</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="G4" s="27">
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" s="72">
         <v>2</v>
       </c>
-      <c r="H4" s="46">
+      <c r="J4" s="74">
         <v>3.125E-2</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="L4" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="K4" s="25">
+      <c r="M4" s="25">
         <v>12</v>
       </c>
-      <c r="L4" s="25">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>22</v>
       </c>
@@ -3083,20 +3142,26 @@
       <c r="E5" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="46"/>
-      <c r="J5" s="25" t="s">
+      <c r="I5" s="27">
+        <v>6</v>
+      </c>
+      <c r="J5" s="46"/>
+      <c r="L5" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="K5" s="25">
+      <c r="M5" s="25">
         <v>8</v>
       </c>
-      <c r="L5" s="25"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N5" s="25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>25</v>
       </c>
@@ -3112,22 +3177,28 @@
       <c r="E6" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="F6" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="G6" s="27">
-        <v>4</v>
-      </c>
-      <c r="H6" s="47"/>
-      <c r="J6" s="25" t="s">
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="I6" s="27">
+        <v>4</v>
+      </c>
+      <c r="J6" s="47">
+        <v>0.125</v>
+      </c>
+      <c r="L6" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="K6" s="25">
+      <c r="M6" s="25">
         <v>8</v>
       </c>
-      <c r="L6" s="25"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N6" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>27</v>
       </c>
@@ -3141,24 +3212,24 @@
         <v>2</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="G7" s="27">
-        <v>4</v>
-      </c>
-      <c r="H7" s="47"/>
-      <c r="J7" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="47"/>
+      <c r="L7" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="K7" s="25">
+      <c r="M7" s="25">
         <v>8</v>
       </c>
-      <c r="L7" s="25"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N7" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>29</v>
       </c>
@@ -3174,22 +3245,28 @@
       <c r="E8" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="F8" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="G8" s="27">
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" s="27">
         <v>2</v>
       </c>
-      <c r="H8" s="46"/>
-      <c r="J8" s="25" t="s">
+      <c r="J8" s="46">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="L8" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="K8" s="25">
+      <c r="M8" s="25">
         <v>8</v>
       </c>
-      <c r="L8" s="25"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N8" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>31</v>
       </c>
@@ -3203,24 +3280,24 @@
         <v>2</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>127</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="F9" s="27"/>
       <c r="G9" s="27"/>
-      <c r="H9" s="46"/>
-      <c r="J9" s="25" t="s">
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="46"/>
+      <c r="L9" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="K9" s="25">
+      <c r="M9" s="25">
         <v>6</v>
       </c>
-      <c r="L9" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N9" s="25">
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>33</v>
       </c>
@@ -3236,26 +3313,28 @@
       <c r="E10" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="G10" s="27">
-        <v>4</v>
-      </c>
-      <c r="H10" s="46">
+      <c r="I10" s="27">
+        <v>4</v>
+      </c>
+      <c r="J10" s="46">
         <v>0.1875</v>
       </c>
-      <c r="J10" s="25" t="s">
+      <c r="L10" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="K10" s="25">
+      <c r="M10" s="25">
         <v>10</v>
       </c>
-      <c r="L10" s="54">
+      <c r="N10" s="53">
         <v>10.5</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>35</v>
       </c>
@@ -3271,26 +3350,30 @@
       <c r="E11" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="F11" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="G11" s="27">
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="I11" s="27">
         <v>5</v>
       </c>
-      <c r="H11" s="46"/>
-      <c r="J11" s="28" t="s">
+      <c r="J11" s="46">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="L11" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="K11" s="28">
-        <f>SUM(K3:K10)</f>
+      <c r="M11" s="28">
+        <f>SUM(M3:M10)</f>
         <v>68</v>
       </c>
-      <c r="L11" s="28">
-        <f>SUM(L3:L10)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N11" s="28">
+        <f>SUM(N3:N10)</f>
+        <v>50.65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
         <v>37</v>
       </c>
@@ -3306,17 +3389,19 @@
       <c r="E12" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="F12" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="G12" s="27">
-        <v>4</v>
-      </c>
-      <c r="H12" s="46">
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="I12" s="27">
+        <v>4</v>
+      </c>
+      <c r="J12" s="46">
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>130</v>
       </c>
@@ -3332,37 +3417,41 @@
       <c r="E13" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="F13" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="G13" s="27">
-        <v>4</v>
-      </c>
-      <c r="H13" s="46">
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="I13" s="27">
+        <v>4</v>
+      </c>
+      <c r="J13" s="46">
         <v>0.20833333333333334</v>
       </c>
-      <c r="K13" s="25"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="25"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>5</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="66"/>
-      <c r="J14" s="63" t="s">
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="L14" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="K14" s="64"/>
-      <c r="L14" s="64"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="63"/>
+      <c r="N14" s="63"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
         <v>40</v>
       </c>
@@ -3378,106 +3467,98 @@
       <c r="E15" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="G15" s="27">
+      <c r="I15" s="27">
         <v>7</v>
       </c>
-      <c r="H15" s="46">
+      <c r="J15" s="46">
         <v>0.25</v>
       </c>
-      <c r="J15" s="25" t="s">
+      <c r="L15" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="K15" s="25" t="s">
+      <c r="M15" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="L15" s="25"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="27">
-        <v>4</v>
-      </c>
-      <c r="D16" s="27">
-        <v>2</v>
-      </c>
+      <c r="N15" s="25"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="33"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
       <c r="E16" s="27"/>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="48"/>
+      <c r="L16" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="M16" s="25">
+        <v>1</v>
+      </c>
+      <c r="N16" s="25"/>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="41"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="49"/>
+      <c r="L17" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="M17" s="25">
+        <v>3</v>
+      </c>
+      <c r="N17" s="25"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I18">
+        <f>SUM(I4:I13)+SUM(I15:I17)+SUM(I21)+SUM(I23:I28)</f>
+        <v>55</v>
+      </c>
+      <c r="L18" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="M18" s="25">
+        <v>3</v>
+      </c>
+      <c r="N18" s="25"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="30"/>
+      <c r="L19" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="G16" s="27"/>
-      <c r="H16" s="48"/>
-      <c r="J16" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="K16" s="25">
-        <v>1</v>
-      </c>
-      <c r="L16" s="25"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="43">
-        <v>4</v>
-      </c>
-      <c r="D17" s="43">
-        <v>2</v>
-      </c>
-      <c r="E17" s="43"/>
-      <c r="F17" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="49"/>
-      <c r="J17" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="K17" s="25">
-        <v>3</v>
-      </c>
-      <c r="L17" s="25"/>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J18" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="K18" s="25">
-        <v>3</v>
-      </c>
-      <c r="L18" s="25"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="61" t="s">
-        <v>137</v>
-      </c>
-      <c r="B19" s="62"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="30"/>
-      <c r="J19" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="K19" s="25">
+      <c r="M19" s="25">
         <v>13</v>
       </c>
-      <c r="L19" s="25"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N19" s="25"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>0</v>
       </c>
@@ -3493,25 +3574,27 @@
       <c r="E20" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="I20" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="H20" s="19" t="s">
+      <c r="J20" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="J20" s="28" t="s">
+      <c r="L20" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="K20" s="28">
-        <f>SUM(K16:K19)</f>
+      <c r="M20" s="28">
+        <f>SUM(M16:M19)</f>
         <v>20</v>
       </c>
-      <c r="L20" s="28"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N20" s="28"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="33">
         <v>0</v>
       </c>
@@ -3527,35 +3610,39 @@
       <c r="E21" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="G21" s="27">
-        <v>4</v>
-      </c>
-      <c r="H21" s="46">
+      <c r="I21" s="27">
+        <v>4</v>
+      </c>
+      <c r="J21" s="46">
         <v>0.20833333333333334</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="57" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="58">
-        <v>4</v>
-      </c>
-      <c r="D22" s="58">
-        <v>1</v>
-      </c>
-      <c r="E22" s="58"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="57"/>
-      <c r="H22" s="58"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="56">
+        <v>4</v>
+      </c>
+      <c r="D22" s="56">
+        <v>1</v>
+      </c>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="55"/>
+      <c r="J22" s="56"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
         <v>7</v>
       </c>
@@ -3571,13 +3658,19 @@
       <c r="E23" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="G23" s="27"/>
-      <c r="H23" s="35"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I23" s="27">
+        <v>1</v>
+      </c>
+      <c r="J23" s="35">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
         <v>9</v>
       </c>
@@ -3593,17 +3686,19 @@
       <c r="E24" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="G24" s="27">
+      <c r="I24" s="27">
         <v>3</v>
       </c>
-      <c r="H24" s="35">
+      <c r="J24" s="35">
         <v>0.1875</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
         <v>11</v>
       </c>
@@ -3617,41 +3712,45 @@
         <v>1</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>128</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="F25" s="27"/>
       <c r="G25" s="27"/>
-      <c r="H25" s="35"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="33" t="s">
+      <c r="H25" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="I25" s="27"/>
+      <c r="J25" s="35"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="27">
-        <v>4</v>
-      </c>
-      <c r="D26" s="27">
-        <v>1</v>
-      </c>
-      <c r="E26" s="27" t="s">
+      <c r="C26" s="72">
+        <v>4</v>
+      </c>
+      <c r="D26" s="72">
+        <v>1</v>
+      </c>
+      <c r="E26" s="72" t="s">
         <v>119</v>
       </c>
-      <c r="F26" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="G26" s="27">
+      <c r="F26" s="72"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="69" t="s">
+        <v>127</v>
+      </c>
+      <c r="I26" s="72">
         <v>3</v>
       </c>
-      <c r="H26" s="53" t="s">
+      <c r="J26" s="73" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
         <v>16</v>
       </c>
@@ -3667,15 +3766,19 @@
       <c r="E27" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="F27" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G27" s="27">
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="I27" s="27">
         <v>2</v>
       </c>
-      <c r="H27" s="35"/>
-    </row>
-    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J27" s="35">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="41" t="s">
         <v>18</v>
       </c>
@@ -3691,24 +3794,31 @@
       <c r="E28" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="F28" s="44" t="s">
-        <v>128</v>
-      </c>
+      <c r="F28" s="43"/>
       <c r="G28" s="43"/>
-      <c r="H28" s="45"/>
+      <c r="H28" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="I28" s="43">
+        <v>4</v>
+      </c>
+      <c r="J28" s="45">
+        <v>0.125</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B14:J14"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="I22:J22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
[Alex Becker] - Definido minhas funcionalidades a serem feitas no ciclo 3.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Requisitos" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="147">
   <si>
     <t>ID</t>
   </si>
@@ -446,13 +446,25 @@
   </si>
   <si>
     <t>Status Validação</t>
+  </si>
+  <si>
+    <t>Total Planejadas</t>
+  </si>
+  <si>
+    <t>Criar ata da sessão de realização da prova didática</t>
+  </si>
+  <si>
+    <t>Criar ata da sessão de divulgação do resultado da prova didática</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -500,6 +512,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -817,7 +837,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -965,6 +985,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -992,6 +1040,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1005,25 +1056,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1350,18 +1382,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="H1" s="59" t="s">
+      <c r="A1" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="H1" s="69" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="59"/>
+      <c r="I1" s="69"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1491,21 +1523,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="56">
-        <v>4</v>
-      </c>
-      <c r="D7" s="56">
-        <v>1</v>
-      </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="57"/>
-      <c r="H7" s="59" t="s">
+      <c r="B7" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="66">
+        <v>4</v>
+      </c>
+      <c r="D7" s="66">
+        <v>1</v>
+      </c>
+      <c r="E7" s="66"/>
+      <c r="F7" s="67"/>
+      <c r="H7" s="69" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="59"/>
+      <c r="I7" s="69"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1664,8 +1696,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="64"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1713,13 +1745,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="57"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="67"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1931,13 +1963,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="57"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="67"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -1997,13 +2029,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="55" t="s">
+      <c r="B31" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="57"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="67"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2249,13 +2281,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="55" t="s">
+      <c r="B47" s="65" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="56"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="57"/>
+      <c r="C47" s="66"/>
+      <c r="D47" s="66"/>
+      <c r="E47" s="66"/>
+      <c r="F47" s="67"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2373,13 +2405,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="55" t="s">
+      <c r="B55" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="56"/>
-      <c r="D55" s="56"/>
-      <c r="E55" s="56"/>
-      <c r="F55" s="57"/>
+      <c r="C55" s="66"/>
+      <c r="D55" s="66"/>
+      <c r="E55" s="66"/>
+      <c r="F55" s="67"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2485,20 +2517,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
+      <c r="A1" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
       <c r="G1" s="30"/>
-      <c r="I1" s="62" t="s">
+      <c r="I1" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -2664,17 +2696,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="56">
-        <v>4</v>
-      </c>
-      <c r="D7" s="56">
-        <v>1</v>
-      </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="57"/>
+      <c r="B7" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="66">
+        <v>4</v>
+      </c>
+      <c r="D7" s="66">
+        <v>1</v>
+      </c>
+      <c r="E7" s="66"/>
+      <c r="F7" s="67"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -2885,11 +2917,11 @@
       <c r="G14" s="35">
         <v>0</v>
       </c>
-      <c r="I14" s="62" t="s">
+      <c r="I14" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="63"/>
-      <c r="K14" s="63"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="73"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="41" t="s">
@@ -2985,8 +3017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3005,23 +3037,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="64"/>
+      <c r="A1" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="75"/>
       <c r="I1" s="50"/>
       <c r="J1" s="30"/>
-      <c r="L1" s="62" t="s">
+      <c r="L1" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -3068,17 +3100,17 @@
       <c r="A3" s="39">
         <v>4</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="68"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="79"/>
       <c r="L3" s="25" t="s">
         <v>118</v>
       </c>
@@ -3090,30 +3122,30 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="72">
-        <v>4</v>
-      </c>
-      <c r="D4" s="72">
+      <c r="C4" s="59">
+        <v>4</v>
+      </c>
+      <c r="D4" s="59">
         <v>2</v>
       </c>
-      <c r="E4" s="72" t="s">
+      <c r="E4" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72" t="s">
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59" t="s">
         <v>127</v>
       </c>
-      <c r="I4" s="72">
+      <c r="I4" s="59">
         <v>2</v>
       </c>
-      <c r="J4" s="74">
+      <c r="J4" s="61">
         <v>3.125E-2</v>
       </c>
       <c r="L4" s="25" t="s">
@@ -3434,22 +3466,22 @@
       <c r="A14" s="9">
         <v>5</v>
       </c>
-      <c r="B14" s="65" t="s">
+      <c r="B14" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="L14" s="62" t="s">
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="76"/>
+      <c r="J14" s="76"/>
+      <c r="L14" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="M14" s="63"/>
-      <c r="N14" s="63"/>
+      <c r="M14" s="73"/>
+      <c r="N14" s="73"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
@@ -3538,16 +3570,16 @@
       <c r="N18" s="25"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="70" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="61"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
       <c r="I19" s="51"/>
       <c r="J19" s="30"/>
       <c r="L19" s="29" t="s">
@@ -3626,21 +3658,21 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="56">
-        <v>4</v>
-      </c>
-      <c r="D22" s="56">
-        <v>1</v>
-      </c>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="55"/>
-      <c r="J22" s="56"/>
+      <c r="B22" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="66">
+        <v>4</v>
+      </c>
+      <c r="D22" s="66">
+        <v>1</v>
+      </c>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="66"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -3723,30 +3755,30 @@
       <c r="J25" s="35"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="70" t="s">
+      <c r="A26" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="71" t="s">
+      <c r="B26" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="72">
-        <v>4</v>
-      </c>
-      <c r="D26" s="72">
-        <v>1</v>
-      </c>
-      <c r="E26" s="72" t="s">
+      <c r="C26" s="59">
+        <v>4</v>
+      </c>
+      <c r="D26" s="59">
+        <v>1</v>
+      </c>
+      <c r="E26" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="69" t="s">
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="I26" s="72">
+      <c r="I26" s="59">
         <v>3</v>
       </c>
-      <c r="J26" s="73" t="s">
+      <c r="J26" s="60" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3824,12 +3856,525 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="30"/>
+      <c r="L1" s="72" t="s">
+        <v>133</v>
+      </c>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="52" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="M2" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="55">
+        <v>6</v>
+      </c>
+      <c r="B3" s="76" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="L3" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="M3" s="54">
+        <v>6</v>
+      </c>
+      <c r="N3" s="54"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="54">
+        <v>4</v>
+      </c>
+      <c r="D4" s="54">
+        <v>3</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="54" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" s="54" t="s">
+        <v>127</v>
+      </c>
+      <c r="H4" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="I4" s="54">
+        <v>3</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="L4" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="27">
+        <v>4</v>
+      </c>
+      <c r="D5" s="27">
+        <v>3</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" s="54" t="s">
+        <v>127</v>
+      </c>
+      <c r="G5" s="54" t="s">
+        <v>127</v>
+      </c>
+      <c r="H5" s="62" t="s">
+        <v>146</v>
+      </c>
+      <c r="I5" s="27">
+        <v>3</v>
+      </c>
+      <c r="J5" s="47"/>
+      <c r="L5" s="54" t="s">
+        <v>123</v>
+      </c>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L6" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="47"/>
+      <c r="L7" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="33"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="46"/>
+      <c r="L8" s="54" t="s">
+        <v>124</v>
+      </c>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="46"/>
+      <c r="L9" s="54" t="s">
+        <v>119</v>
+      </c>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="33"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="46"/>
+      <c r="L10" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="M10" s="54"/>
+      <c r="N10" s="53"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="33"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="46"/>
+      <c r="L11" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="M11" s="28">
+        <f>SUM(M3:M10)</f>
+        <v>6</v>
+      </c>
+      <c r="N11" s="28">
+        <f>SUM(N3:N10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="33"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="46"/>
+      <c r="L12" s="63" t="s">
+        <v>143</v>
+      </c>
+      <c r="M12" s="63">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="46"/>
+      <c r="M13" s="54"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L14" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="M14" s="73"/>
+      <c r="N14" s="73"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="33"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="46"/>
+      <c r="L15" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="M15" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="N15" s="54"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="33"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="48"/>
+      <c r="L16" s="54" t="s">
+        <v>125</v>
+      </c>
+      <c r="M16" s="54"/>
+      <c r="N16" s="54"/>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="41"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="49"/>
+      <c r="L17" s="54" t="s">
+        <v>126</v>
+      </c>
+      <c r="M17" s="54"/>
+      <c r="N17" s="54"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L18" s="54" t="s">
+        <v>128</v>
+      </c>
+      <c r="M18" s="54"/>
+      <c r="N18" s="54"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="70" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" s="71"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="30"/>
+      <c r="L19" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="M19" s="54"/>
+      <c r="N19" s="54"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="J20" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="L20" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="M20" s="28">
+        <f>SUM(M16:M19)</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="28"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="33"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="46"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="33"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="35"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="33"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="35"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="33"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="35"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="57"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="60"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="33"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="35"/>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="41"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="45"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="A19:H19"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Douglas Giordano] - Atualização responsabilidade incremento 3
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="147">
   <si>
     <t>ID</t>
   </si>
@@ -837,7 +837,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1013,6 +1013,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1022,10 +1028,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1364,8 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1382,18 +1385,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="H1" s="69" t="s">
+      <c r="A1" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="H1" s="66" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="69"/>
+      <c r="I1" s="66"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1523,21 +1526,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="65" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="66">
-        <v>4</v>
-      </c>
-      <c r="D7" s="66">
-        <v>1</v>
-      </c>
-      <c r="E7" s="66"/>
-      <c r="F7" s="67"/>
-      <c r="H7" s="69" t="s">
+      <c r="B7" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="68">
+        <v>4</v>
+      </c>
+      <c r="D7" s="68">
+        <v>1</v>
+      </c>
+      <c r="E7" s="68"/>
+      <c r="F7" s="69"/>
+      <c r="H7" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="69"/>
+      <c r="I7" s="66"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1696,8 +1699,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="64"/>
-      <c r="K13" s="64"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="70"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1745,13 +1748,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="65" t="s">
+      <c r="B16" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="67"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="69"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1916,7 +1919,7 @@
         <v>117</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1963,13 +1966,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="65" t="s">
+      <c r="B27" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="66"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="67"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="69"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -2000,9 +2003,11 @@
         <v>4</v>
       </c>
       <c r="D29" s="4">
-        <v>2</v>
-      </c>
-      <c r="E29" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="F29" s="7" t="s">
         <v>127</v>
       </c>
@@ -2018,9 +2023,11 @@
         <v>4</v>
       </c>
       <c r="D30" s="4">
-        <v>2</v>
-      </c>
-      <c r="E30" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="F30" s="7" t="s">
         <v>127</v>
       </c>
@@ -2029,13 +2036,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="65" t="s">
+      <c r="B31" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="66"/>
-      <c r="D31" s="66"/>
-      <c r="E31" s="66"/>
-      <c r="F31" s="67"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="68"/>
+      <c r="F31" s="69"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2281,13 +2288,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="65" t="s">
+      <c r="B47" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="66"/>
-      <c r="D47" s="66"/>
-      <c r="E47" s="66"/>
-      <c r="F47" s="67"/>
+      <c r="C47" s="68"/>
+      <c r="D47" s="68"/>
+      <c r="E47" s="68"/>
+      <c r="F47" s="69"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2405,13 +2412,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="65" t="s">
+      <c r="B55" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="66"/>
-      <c r="D55" s="66"/>
-      <c r="E55" s="66"/>
-      <c r="F55" s="67"/>
+      <c r="C55" s="68"/>
+      <c r="D55" s="68"/>
+      <c r="E55" s="68"/>
+      <c r="F55" s="69"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2479,16 +2486,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B55:F55"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B7:F7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B55:F55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2517,20 +2524,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
+      <c r="A1" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
       <c r="G1" s="30"/>
-      <c r="I1" s="72" t="s">
+      <c r="I1" s="73" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -2696,17 +2703,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="65" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="66">
-        <v>4</v>
-      </c>
-      <c r="D7" s="66">
-        <v>1</v>
-      </c>
-      <c r="E7" s="66"/>
-      <c r="F7" s="67"/>
+      <c r="B7" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="68">
+        <v>4</v>
+      </c>
+      <c r="D7" s="68">
+        <v>1</v>
+      </c>
+      <c r="E7" s="68"/>
+      <c r="F7" s="69"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -2917,11 +2924,11 @@
       <c r="G14" s="35">
         <v>0</v>
       </c>
-      <c r="I14" s="72" t="s">
+      <c r="I14" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="73"/>
-      <c r="K14" s="73"/>
+      <c r="J14" s="74"/>
+      <c r="K14" s="74"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="41" t="s">
@@ -3017,8 +3024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3037,23 +3044,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="75"/>
+      <c r="A1" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="76"/>
       <c r="I1" s="50"/>
       <c r="J1" s="30"/>
-      <c r="L1" s="72" t="s">
+      <c r="L1" s="73" t="s">
         <v>133</v>
       </c>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -3100,17 +3107,17 @@
       <c r="A3" s="39">
         <v>4</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="80"/>
       <c r="L3" s="25" t="s">
         <v>118</v>
       </c>
@@ -3385,7 +3392,7 @@
       <c r="F11" s="27"/>
       <c r="G11" s="27"/>
       <c r="H11" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I11" s="27">
         <v>5</v>
@@ -3466,22 +3473,22 @@
       <c r="A14" s="9">
         <v>5</v>
       </c>
-      <c r="B14" s="76" t="s">
+      <c r="B14" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="76"/>
-      <c r="I14" s="76"/>
-      <c r="J14" s="76"/>
-      <c r="L14" s="72" t="s">
+      <c r="C14" s="77"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="77"/>
+      <c r="L14" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="M14" s="73"/>
-      <c r="N14" s="73"/>
+      <c r="M14" s="74"/>
+      <c r="N14" s="74"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
@@ -3570,16 +3577,16 @@
       <c r="N18" s="25"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="71" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="71"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="71"/>
+      <c r="B19" s="72"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="72"/>
       <c r="I19" s="51"/>
       <c r="J19" s="30"/>
       <c r="L19" s="29" t="s">
@@ -3658,21 +3665,21 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="65" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="66">
-        <v>4</v>
-      </c>
-      <c r="D22" s="66">
-        <v>1</v>
-      </c>
-      <c r="E22" s="66"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="65"/>
-      <c r="J22" s="66"/>
+      <c r="B22" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="68">
+        <v>4</v>
+      </c>
+      <c r="D22" s="68">
+        <v>1</v>
+      </c>
+      <c r="E22" s="68"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="68"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -3839,6 +3846,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="HkpizirgCBmsJxAfyUjPKSTIOPqPhtoe6Lx2nL9JGyc5aA/m7tusagY1QRkNkTuqssViaYUKt5eAw8C5nwkYpg==" saltValue="Y9y8ekWlbOPqhkC8OsbfyA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="8">
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="L14:N14"/>
@@ -3858,8 +3866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3879,23 +3887,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="75"/>
+      <c r="A1" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="76"/>
       <c r="I1" s="50"/>
       <c r="J1" s="30"/>
-      <c r="L1" s="72" t="s">
+      <c r="L1" s="73" t="s">
         <v>133</v>
       </c>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -3942,17 +3950,17 @@
       <c r="A3" s="55">
         <v>6</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
       <c r="L3" s="54" t="s">
         <v>118</v>
       </c>
@@ -3993,7 +4001,9 @@
       <c r="L4" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="M4" s="54"/>
+      <c r="M4" s="54">
+        <v>7</v>
+      </c>
       <c r="N4" s="54"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -4032,6 +4042,33 @@
       <c r="N5" s="54"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="27">
+        <v>4</v>
+      </c>
+      <c r="D6" s="27">
+        <v>2</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G6" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="H6" s="64" t="s">
+        <v>146</v>
+      </c>
+      <c r="I6" s="64">
+        <v>4</v>
+      </c>
       <c r="L6" s="54" t="s">
         <v>121</v>
       </c>
@@ -4039,15 +4076,33 @@
       <c r="N6" s="54"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
+      <c r="A7" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="27">
+        <v>4</v>
+      </c>
+      <c r="D7" s="27">
+        <v>2</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G7" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="I7" s="27">
+        <v>3</v>
+      </c>
       <c r="J7" s="47"/>
       <c r="L7" s="54" t="s">
         <v>122</v>
@@ -4122,7 +4177,7 @@
       </c>
       <c r="M11" s="28">
         <f>SUM(M3:M10)</f>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="N11" s="28">
         <f>SUM(N3:N10)</f>
@@ -4161,11 +4216,11 @@
       <c r="M13" s="54"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L14" s="72" t="s">
+      <c r="L14" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="M14" s="73"/>
-      <c r="N14" s="73"/>
+      <c r="M14" s="74"/>
+      <c r="N14" s="74"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
@@ -4200,7 +4255,9 @@
       <c r="L16" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="M16" s="54"/>
+      <c r="M16" s="54">
+        <v>0</v>
+      </c>
       <c r="N16" s="54"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4217,33 +4274,39 @@
       <c r="L17" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="M17" s="54"/>
+      <c r="M17" s="54">
+        <v>0</v>
+      </c>
       <c r="N17" s="54"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L18" s="54" t="s">
         <v>128</v>
       </c>
-      <c r="M18" s="54"/>
+      <c r="M18" s="54">
+        <v>3</v>
+      </c>
       <c r="N18" s="54"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="71" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="71"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="71"/>
+      <c r="B19" s="72"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="72"/>
       <c r="I19" s="51"/>
       <c r="J19" s="30"/>
       <c r="L19" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="M19" s="54"/>
+      <c r="M19" s="54">
+        <v>1</v>
+      </c>
       <c r="N19" s="54"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -4278,7 +4341,7 @@
       </c>
       <c r="M20" s="28">
         <f>SUM(M16:M19)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N20" s="28"/>
     </row>

</xml_diff>

<commit_message>
[Edison Moura] Atualizando planilha com atribuição de tarefa e horas disponíveis.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="148">
   <si>
     <t>ID</t>
   </si>
@@ -458,6 +458,9 @@
   </si>
   <si>
     <t>Em andamento</t>
+  </si>
+  <si>
+    <t>Edison</t>
   </si>
 </sst>
 </file>
@@ -1013,10 +1016,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1028,7 +1028,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1367,8 +1370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,18 +1388,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="H1" s="66" t="s">
+      <c r="A1" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="H1" s="70" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="66"/>
+      <c r="I1" s="70"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1526,21 +1529,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="67" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="68">
-        <v>4</v>
-      </c>
-      <c r="D7" s="68">
-        <v>1</v>
-      </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
-      <c r="H7" s="66" t="s">
+      <c r="B7" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="67">
+        <v>4</v>
+      </c>
+      <c r="D7" s="67">
+        <v>1</v>
+      </c>
+      <c r="E7" s="67"/>
+      <c r="F7" s="68"/>
+      <c r="H7" s="70" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="66"/>
+      <c r="I7" s="70"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1699,8 +1702,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="70"/>
-      <c r="K13" s="70"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="65"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1748,13 +1751,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="67" t="s">
+      <c r="B16" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="69"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="68"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1966,13 +1969,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="67" t="s">
+      <c r="B27" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="68"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="69"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="68"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -2036,13 +2039,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="67" t="s">
+      <c r="B31" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="68"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="69"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="68"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2288,13 +2291,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="67" t="s">
+      <c r="B47" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="68"/>
-      <c r="D47" s="68"/>
-      <c r="E47" s="68"/>
-      <c r="F47" s="69"/>
+      <c r="C47" s="67"/>
+      <c r="D47" s="67"/>
+      <c r="E47" s="67"/>
+      <c r="F47" s="68"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2412,13 +2415,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="67" t="s">
+      <c r="B55" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="68"/>
-      <c r="D55" s="68"/>
-      <c r="E55" s="68"/>
-      <c r="F55" s="69"/>
+      <c r="C55" s="67"/>
+      <c r="D55" s="67"/>
+      <c r="E55" s="67"/>
+      <c r="F55" s="68"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2486,16 +2489,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B7:F7"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B55:F55"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2703,17 +2706,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="67" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="68">
-        <v>4</v>
-      </c>
-      <c r="D7" s="68">
-        <v>1</v>
-      </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
+      <c r="B7" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="67">
+        <v>4</v>
+      </c>
+      <c r="D7" s="67">
+        <v>1</v>
+      </c>
+      <c r="E7" s="67"/>
+      <c r="F7" s="68"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -3665,21 +3668,21 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="67" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="68">
-        <v>4</v>
-      </c>
-      <c r="D22" s="68">
-        <v>1</v>
-      </c>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="69"/>
-      <c r="I22" s="67"/>
-      <c r="J22" s="68"/>
+      <c r="B22" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="67">
+        <v>4</v>
+      </c>
+      <c r="D22" s="67">
+        <v>1</v>
+      </c>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="66"/>
+      <c r="J22" s="67"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -3866,8 +3869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4111,15 +4114,33 @@
       <c r="N7" s="54"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
+      <c r="A8" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="27">
+        <v>4</v>
+      </c>
+      <c r="D8" s="27">
+        <v>3</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="I8" s="27">
+        <v>3</v>
+      </c>
       <c r="J8" s="46"/>
       <c r="L8" s="54" t="s">
         <v>124</v>
@@ -4139,9 +4160,11 @@
       <c r="I9" s="27"/>
       <c r="J9" s="46"/>
       <c r="L9" s="54" t="s">
-        <v>119</v>
-      </c>
-      <c r="M9" s="54"/>
+        <v>147</v>
+      </c>
+      <c r="M9" s="54">
+        <v>5</v>
+      </c>
       <c r="N9" s="54"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -4177,7 +4200,7 @@
       </c>
       <c r="M11" s="28">
         <f>SUM(M3:M10)</f>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="N11" s="28">
         <f>SUM(N3:N10)</f>

</xml_diff>

<commit_message>
[Gean Pereira] - Atualização da planilha de responsabilidades com o meu novo CDU, e refatoração da planilha
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
@@ -12,12 +12,12 @@
     <sheet name="Incremento 2" sheetId="3" r:id="rId3"/>
     <sheet name="Incremento 3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="150">
   <si>
     <t>ID</t>
   </si>
@@ -461,6 +461,12 @@
   </si>
   <si>
     <t>Edison</t>
+  </si>
+  <si>
+    <t>Status Programação</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 03:30</t>
   </si>
 </sst>
 </file>
@@ -840,7 +846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1016,10 +1022,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1031,7 +1037,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1062,6 +1071,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1124,7 +1149,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1159,7 +1184,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1388,18 +1413,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="H1" s="66" t="s">
+      <c r="A1" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="H1" s="71" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="66"/>
+      <c r="I1" s="71"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1540,10 +1565,10 @@
       </c>
       <c r="E7" s="68"/>
       <c r="F7" s="69"/>
-      <c r="H7" s="66" t="s">
+      <c r="H7" s="71" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="66"/>
+      <c r="I7" s="71"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1702,8 +1727,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="70"/>
-      <c r="K13" s="70"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="66"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -2489,16 +2514,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B7:F7"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B55:F55"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2527,20 +2552,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
+      <c r="A1" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
       <c r="G1" s="30"/>
-      <c r="I1" s="73" t="s">
+      <c r="I1" s="74" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -2927,11 +2952,11 @@
       <c r="G14" s="35">
         <v>0</v>
       </c>
-      <c r="I14" s="73" t="s">
+      <c r="I14" s="74" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="74"/>
-      <c r="K14" s="74"/>
+      <c r="J14" s="75"/>
+      <c r="K14" s="75"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="41" t="s">
@@ -3027,8 +3052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3047,23 +3072,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="76"/>
+      <c r="A1" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="77"/>
       <c r="I1" s="50"/>
       <c r="J1" s="30"/>
-      <c r="L1" s="73" t="s">
+      <c r="L1" s="74" t="s">
         <v>133</v>
       </c>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -3110,17 +3135,17 @@
       <c r="A3" s="39">
         <v>4</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="81"/>
       <c r="L3" s="25" t="s">
         <v>118</v>
       </c>
@@ -3476,22 +3501,22 @@
       <c r="A14" s="9">
         <v>5</v>
       </c>
-      <c r="B14" s="77" t="s">
+      <c r="B14" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
-      <c r="L14" s="73" t="s">
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="78"/>
+      <c r="J14" s="78"/>
+      <c r="L14" s="74" t="s">
         <v>102</v>
       </c>
-      <c r="M14" s="74"/>
-      <c r="N14" s="74"/>
+      <c r="M14" s="75"/>
+      <c r="N14" s="75"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
@@ -3580,16 +3605,16 @@
       <c r="N18" s="25"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="71" t="s">
+      <c r="A19" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="72"/>
-      <c r="C19" s="72"/>
-      <c r="D19" s="72"/>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="72"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
       <c r="I19" s="51"/>
       <c r="J19" s="30"/>
       <c r="L19" s="29" t="s">
@@ -3867,10 +3892,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3879,36 +3904,38 @@
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
       <c r="H1" s="76"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="30"/>
-      <c r="L1" s="73" t="s">
+      <c r="I1" s="77"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="30"/>
+      <c r="M1" s="74" t="s">
         <v>133</v>
       </c>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
@@ -3928,51 +3955,55 @@
         <v>141</v>
       </c>
       <c r="G2" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="H2" s="52" t="s">
         <v>142</v>
       </c>
-      <c r="H2" s="52" t="s">
+      <c r="I2" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="J2" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="K2" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="M2" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="N2" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="N2" s="28" t="s">
+      <c r="O2" s="28" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="55">
         <v>6</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="L3" s="54" t="s">
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="M3" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="M3" s="54">
+      <c r="N3" s="54">
         <v>6</v>
       </c>
-      <c r="N3" s="54"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="54"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>57</v>
       </c>
@@ -3991,25 +4022,28 @@
       <c r="F4" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="G4" s="54" t="s">
+      <c r="G4" s="65" t="s">
         <v>127</v>
       </c>
       <c r="H4" s="54" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" s="54" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="54">
+      <c r="J4" s="54">
         <v>3</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="L4" s="54" t="s">
+      <c r="K4" s="7"/>
+      <c r="M4" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="M4" s="54">
+      <c r="N4" s="54">
         <v>7</v>
       </c>
-      <c r="N4" s="54"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" s="54"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>59</v>
       </c>
@@ -4028,23 +4062,28 @@
       <c r="F5" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="G5" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="H5" s="62" t="s">
+      <c r="G5" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="H5" s="54" t="s">
+        <v>127</v>
+      </c>
+      <c r="I5" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="I5" s="27">
+      <c r="J5" s="27">
         <v>3</v>
       </c>
-      <c r="J5" s="47"/>
-      <c r="L5" s="54" t="s">
+      <c r="K5" s="47"/>
+      <c r="M5" s="54" t="s">
         <v>123</v>
       </c>
-      <c r="M5" s="54"/>
-      <c r="N5" s="54"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N5" s="54">
+        <v>6</v>
+      </c>
+      <c r="O5" s="54"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>42</v>
       </c>
@@ -4063,22 +4102,25 @@
       <c r="F6" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="G6" s="64" t="s">
+      <c r="G6" s="7" t="s">
         <v>127</v>
       </c>
       <c r="H6" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="I6" s="64" t="s">
         <v>146</v>
       </c>
-      <c r="I6" s="64">
-        <v>4</v>
-      </c>
-      <c r="L6" s="54" t="s">
+      <c r="J6" s="64">
+        <v>4</v>
+      </c>
+      <c r="M6" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="M6" s="54"/>
       <c r="N6" s="54"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" s="54"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>44</v>
       </c>
@@ -4097,23 +4139,26 @@
       <c r="F7" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="G7" s="64" t="s">
-        <v>127</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="I7" s="27">
+      <c r="G7" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="J7" s="27">
         <v>3</v>
       </c>
-      <c r="J7" s="47"/>
-      <c r="L7" s="54" t="s">
+      <c r="K7" s="47"/>
+      <c r="M7" s="54" t="s">
         <v>122</v>
       </c>
-      <c r="M7" s="54"/>
       <c r="N7" s="54"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" s="54"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>86</v>
       </c>
@@ -4138,17 +4183,20 @@
       <c r="H8" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="I8" s="27">
+      <c r="I8" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="J8" s="27">
         <v>3</v>
       </c>
-      <c r="J8" s="46"/>
-      <c r="L8" s="54" t="s">
+      <c r="K8" s="46"/>
+      <c r="M8" s="54" t="s">
         <v>124</v>
       </c>
-      <c r="M8" s="54"/>
       <c r="N8" s="54"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" s="54"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>100</v>
       </c>
@@ -4173,36 +4221,60 @@
       <c r="H9" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="I9" s="27">
+      <c r="I9" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="J9" s="27">
         <v>2</v>
       </c>
-      <c r="J9" s="46"/>
-      <c r="L9" s="54" t="s">
+      <c r="K9" s="46"/>
+      <c r="M9" s="54" t="s">
         <v>147</v>
       </c>
-      <c r="M9" s="54">
+      <c r="N9" s="54">
         <v>5</v>
       </c>
-      <c r="N9" s="54"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="46"/>
-      <c r="L10" s="54" t="s">
+      <c r="O9" s="54"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="27">
+        <v>4</v>
+      </c>
+      <c r="D10" s="27">
+        <v>2</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="H10" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="I10" s="65" t="s">
+        <v>146</v>
+      </c>
+      <c r="J10" s="27">
+        <v>3</v>
+      </c>
+      <c r="K10" s="46"/>
+      <c r="M10" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="M10" s="54"/>
-      <c r="N10" s="53"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N10" s="54"/>
+      <c r="O10" s="53"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="33"/>
       <c r="B11" s="3"/>
       <c r="C11" s="27"/>
@@ -4212,20 +4284,21 @@
       <c r="G11" s="27"/>
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
-      <c r="J11" s="46"/>
-      <c r="L11" s="28" t="s">
+      <c r="J11" s="27"/>
+      <c r="K11" s="46"/>
+      <c r="M11" s="28" t="s">
         <v>135</v>
-      </c>
-      <c r="M11" s="28">
-        <f>SUM(M3:M10)</f>
-        <v>18</v>
       </c>
       <c r="N11" s="28">
         <f>SUM(N3:N10)</f>
+        <v>24</v>
+      </c>
+      <c r="O11" s="28">
+        <f>SUM(O3:O10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="33"/>
       <c r="B12" s="3"/>
       <c r="C12" s="27"/>
@@ -4235,15 +4308,16 @@
       <c r="G12" s="27"/>
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
-      <c r="J12" s="46"/>
-      <c r="L12" s="63" t="s">
+      <c r="J12" s="27"/>
+      <c r="K12" s="46"/>
+      <c r="M12" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="M12" s="63">
+      <c r="N12" s="63">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="33"/>
       <c r="B13" s="3"/>
       <c r="C13" s="27"/>
@@ -4253,17 +4327,18 @@
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
-      <c r="J13" s="46"/>
-      <c r="M13" s="54"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L14" s="73" t="s">
+      <c r="J13" s="27"/>
+      <c r="K13" s="46"/>
+      <c r="N13" s="54"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M14" s="74" t="s">
         <v>102</v>
       </c>
-      <c r="M14" s="74"/>
-      <c r="N14" s="74"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N14" s="75"/>
+      <c r="O14" s="75"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
       <c r="B15" s="3"/>
       <c r="C15" s="27"/>
@@ -4273,16 +4348,17 @@
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
-      <c r="J15" s="46"/>
-      <c r="L15" s="54" t="s">
+      <c r="J15" s="27"/>
+      <c r="K15" s="46"/>
+      <c r="M15" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="M15" s="54" t="s">
+      <c r="N15" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="N15" s="54"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="54"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
       <c r="B16" s="3"/>
       <c r="C16" s="27"/>
@@ -4292,16 +4368,17 @@
       <c r="G16" s="27"/>
       <c r="H16" s="27"/>
       <c r="I16" s="27"/>
-      <c r="J16" s="48"/>
-      <c r="L16" s="54" t="s">
+      <c r="J16" s="27"/>
+      <c r="K16" s="48"/>
+      <c r="M16" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="M16" s="54">
+      <c r="N16" s="54">
         <v>0</v>
       </c>
-      <c r="N16" s="54"/>
-    </row>
-    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O16" s="54"/>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="41"/>
       <c r="B17" s="42"/>
       <c r="C17" s="43"/>
@@ -4311,46 +4388,48 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="49"/>
-      <c r="L17" s="54" t="s">
+      <c r="J17" s="6"/>
+      <c r="K17" s="49"/>
+      <c r="M17" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="M17" s="54">
-        <v>0</v>
-      </c>
-      <c r="N17" s="54"/>
-    </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L18" s="54" t="s">
+      <c r="N17" s="54">
+        <v>2</v>
+      </c>
+      <c r="O17" s="54"/>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M18" s="54" t="s">
         <v>128</v>
       </c>
-      <c r="M18" s="54">
-        <v>3</v>
-      </c>
-      <c r="N18" s="54"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="71" t="s">
+      <c r="N18" s="54">
+        <v>4</v>
+      </c>
+      <c r="O18" s="54"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="72"/>
-      <c r="C19" s="72"/>
-      <c r="D19" s="72"/>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="30"/>
-      <c r="L19" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="M19" s="54">
-        <v>1</v>
-      </c>
-      <c r="N19" s="54"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="73"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="73"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="30"/>
+      <c r="M19" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="N19" s="54">
+        <v>5</v>
+      </c>
+      <c r="O19" s="54"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>0</v>
       </c>
@@ -4366,75 +4445,174 @@
       <c r="E20" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19" t="s">
+      <c r="F20" s="52" t="s">
+        <v>141</v>
+      </c>
+      <c r="G20" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="H20" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="I20" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="I20" s="19" t="s">
+      <c r="J20" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="J20" s="19" t="s">
+      <c r="K20" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="L20" s="28" t="s">
+      <c r="M20" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="M20" s="28">
-        <f>SUM(M16:M19)</f>
-        <v>4</v>
-      </c>
-      <c r="N20" s="28"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="46"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="35"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="33"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="35"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="33"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="35"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N20" s="28">
+        <f>SUM(N16:N19)</f>
+        <v>11</v>
+      </c>
+      <c r="O20" s="28"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="27">
+        <v>4</v>
+      </c>
+      <c r="D21" s="27">
+        <v>2</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="I21" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="J21" s="82">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K21" s="46">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="27">
+        <v>4</v>
+      </c>
+      <c r="D22" s="27">
+        <v>1</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="J22" s="35">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K22" s="35">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="59">
+        <v>4</v>
+      </c>
+      <c r="D23" s="59">
+        <v>1</v>
+      </c>
+      <c r="E23" s="59" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="G23" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="H23" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="I23" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="J23" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="K23" s="60" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="84" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="85">
+        <v>4</v>
+      </c>
+      <c r="D24" s="85">
+        <v>1</v>
+      </c>
+      <c r="E24" s="85" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" s="86" t="s">
+        <v>127</v>
+      </c>
+      <c r="G24" s="86" t="s">
+        <v>127</v>
+      </c>
+      <c r="H24" s="86" t="s">
+        <v>127</v>
+      </c>
+      <c r="I24" s="86" t="s">
+        <v>127</v>
+      </c>
+      <c r="J24" s="87">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K24" s="87">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="57"/>
       <c r="B25" s="58"/>
       <c r="C25" s="59"/>
@@ -4442,11 +4620,12 @@
       <c r="E25" s="59"/>
       <c r="F25" s="59"/>
       <c r="G25" s="59"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="60"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H25" s="59"/>
+      <c r="I25" s="56"/>
+      <c r="J25" s="59"/>
+      <c r="K25" s="60"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="33"/>
       <c r="B26" s="3"/>
       <c r="C26" s="27"/>
@@ -4454,11 +4633,12 @@
       <c r="E26" s="27"/>
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="35"/>
-    </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H26" s="27"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="35"/>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="41"/>
       <c r="B27" s="42"/>
       <c r="C27" s="43"/>
@@ -4466,17 +4646,18 @@
       <c r="E27" s="43"/>
       <c r="F27" s="43"/>
       <c r="G27" s="43"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="45"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="A19:I19"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Gean Pereira] - Outra refatoração
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="151">
   <si>
     <t>ID</t>
   </si>
@@ -467,6 +467,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 03:30</t>
+  </si>
+  <si>
+    <t>Status Testes</t>
   </si>
 </sst>
 </file>
@@ -846,7 +849,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1028,6 +1031,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1037,10 +1062,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1071,22 +1093,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1413,18 +1419,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="H1" s="71" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="H1" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="71"/>
+      <c r="I1" s="74"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1554,21 +1560,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="67" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="68">
-        <v>4</v>
-      </c>
-      <c r="D7" s="68">
+      <c r="B7" s="75" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="76">
+        <v>4</v>
+      </c>
+      <c r="D7" s="76">
         <v>1</v>
       </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
-      <c r="H7" s="71" t="s">
+      <c r="E7" s="76"/>
+      <c r="F7" s="77"/>
+      <c r="H7" s="74" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="71"/>
+      <c r="I7" s="74"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1727,8 +1733,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="66"/>
-      <c r="K13" s="66"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="78"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1776,13 +1782,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="67" t="s">
+      <c r="B16" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="69"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="77"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1994,13 +2000,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="67" t="s">
+      <c r="B27" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="68"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="69"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="77"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -2064,13 +2070,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="67" t="s">
+      <c r="B31" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="68"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="69"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="76"/>
+      <c r="F31" s="77"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2316,13 +2322,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="67" t="s">
+      <c r="B47" s="75" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="68"/>
-      <c r="D47" s="68"/>
-      <c r="E47" s="68"/>
-      <c r="F47" s="69"/>
+      <c r="C47" s="76"/>
+      <c r="D47" s="76"/>
+      <c r="E47" s="76"/>
+      <c r="F47" s="77"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2440,13 +2446,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="67" t="s">
+      <c r="B55" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="68"/>
-      <c r="D55" s="68"/>
-      <c r="E55" s="68"/>
-      <c r="F55" s="69"/>
+      <c r="C55" s="76"/>
+      <c r="D55" s="76"/>
+      <c r="E55" s="76"/>
+      <c r="F55" s="77"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2514,16 +2520,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B55:F55"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B7:F7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B55:F55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2552,20 +2558,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
       <c r="G1" s="30"/>
-      <c r="I1" s="74" t="s">
+      <c r="I1" s="81" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -2731,17 +2737,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="67" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="68">
-        <v>4</v>
-      </c>
-      <c r="D7" s="68">
+      <c r="B7" s="75" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="76">
+        <v>4</v>
+      </c>
+      <c r="D7" s="76">
         <v>1</v>
       </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="77"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -2952,11 +2958,11 @@
       <c r="G14" s="35">
         <v>0</v>
       </c>
-      <c r="I14" s="74" t="s">
+      <c r="I14" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="75"/>
-      <c r="K14" s="75"/>
+      <c r="J14" s="82"/>
+      <c r="K14" s="82"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="41" t="s">
@@ -3072,23 +3078,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="77"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="84"/>
       <c r="I1" s="50"/>
       <c r="J1" s="30"/>
-      <c r="L1" s="74" t="s">
+      <c r="L1" s="81" t="s">
         <v>133</v>
       </c>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -3135,17 +3141,17 @@
       <c r="A3" s="39">
         <v>4</v>
       </c>
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="81"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="88"/>
       <c r="L3" s="25" t="s">
         <v>118</v>
       </c>
@@ -3501,22 +3507,22 @@
       <c r="A14" s="9">
         <v>5</v>
       </c>
-      <c r="B14" s="78" t="s">
+      <c r="B14" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="L14" s="74" t="s">
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="85"/>
+      <c r="L14" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="M14" s="75"/>
-      <c r="N14" s="75"/>
+      <c r="M14" s="82"/>
+      <c r="N14" s="82"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
@@ -3605,16 +3611,16 @@
       <c r="N18" s="25"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="72" t="s">
+      <c r="A19" s="79" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="73"/>
+      <c r="B19" s="80"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="80"/>
       <c r="I19" s="51"/>
       <c r="J19" s="30"/>
       <c r="L19" s="29" t="s">
@@ -3693,21 +3699,21 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="67" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="68">
-        <v>4</v>
-      </c>
-      <c r="D22" s="68">
+      <c r="B22" s="75" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="76">
+        <v>4</v>
+      </c>
+      <c r="D22" s="76">
         <v>1</v>
       </c>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="69"/>
-      <c r="I22" s="67"/>
-      <c r="J22" s="68"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="75"/>
+      <c r="J22" s="76"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -3892,10 +3898,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3905,37 +3911,38 @@
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="26.42578125" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="30"/>
-      <c r="M1" s="74" t="s">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="30"/>
+      <c r="N1" s="81" t="s">
         <v>133</v>
       </c>
-      <c r="N1" s="75"/>
-      <c r="O1" s="75"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
@@ -3958,52 +3965,56 @@
         <v>148</v>
       </c>
       <c r="H2" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="I2" s="52" t="s">
         <v>142</v>
       </c>
-      <c r="I2" s="52" t="s">
+      <c r="J2" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="K2" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="L2" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="N2" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="N2" s="28" t="s">
+      <c r="O2" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="O2" s="28" t="s">
+      <c r="P2" s="28" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="55">
         <v>6</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="M3" s="54" t="s">
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="N3" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="N3" s="54">
+      <c r="O3" s="54">
         <v>6</v>
       </c>
-      <c r="O3" s="54"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3" s="54"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>57</v>
       </c>
@@ -4025,25 +4036,28 @@
       <c r="G4" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="H4" s="54" t="s">
+      <c r="H4" s="66" t="s">
         <v>127</v>
       </c>
       <c r="I4" s="54" t="s">
+        <v>127</v>
+      </c>
+      <c r="J4" s="54" t="s">
         <v>146</v>
       </c>
-      <c r="J4" s="54">
+      <c r="K4" s="54">
         <v>3</v>
       </c>
-      <c r="K4" s="7"/>
-      <c r="M4" s="54" t="s">
+      <c r="L4" s="7"/>
+      <c r="N4" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="N4" s="54">
+      <c r="O4" s="54">
         <v>7</v>
       </c>
-      <c r="O4" s="54"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="54"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>59</v>
       </c>
@@ -4065,25 +4079,28 @@
       <c r="G5" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="H5" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="I5" s="62" t="s">
+      <c r="H5" s="66" t="s">
+        <v>127</v>
+      </c>
+      <c r="I5" s="54" t="s">
+        <v>127</v>
+      </c>
+      <c r="J5" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="J5" s="27">
+      <c r="K5" s="27">
         <v>3</v>
       </c>
-      <c r="K5" s="47"/>
-      <c r="M5" s="54" t="s">
+      <c r="L5" s="47"/>
+      <c r="N5" s="54" t="s">
         <v>123</v>
       </c>
-      <c r="N5" s="54">
+      <c r="O5" s="54">
         <v>6</v>
       </c>
-      <c r="O5" s="54"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="54"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>42</v>
       </c>
@@ -4105,22 +4122,25 @@
       <c r="G6" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="H6" s="64" t="s">
+      <c r="H6" s="66" t="s">
         <v>127</v>
       </c>
       <c r="I6" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="J6" s="64" t="s">
         <v>146</v>
       </c>
-      <c r="J6" s="64">
-        <v>4</v>
-      </c>
-      <c r="M6" s="54" t="s">
+      <c r="K6" s="64">
+        <v>4</v>
+      </c>
+      <c r="N6" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="N6" s="54"/>
       <c r="O6" s="54"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" s="54"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>44</v>
       </c>
@@ -4142,23 +4162,26 @@
       <c r="G7" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="H7" s="64" t="s">
-        <v>127</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="J7" s="27">
+      <c r="H7" s="66" t="s">
+        <v>127</v>
+      </c>
+      <c r="I7" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="K7" s="27">
         <v>3</v>
       </c>
-      <c r="K7" s="47"/>
-      <c r="M7" s="54" t="s">
+      <c r="L7" s="47"/>
+      <c r="N7" s="54" t="s">
         <v>122</v>
       </c>
-      <c r="N7" s="54"/>
       <c r="O7" s="54"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" s="54"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>86</v>
       </c>
@@ -4180,23 +4203,26 @@
       <c r="G8" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="66" t="s">
         <v>127</v>
       </c>
       <c r="I8" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="J8" s="27">
+      <c r="J8" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="K8" s="27">
         <v>3</v>
       </c>
-      <c r="K8" s="46"/>
-      <c r="M8" s="54" t="s">
+      <c r="L8" s="46"/>
+      <c r="N8" s="54" t="s">
         <v>124</v>
       </c>
-      <c r="N8" s="54"/>
       <c r="O8" s="54"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" s="54"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>100</v>
       </c>
@@ -4218,25 +4244,28 @@
       <c r="G9" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="H9" s="66" t="s">
         <v>127</v>
       </c>
       <c r="I9" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="K9" s="27">
         <v>2</v>
       </c>
-      <c r="K9" s="46"/>
-      <c r="M9" s="54" t="s">
+      <c r="L9" s="46"/>
+      <c r="N9" s="54" t="s">
         <v>147</v>
       </c>
-      <c r="N9" s="54">
+      <c r="O9" s="54">
         <v>5</v>
       </c>
-      <c r="O9" s="54"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9" s="54"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>27</v>
       </c>
@@ -4258,23 +4287,26 @@
       <c r="G10" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="H10" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="I10" s="65" t="s">
+      <c r="H10" s="66" t="s">
+        <v>127</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="J10" s="65" t="s">
         <v>146</v>
       </c>
-      <c r="J10" s="27">
+      <c r="K10" s="27">
         <v>3</v>
       </c>
-      <c r="K10" s="46"/>
-      <c r="M10" s="54" t="s">
+      <c r="L10" s="46"/>
+      <c r="N10" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="N10" s="54"/>
-      <c r="O10" s="53"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O10" s="54"/>
+      <c r="P10" s="53"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="33"/>
       <c r="B11" s="3"/>
       <c r="C11" s="27"/>
@@ -4285,20 +4317,21 @@
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
       <c r="J11" s="27"/>
-      <c r="K11" s="46"/>
-      <c r="M11" s="28" t="s">
+      <c r="K11" s="27"/>
+      <c r="L11" s="46"/>
+      <c r="N11" s="28" t="s">
         <v>135</v>
-      </c>
-      <c r="N11" s="28">
-        <f>SUM(N3:N10)</f>
-        <v>24</v>
       </c>
       <c r="O11" s="28">
         <f>SUM(O3:O10)</f>
+        <v>24</v>
+      </c>
+      <c r="P11" s="28">
+        <f>SUM(P3:P10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="33"/>
       <c r="B12" s="3"/>
       <c r="C12" s="27"/>
@@ -4309,15 +4342,16 @@
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
-      <c r="K12" s="46"/>
-      <c r="M12" s="63" t="s">
+      <c r="K12" s="27"/>
+      <c r="L12" s="46"/>
+      <c r="N12" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="N12" s="63">
+      <c r="O12" s="63">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="33"/>
       <c r="B13" s="3"/>
       <c r="C13" s="27"/>
@@ -4328,17 +4362,18 @@
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
-      <c r="K13" s="46"/>
-      <c r="N13" s="54"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M14" s="74" t="s">
+      <c r="K13" s="27"/>
+      <c r="L13" s="46"/>
+      <c r="O13" s="54"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N14" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="N14" s="75"/>
-      <c r="O14" s="75"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O14" s="82"/>
+      <c r="P14" s="82"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
       <c r="B15" s="3"/>
       <c r="C15" s="27"/>
@@ -4349,16 +4384,17 @@
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
-      <c r="K15" s="46"/>
-      <c r="M15" s="54" t="s">
+      <c r="K15" s="27"/>
+      <c r="L15" s="46"/>
+      <c r="N15" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="N15" s="54" t="s">
+      <c r="O15" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="O15" s="54"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15" s="54"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
       <c r="B16" s="3"/>
       <c r="C16" s="27"/>
@@ -4369,16 +4405,17 @@
       <c r="H16" s="27"/>
       <c r="I16" s="27"/>
       <c r="J16" s="27"/>
-      <c r="K16" s="48"/>
-      <c r="M16" s="54" t="s">
+      <c r="K16" s="27"/>
+      <c r="L16" s="48"/>
+      <c r="N16" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="N16" s="54">
+      <c r="O16" s="54">
         <v>0</v>
       </c>
-      <c r="O16" s="54"/>
-    </row>
-    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P16" s="54"/>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="41"/>
       <c r="B17" s="42"/>
       <c r="C17" s="43"/>
@@ -4389,47 +4426,49 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="49"/>
-      <c r="M17" s="54" t="s">
+      <c r="K17" s="6"/>
+      <c r="L17" s="49"/>
+      <c r="N17" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="N17" s="54">
+      <c r="O17" s="54">
         <v>2</v>
       </c>
-      <c r="O17" s="54"/>
-    </row>
-    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M18" s="54" t="s">
+      <c r="P17" s="54"/>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N18" s="54" t="s">
         <v>128</v>
       </c>
-      <c r="N18" s="54">
-        <v>4</v>
-      </c>
-      <c r="O18" s="54"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="72" t="s">
+      <c r="O18" s="54">
+        <v>4</v>
+      </c>
+      <c r="P18" s="54"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="79" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="30"/>
-      <c r="M19" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="N19" s="54">
+      <c r="B19" s="80"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="80"/>
+      <c r="I19" s="80"/>
+      <c r="J19" s="80"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="30"/>
+      <c r="N19" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="O19" s="54">
         <v>5</v>
       </c>
-      <c r="O19" s="54"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19" s="54"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>0</v>
       </c>
@@ -4452,27 +4491,30 @@
         <v>148</v>
       </c>
       <c r="H20" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="I20" s="52" t="s">
         <v>142</v>
       </c>
-      <c r="I20" s="19" t="s">
+      <c r="J20" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="J20" s="19" t="s">
+      <c r="K20" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="K20" s="19" t="s">
+      <c r="L20" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="M20" s="28" t="s">
+      <c r="N20" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="N20" s="28">
-        <f>SUM(N16:N19)</f>
+      <c r="O20" s="28">
+        <f>SUM(O16:O19)</f>
         <v>11</v>
       </c>
-      <c r="O20" s="28"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20" s="28"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
         <v>29</v>
       </c>
@@ -4497,17 +4539,20 @@
       <c r="H21" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="I21" s="27" t="s">
+      <c r="I21" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="J21" s="82">
+      <c r="J21" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="K21" s="67">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="K21" s="46">
+      <c r="L21" s="46">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
         <v>16</v>
       </c>
@@ -4535,14 +4580,17 @@
       <c r="I22" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="J22" s="35">
-        <v>8.3333333333333329E-2</v>
+      <c r="J22" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="K22" s="35">
         <v>8.3333333333333329E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L22" s="35">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="57" t="s">
         <v>13</v>
       </c>
@@ -4570,49 +4618,55 @@
       <c r="I23" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="J23" s="60" t="s">
+      <c r="J23" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="K23" s="60" t="s">
         <v>149</v>
       </c>
-      <c r="K23" s="60" t="s">
+      <c r="L23" s="60" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="83" t="s">
+    <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="84" t="s">
+      <c r="B24" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="85">
-        <v>4</v>
-      </c>
-      <c r="D24" s="85">
+      <c r="C24" s="70">
+        <v>4</v>
+      </c>
+      <c r="D24" s="70">
         <v>1</v>
       </c>
-      <c r="E24" s="85" t="s">
+      <c r="E24" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="F24" s="86" t="s">
-        <v>127</v>
-      </c>
-      <c r="G24" s="86" t="s">
-        <v>127</v>
-      </c>
-      <c r="H24" s="86" t="s">
-        <v>127</v>
-      </c>
-      <c r="I24" s="86" t="s">
-        <v>127</v>
-      </c>
-      <c r="J24" s="87">
+      <c r="F24" s="71" t="s">
+        <v>127</v>
+      </c>
+      <c r="G24" s="71" t="s">
+        <v>127</v>
+      </c>
+      <c r="H24" s="71" t="s">
+        <v>127</v>
+      </c>
+      <c r="I24" s="71" t="s">
+        <v>127</v>
+      </c>
+      <c r="J24" s="71" t="s">
+        <v>127</v>
+      </c>
+      <c r="K24" s="72">
         <v>0.16666666666666666</v>
       </c>
-      <c r="K24" s="87">
+      <c r="L24" s="72">
         <v>0.125</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="57"/>
       <c r="B25" s="58"/>
       <c r="C25" s="59"/>
@@ -4621,11 +4675,12 @@
       <c r="F25" s="59"/>
       <c r="G25" s="59"/>
       <c r="H25" s="59"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="60"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I25" s="59"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="59"/>
+      <c r="L25" s="60"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="33"/>
       <c r="B26" s="3"/>
       <c r="C26" s="27"/>
@@ -4634,11 +4689,12 @@
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="35"/>
-    </row>
-    <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I26" s="27"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="35"/>
+    </row>
+    <row r="27" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="41"/>
       <c r="B27" s="42"/>
       <c r="C27" s="43"/>
@@ -4647,17 +4703,18 @@
       <c r="F27" s="43"/>
       <c r="G27" s="43"/>
       <c r="H27" s="43"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="45"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="A19:I19"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="A19:J19"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Edison Moura] Atualizando planilha
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
@@ -12,12 +12,12 @@
     <sheet name="Incremento 2" sheetId="3" r:id="rId3"/>
     <sheet name="Incremento 3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="152">
   <si>
     <t>ID</t>
   </si>
@@ -470,6 +470,9 @@
   </si>
   <si>
     <t>Status Testes</t>
+  </si>
+  <si>
+    <t>0.5</t>
   </si>
 </sst>
 </file>
@@ -849,7 +852,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1047,10 +1050,7 @@
     <xf numFmtId="20" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1062,7 +1062,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1093,6 +1096,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1155,7 +1161,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1190,7 +1196,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1419,18 +1425,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="H1" s="74" t="s">
+      <c r="A1" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="H1" s="78" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="74"/>
+      <c r="I1" s="78"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1560,21 +1566,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="75" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="76">
-        <v>4</v>
-      </c>
-      <c r="D7" s="76">
-        <v>1</v>
-      </c>
-      <c r="E7" s="76"/>
-      <c r="F7" s="77"/>
-      <c r="H7" s="74" t="s">
+      <c r="B7" s="74" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="75">
+        <v>4</v>
+      </c>
+      <c r="D7" s="75">
+        <v>1</v>
+      </c>
+      <c r="E7" s="75"/>
+      <c r="F7" s="76"/>
+      <c r="H7" s="78" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="74"/>
+      <c r="I7" s="78"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1733,8 +1739,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1782,13 +1788,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="76"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="77"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="76"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2000,13 +2006,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="75" t="s">
+      <c r="B27" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="76"/>
-      <c r="D27" s="76"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="77"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="76"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -2070,13 +2076,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="75" t="s">
+      <c r="B31" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="76"/>
-      <c r="D31" s="76"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="77"/>
+      <c r="C31" s="75"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="75"/>
+      <c r="F31" s="76"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2322,13 +2328,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="75" t="s">
+      <c r="B47" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="76"/>
-      <c r="D47" s="76"/>
-      <c r="E47" s="76"/>
-      <c r="F47" s="77"/>
+      <c r="C47" s="75"/>
+      <c r="D47" s="75"/>
+      <c r="E47" s="75"/>
+      <c r="F47" s="76"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2446,13 +2452,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="75" t="s">
+      <c r="B55" s="74" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="76"/>
-      <c r="D55" s="76"/>
-      <c r="E55" s="76"/>
-      <c r="F55" s="77"/>
+      <c r="C55" s="75"/>
+      <c r="D55" s="75"/>
+      <c r="E55" s="75"/>
+      <c r="F55" s="76"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2520,16 +2526,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B7:F7"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B55:F55"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2737,17 +2743,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="75" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="76">
-        <v>4</v>
-      </c>
-      <c r="D7" s="76">
-        <v>1</v>
-      </c>
-      <c r="E7" s="76"/>
-      <c r="F7" s="77"/>
+      <c r="B7" s="74" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="75">
+        <v>4</v>
+      </c>
+      <c r="D7" s="75">
+        <v>1</v>
+      </c>
+      <c r="E7" s="75"/>
+      <c r="F7" s="76"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -3058,8 +3064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3699,21 +3705,21 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="75" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="76">
-        <v>4</v>
-      </c>
-      <c r="D22" s="76">
-        <v>1</v>
-      </c>
-      <c r="E22" s="76"/>
-      <c r="F22" s="76"/>
-      <c r="G22" s="76"/>
-      <c r="H22" s="77"/>
-      <c r="I22" s="75"/>
-      <c r="J22" s="76"/>
+      <c r="B22" s="74" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="75">
+        <v>4</v>
+      </c>
+      <c r="D22" s="75">
+        <v>1</v>
+      </c>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="75"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -3900,8 +3906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4201,7 +4207,7 @@
         <v>127</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="H8" s="66" t="s">
         <v>127</v>
@@ -4210,12 +4216,14 @@
         <v>127</v>
       </c>
       <c r="J8" s="27" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="K8" s="27">
         <v>3</v>
       </c>
-      <c r="L8" s="46"/>
+      <c r="L8" s="46" t="s">
+        <v>151</v>
+      </c>
       <c r="N8" s="54" t="s">
         <v>124</v>
       </c>
@@ -4242,7 +4250,7 @@
         <v>127</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="H9" s="66" t="s">
         <v>127</v>
@@ -4251,19 +4259,23 @@
         <v>127</v>
       </c>
       <c r="J9" s="27" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="K9" s="27">
         <v>2</v>
       </c>
-      <c r="L9" s="46"/>
+      <c r="L9" s="46" t="s">
+        <v>151</v>
+      </c>
       <c r="N9" s="54" t="s">
         <v>147</v>
       </c>
       <c r="O9" s="54">
         <v>5</v>
       </c>
-      <c r="P9" s="54"/>
+      <c r="P9" s="54">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
@@ -4328,7 +4340,7 @@
       </c>
       <c r="P11" s="28">
         <f>SUM(P3:P10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -4609,8 +4621,8 @@
       <c r="F23" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="G23" s="56" t="s">
-        <v>127</v>
+      <c r="G23" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="H23" s="56" t="s">
         <v>127</v>
@@ -4618,8 +4630,8 @@
       <c r="I23" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="J23" s="56" t="s">
-        <v>127</v>
+      <c r="J23" s="89" t="s">
+        <v>146</v>
       </c>
       <c r="K23" s="60" t="s">
         <v>149</v>

</xml_diff>

<commit_message>
[Douglas Giordano] - Atualizado planilha de responsabilidade e refatorado relatorio de julgamento prova de titulos.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="153">
   <si>
     <t>ID</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t>0.5</t>
+  </si>
+  <si>
+    <t>Finalizado</t>
   </si>
 </sst>
 </file>
@@ -852,7 +855,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1053,6 +1056,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1062,10 +1074,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1096,9 +1105,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1425,18 +1431,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="H1" s="78" t="s">
+      <c r="A1" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="H1" s="76" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="78"/>
+      <c r="I1" s="76"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1566,21 +1572,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="74" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="75">
-        <v>4</v>
-      </c>
-      <c r="D7" s="75">
-        <v>1</v>
-      </c>
-      <c r="E7" s="75"/>
-      <c r="F7" s="76"/>
-      <c r="H7" s="78" t="s">
+      <c r="B7" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="78">
+        <v>4</v>
+      </c>
+      <c r="D7" s="78">
+        <v>1</v>
+      </c>
+      <c r="E7" s="78"/>
+      <c r="F7" s="79"/>
+      <c r="H7" s="76" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="78"/>
+      <c r="I7" s="76"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1739,8 +1745,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="73"/>
-      <c r="K13" s="73"/>
+      <c r="J13" s="80"/>
+      <c r="K13" s="80"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1788,13 +1794,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="74" t="s">
+      <c r="B16" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="76"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="79"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2006,13 +2012,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="74" t="s">
+      <c r="B27" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="76"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="79"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -2076,13 +2082,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="74" t="s">
+      <c r="B31" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="76"/>
+      <c r="C31" s="78"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="78"/>
+      <c r="F31" s="79"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2328,13 +2334,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="74" t="s">
+      <c r="B47" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="75"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="75"/>
-      <c r="F47" s="76"/>
+      <c r="C47" s="78"/>
+      <c r="D47" s="78"/>
+      <c r="E47" s="78"/>
+      <c r="F47" s="79"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2452,13 +2458,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="74" t="s">
+      <c r="B55" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="75"/>
-      <c r="D55" s="75"/>
-      <c r="E55" s="75"/>
-      <c r="F55" s="76"/>
+      <c r="C55" s="78"/>
+      <c r="D55" s="78"/>
+      <c r="E55" s="78"/>
+      <c r="F55" s="79"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2526,16 +2532,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B55:F55"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B7:F7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B55:F55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2564,20 +2570,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
+      <c r="A1" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
       <c r="G1" s="30"/>
-      <c r="I1" s="81" t="s">
+      <c r="I1" s="83" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -2743,17 +2749,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="74" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="75">
-        <v>4</v>
-      </c>
-      <c r="D7" s="75">
-        <v>1</v>
-      </c>
-      <c r="E7" s="75"/>
-      <c r="F7" s="76"/>
+      <c r="B7" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="78">
+        <v>4</v>
+      </c>
+      <c r="D7" s="78">
+        <v>1</v>
+      </c>
+      <c r="E7" s="78"/>
+      <c r="F7" s="79"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -2964,11 +2970,11 @@
       <c r="G14" s="35">
         <v>0</v>
       </c>
-      <c r="I14" s="81" t="s">
+      <c r="I14" s="83" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="82"/>
-      <c r="K14" s="82"/>
+      <c r="J14" s="84"/>
+      <c r="K14" s="84"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="41" t="s">
@@ -3084,23 +3090,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="84"/>
+      <c r="A1" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="86"/>
       <c r="I1" s="50"/>
       <c r="J1" s="30"/>
-      <c r="L1" s="81" t="s">
+      <c r="L1" s="83" t="s">
         <v>133</v>
       </c>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -3147,17 +3153,17 @@
       <c r="A3" s="39">
         <v>4</v>
       </c>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="88"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="90"/>
       <c r="L3" s="25" t="s">
         <v>118</v>
       </c>
@@ -3513,22 +3519,22 @@
       <c r="A14" s="9">
         <v>5</v>
       </c>
-      <c r="B14" s="85" t="s">
+      <c r="B14" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="85"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="85"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="85"/>
-      <c r="I14" s="85"/>
-      <c r="J14" s="85"/>
-      <c r="L14" s="81" t="s">
+      <c r="C14" s="87"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="87"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="87"/>
+      <c r="I14" s="87"/>
+      <c r="J14" s="87"/>
+      <c r="L14" s="83" t="s">
         <v>102</v>
       </c>
-      <c r="M14" s="82"/>
-      <c r="N14" s="82"/>
+      <c r="M14" s="84"/>
+      <c r="N14" s="84"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
@@ -3617,16 +3623,16 @@
       <c r="N18" s="25"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="79" t="s">
+      <c r="A19" s="81" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="80"/>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="80"/>
-      <c r="G19" s="80"/>
-      <c r="H19" s="80"/>
+      <c r="B19" s="82"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="82"/>
+      <c r="H19" s="82"/>
       <c r="I19" s="51"/>
       <c r="J19" s="30"/>
       <c r="L19" s="29" t="s">
@@ -3705,21 +3711,21 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="74" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="75">
-        <v>4</v>
-      </c>
-      <c r="D22" s="75">
-        <v>1</v>
-      </c>
-      <c r="E22" s="75"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="76"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="75"/>
+      <c r="B22" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="78">
+        <v>4</v>
+      </c>
+      <c r="D22" s="78">
+        <v>1</v>
+      </c>
+      <c r="E22" s="78"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="77"/>
+      <c r="J22" s="78"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -3906,8 +3912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3928,25 +3934,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="84"/>
+      <c r="A1" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="86"/>
       <c r="K1" s="50"/>
       <c r="L1" s="30"/>
-      <c r="N1" s="81" t="s">
+      <c r="N1" s="83" t="s">
         <v>133</v>
       </c>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -3999,19 +4005,19 @@
       <c r="A3" s="55">
         <v>6</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
       <c r="N3" s="54" t="s">
         <v>118</v>
       </c>
@@ -4061,7 +4067,9 @@
       <c r="O4" s="54">
         <v>7</v>
       </c>
-      <c r="P4" s="54"/>
+      <c r="P4" s="54">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
@@ -4123,10 +4131,10 @@
         <v>117</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="H6" s="66" t="s">
         <v>127</v>
@@ -4139,6 +4147,9 @@
       </c>
       <c r="K6" s="64">
         <v>4</v>
+      </c>
+      <c r="L6" s="73">
+        <v>3</v>
       </c>
       <c r="N6" s="54" t="s">
         <v>121</v>
@@ -4163,10 +4174,10 @@
         <v>117</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="H7" s="66" t="s">
         <v>127</v>
@@ -4340,7 +4351,7 @@
       </c>
       <c r="P11" s="28">
         <f>SUM(P3:P10)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -4379,11 +4390,11 @@
       <c r="O13" s="54"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N14" s="81" t="s">
+      <c r="N14" s="83" t="s">
         <v>102</v>
       </c>
-      <c r="O14" s="82"/>
-      <c r="P14" s="82"/>
+      <c r="O14" s="84"/>
+      <c r="P14" s="84"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
@@ -4458,18 +4469,18 @@
       <c r="P18" s="54"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="79" t="s">
+      <c r="A19" s="81" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="80"/>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="80"/>
-      <c r="G19" s="80"/>
-      <c r="H19" s="80"/>
-      <c r="I19" s="80"/>
-      <c r="J19" s="80"/>
+      <c r="B19" s="82"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="82"/>
+      <c r="H19" s="82"/>
+      <c r="I19" s="82"/>
+      <c r="J19" s="82"/>
       <c r="K19" s="51"/>
       <c r="L19" s="30"/>
       <c r="N19" s="29" t="s">
@@ -4630,7 +4641,7 @@
       <c r="I23" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="J23" s="89" t="s">
+      <c r="J23" s="74" t="s">
         <v>146</v>
       </c>
       <c r="K23" s="60" t="s">

</xml_diff>

<commit_message>
[Douglas Giordano] - Atualizado planilha de responsabilidades e refatorado recibo de devolução de documentação.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -855,7 +855,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1059,10 +1059,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1074,7 +1071,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1105,6 +1105,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1431,18 +1434,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="H1" s="76" t="s">
+      <c r="A1" s="79" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="H1" s="80" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="76"/>
+      <c r="I1" s="80"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1572,21 +1575,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="77" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="78">
-        <v>4</v>
-      </c>
-      <c r="D7" s="78">
-        <v>1</v>
-      </c>
-      <c r="E7" s="78"/>
-      <c r="F7" s="79"/>
-      <c r="H7" s="76" t="s">
+      <c r="B7" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="77">
+        <v>4</v>
+      </c>
+      <c r="D7" s="77">
+        <v>1</v>
+      </c>
+      <c r="E7" s="77"/>
+      <c r="F7" s="78"/>
+      <c r="H7" s="80" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="76"/>
+      <c r="I7" s="80"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1745,8 +1748,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="80"/>
-      <c r="K13" s="80"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1794,13 +1797,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="77" t="s">
+      <c r="B16" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="79"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="78"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2012,13 +2015,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="77" t="s">
+      <c r="B27" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="78"/>
-      <c r="F27" s="79"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="78"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -2082,13 +2085,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="77" t="s">
+      <c r="B31" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="78"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="79"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="78"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2334,13 +2337,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="77" t="s">
+      <c r="B47" s="76" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="78"/>
-      <c r="D47" s="78"/>
-      <c r="E47" s="78"/>
-      <c r="F47" s="79"/>
+      <c r="C47" s="77"/>
+      <c r="D47" s="77"/>
+      <c r="E47" s="77"/>
+      <c r="F47" s="78"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2458,13 +2461,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="77" t="s">
+      <c r="B55" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="78"/>
-      <c r="D55" s="78"/>
-      <c r="E55" s="78"/>
-      <c r="F55" s="79"/>
+      <c r="C55" s="77"/>
+      <c r="D55" s="77"/>
+      <c r="E55" s="77"/>
+      <c r="F55" s="78"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2532,16 +2535,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B7:F7"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B55:F55"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2749,17 +2752,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="77" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="78">
-        <v>4</v>
-      </c>
-      <c r="D7" s="78">
-        <v>1</v>
-      </c>
-      <c r="E7" s="78"/>
-      <c r="F7" s="79"/>
+      <c r="B7" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="77">
+        <v>4</v>
+      </c>
+      <c r="D7" s="77">
+        <v>1</v>
+      </c>
+      <c r="E7" s="77"/>
+      <c r="F7" s="78"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -3711,21 +3714,21 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="77" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="78">
-        <v>4</v>
-      </c>
-      <c r="D22" s="78">
-        <v>1</v>
-      </c>
-      <c r="E22" s="78"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="79"/>
-      <c r="I22" s="77"/>
-      <c r="J22" s="78"/>
+      <c r="B22" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="77">
+        <v>4</v>
+      </c>
+      <c r="D22" s="77">
+        <v>1</v>
+      </c>
+      <c r="E22" s="77"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="77"/>
+      <c r="H22" s="78"/>
+      <c r="I22" s="76"/>
+      <c r="J22" s="77"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -3912,8 +3915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4068,7 +4071,7 @@
         <v>7</v>
       </c>
       <c r="P4" s="54">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -4174,10 +4177,10 @@
         <v>117</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="H7" s="66" t="s">
         <v>127</v>
@@ -4191,7 +4194,9 @@
       <c r="K7" s="27">
         <v>3</v>
       </c>
-      <c r="L7" s="47"/>
+      <c r="L7" s="91">
+        <v>3</v>
+      </c>
       <c r="N7" s="54" t="s">
         <v>122</v>
       </c>
@@ -4351,7 +4356,7 @@
       </c>
       <c r="P11" s="28">
         <f>SUM(P3:P10)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Alex Becker] - Atualização planilha de horas trabalhadas.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -1062,10 +1062,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1077,7 +1074,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1434,18 +1434,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="H1" s="77" t="s">
+      <c r="A1" s="80" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="H1" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="77"/>
+      <c r="I1" s="81"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1575,21 +1575,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="79">
-        <v>4</v>
-      </c>
-      <c r="D7" s="79">
-        <v>1</v>
-      </c>
-      <c r="E7" s="79"/>
-      <c r="F7" s="80"/>
-      <c r="H7" s="77" t="s">
+      <c r="B7" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="78">
+        <v>4</v>
+      </c>
+      <c r="D7" s="78">
+        <v>1</v>
+      </c>
+      <c r="E7" s="78"/>
+      <c r="F7" s="79"/>
+      <c r="H7" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="77"/>
+      <c r="I7" s="81"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1748,8 +1748,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="76"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1797,13 +1797,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="78" t="s">
+      <c r="B16" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="79"/>
-      <c r="D16" s="79"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="80"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="79"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2015,13 +2015,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="78" t="s">
+      <c r="B27" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="80"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="79"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -2085,13 +2085,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="78" t="s">
+      <c r="B31" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="79"/>
-      <c r="D31" s="79"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="80"/>
+      <c r="C31" s="78"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="78"/>
+      <c r="F31" s="79"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2337,13 +2337,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="78" t="s">
+      <c r="B47" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="79"/>
-      <c r="D47" s="79"/>
-      <c r="E47" s="79"/>
-      <c r="F47" s="80"/>
+      <c r="C47" s="78"/>
+      <c r="D47" s="78"/>
+      <c r="E47" s="78"/>
+      <c r="F47" s="79"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2461,13 +2461,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="78" t="s">
+      <c r="B55" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="79"/>
-      <c r="D55" s="79"/>
-      <c r="E55" s="79"/>
-      <c r="F55" s="80"/>
+      <c r="C55" s="78"/>
+      <c r="D55" s="78"/>
+      <c r="E55" s="78"/>
+      <c r="F55" s="79"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2535,16 +2535,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B7:F7"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B55:F55"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2752,17 +2752,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="79">
-        <v>4</v>
-      </c>
-      <c r="D7" s="79">
-        <v>1</v>
-      </c>
-      <c r="E7" s="79"/>
-      <c r="F7" s="80"/>
+      <c r="B7" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="78">
+        <v>4</v>
+      </c>
+      <c r="D7" s="78">
+        <v>1</v>
+      </c>
+      <c r="E7" s="78"/>
+      <c r="F7" s="79"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -3074,7 +3074,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3714,21 +3714,21 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="79">
-        <v>4</v>
-      </c>
-      <c r="D22" s="79">
-        <v>1</v>
-      </c>
-      <c r="E22" s="79"/>
-      <c r="F22" s="79"/>
-      <c r="G22" s="79"/>
-      <c r="H22" s="80"/>
-      <c r="I22" s="78"/>
-      <c r="J22" s="79"/>
+      <c r="B22" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="78">
+        <v>4</v>
+      </c>
+      <c r="D22" s="78">
+        <v>1</v>
+      </c>
+      <c r="E22" s="78"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="77"/>
+      <c r="J22" s="78"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -3915,8 +3915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4027,7 +4027,9 @@
       <c r="O3" s="54">
         <v>6</v>
       </c>
-      <c r="P3" s="54"/>
+      <c r="P3" s="54">
+        <v>6.5</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
@@ -4045,11 +4047,11 @@
       <c r="E4" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="F4" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="G4" s="65" t="s">
-        <v>127</v>
+      <c r="F4" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>151</v>
       </c>
       <c r="H4" s="66" t="s">
         <v>127</v>
@@ -4063,7 +4065,9 @@
       <c r="K4" s="54">
         <v>3</v>
       </c>
-      <c r="L4" s="7"/>
+      <c r="L4" s="46">
+        <v>0.14583333333333334</v>
+      </c>
       <c r="N4" s="54" t="s">
         <v>117</v>
       </c>
@@ -4090,11 +4094,11 @@
       <c r="E5" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="F5" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="G5" s="65" t="s">
-        <v>127</v>
+      <c r="F5" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>151</v>
       </c>
       <c r="H5" s="66" t="s">
         <v>127</v>
@@ -4108,7 +4112,9 @@
       <c r="K5" s="27">
         <v>3</v>
       </c>
-      <c r="L5" s="47"/>
+      <c r="L5" s="47">
+        <v>0.125</v>
+      </c>
       <c r="N5" s="54" t="s">
         <v>123</v>
       </c>
@@ -4356,7 +4362,7 @@
       </c>
       <c r="P11" s="28">
         <f>SUM(P3:P10)</f>
-        <v>9</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Gean Pereira] - Atualização de carga horária
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
@@ -12,7 +12,7 @@
     <sheet name="Incremento 2" sheetId="3" r:id="rId3"/>
     <sheet name="Incremento 3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -466,16 +466,16 @@
     <t>Status Programação</t>
   </si>
   <si>
-    <t xml:space="preserve"> 03:30</t>
-  </si>
-  <si>
     <t>Status Testes</t>
   </si>
   <si>
     <t>Finalizado</t>
   </si>
   <si>
-    <t xml:space="preserve"> 03:0:00</t>
+    <t xml:space="preserve"> 02:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 03:00</t>
   </si>
 </sst>
 </file>
@@ -855,7 +855,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1034,9 +1034,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1065,6 +1062,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1074,10 +1077,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1108,6 +1108,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1170,7 +1183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1205,7 +1218,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1434,18 +1447,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="H1" s="81" t="s">
+      <c r="A1" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="H1" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="81"/>
+      <c r="I1" s="77"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1575,21 +1588,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="77" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="78">
-        <v>4</v>
-      </c>
-      <c r="D7" s="78">
-        <v>1</v>
-      </c>
-      <c r="E7" s="78"/>
-      <c r="F7" s="79"/>
-      <c r="H7" s="81" t="s">
+      <c r="B7" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="79">
+        <v>4</v>
+      </c>
+      <c r="D7" s="79">
+        <v>1</v>
+      </c>
+      <c r="E7" s="79"/>
+      <c r="F7" s="80"/>
+      <c r="H7" s="77" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="81"/>
+      <c r="I7" s="77"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1748,8 +1761,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="76"/>
-      <c r="K13" s="76"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1797,13 +1810,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="77" t="s">
+      <c r="B16" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="79"/>
+      <c r="C16" s="79"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="79"/>
+      <c r="F16" s="80"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2015,13 +2028,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="77" t="s">
+      <c r="B27" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="78"/>
-      <c r="F27" s="79"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="80"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -2085,13 +2098,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="77" t="s">
+      <c r="B31" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="78"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="79"/>
+      <c r="C31" s="79"/>
+      <c r="D31" s="79"/>
+      <c r="E31" s="79"/>
+      <c r="F31" s="80"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2337,13 +2350,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="77" t="s">
+      <c r="B47" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="78"/>
-      <c r="D47" s="78"/>
-      <c r="E47" s="78"/>
-      <c r="F47" s="79"/>
+      <c r="C47" s="79"/>
+      <c r="D47" s="79"/>
+      <c r="E47" s="79"/>
+      <c r="F47" s="80"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2461,13 +2474,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="77" t="s">
+      <c r="B55" s="78" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="78"/>
-      <c r="D55" s="78"/>
-      <c r="E55" s="78"/>
-      <c r="F55" s="79"/>
+      <c r="C55" s="79"/>
+      <c r="D55" s="79"/>
+      <c r="E55" s="79"/>
+      <c r="F55" s="80"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2535,16 +2548,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B55:F55"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B7:F7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B55:F55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2752,17 +2765,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="77" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="78">
-        <v>4</v>
-      </c>
-      <c r="D7" s="78">
-        <v>1</v>
-      </c>
-      <c r="E7" s="78"/>
-      <c r="F7" s="79"/>
+      <c r="B7" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="79">
+        <v>4</v>
+      </c>
+      <c r="D7" s="79">
+        <v>1</v>
+      </c>
+      <c r="E7" s="79"/>
+      <c r="F7" s="80"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -3714,21 +3727,21 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="77" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="78">
-        <v>4</v>
-      </c>
-      <c r="D22" s="78">
-        <v>1</v>
-      </c>
-      <c r="E22" s="78"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="79"/>
-      <c r="I22" s="77"/>
-      <c r="J22" s="78"/>
+      <c r="B22" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="79">
+        <v>4</v>
+      </c>
+      <c r="D22" s="79">
+        <v>1</v>
+      </c>
+      <c r="E22" s="79"/>
+      <c r="F22" s="79"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="78"/>
+      <c r="J22" s="79"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -3916,7 +3929,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3980,7 +3993,7 @@
         <v>148</v>
       </c>
       <c r="H2" s="52" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I2" s="52" t="s">
         <v>142</v>
@@ -4048,12 +4061,12 @@
         <v>118</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="H4" s="66" t="s">
+        <v>150</v>
+      </c>
+      <c r="H4" s="65" t="s">
         <v>127</v>
       </c>
       <c r="I4" s="54" t="s">
@@ -4095,12 +4108,12 @@
         <v>118</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="H5" s="66" t="s">
+        <v>150</v>
+      </c>
+      <c r="H5" s="65" t="s">
         <v>127</v>
       </c>
       <c r="I5" s="54" t="s">
@@ -4121,7 +4134,9 @@
       <c r="O5" s="54">
         <v>6</v>
       </c>
-      <c r="P5" s="54"/>
+      <c r="P5" s="54">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
@@ -4140,12 +4155,12 @@
         <v>117</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="H6" s="66" t="s">
+        <v>150</v>
+      </c>
+      <c r="H6" s="65" t="s">
         <v>127</v>
       </c>
       <c r="I6" s="64" t="s">
@@ -4157,7 +4172,7 @@
       <c r="K6" s="64">
         <v>4</v>
       </c>
-      <c r="L6" s="73">
+      <c r="L6" s="72">
         <v>3</v>
       </c>
       <c r="N6" s="54" t="s">
@@ -4183,12 +4198,12 @@
         <v>117</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="H7" s="66" t="s">
+        <v>150</v>
+      </c>
+      <c r="H7" s="65" t="s">
         <v>127</v>
       </c>
       <c r="I7" s="64" t="s">
@@ -4200,7 +4215,7 @@
       <c r="K7" s="27">
         <v>3</v>
       </c>
-      <c r="L7" s="75">
+      <c r="L7" s="74">
         <v>3</v>
       </c>
       <c r="N7" s="54" t="s">
@@ -4231,7 +4246,7 @@
       <c r="G8" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="H8" s="66" t="s">
+      <c r="H8" s="65" t="s">
         <v>127</v>
       </c>
       <c r="I8" s="27" t="s">
@@ -4243,14 +4258,18 @@
       <c r="K8" s="27">
         <v>3</v>
       </c>
-      <c r="L8" s="75">
+      <c r="L8" s="74">
         <v>1</v>
       </c>
       <c r="N8" s="54" t="s">
         <v>124</v>
       </c>
-      <c r="O8" s="54"/>
-      <c r="P8" s="54"/>
+      <c r="O8" s="54">
+        <v>8</v>
+      </c>
+      <c r="P8" s="96">
+        <v>6.25E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
@@ -4268,13 +4287,13 @@
       <c r="E9" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="F9" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="G9" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="H9" s="66" t="s">
+      <c r="F9" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="H9" s="65" t="s">
         <v>127</v>
       </c>
       <c r="I9" s="27" t="s">
@@ -4286,14 +4305,14 @@
       <c r="K9" s="27">
         <v>2</v>
       </c>
-      <c r="L9" s="75">
+      <c r="L9" s="74">
         <v>1</v>
       </c>
       <c r="N9" s="54" t="s">
         <v>147</v>
       </c>
       <c r="O9" s="54">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P9" s="54">
         <v>3</v>
@@ -4315,25 +4334,27 @@
       <c r="E10" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="F10" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="H10" s="66" t="s">
+      <c r="F10" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="H10" s="65" t="s">
         <v>127</v>
       </c>
       <c r="I10" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="J10" s="65" t="s">
-        <v>146</v>
+      <c r="J10" s="27" t="s">
+        <v>126</v>
       </c>
       <c r="K10" s="27">
         <v>3</v>
       </c>
-      <c r="L10" s="46"/>
+      <c r="L10" s="47">
+        <v>0.125</v>
+      </c>
       <c r="N10" s="54" t="s">
         <v>120</v>
       </c>
@@ -4358,11 +4379,11 @@
       </c>
       <c r="O11" s="28">
         <f>SUM(O3:O10)</f>
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="P11" s="28">
         <f>SUM(P3:P10)</f>
-        <v>15.5</v>
+        <v>23.5625</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -4525,7 +4546,7 @@
         <v>148</v>
       </c>
       <c r="H20" s="52" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I20" s="52" t="s">
         <v>142</v>
@@ -4565,25 +4586,25 @@
         <v>123</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>126</v>
+        <v>150</v>
+      </c>
+      <c r="H21" s="75" t="s">
+        <v>127</v>
+      </c>
+      <c r="I21" s="75" t="s">
+        <v>127</v>
       </c>
       <c r="J21" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="K21" s="67">
+      <c r="K21" s="66">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="L21" s="46">
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -4603,16 +4624,16 @@
         <v>123</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>126</v>
+        <v>150</v>
+      </c>
+      <c r="H22" s="75" t="s">
+        <v>127</v>
+      </c>
+      <c r="I22" s="75" t="s">
+        <v>127</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>126</v>
@@ -4625,78 +4646,78 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="57" t="s">
+      <c r="A23" s="92" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="59">
-        <v>4</v>
-      </c>
-      <c r="D23" s="59">
-        <v>1</v>
-      </c>
-      <c r="E23" s="59" t="s">
+      <c r="C23" s="94">
+        <v>4</v>
+      </c>
+      <c r="D23" s="94">
+        <v>1</v>
+      </c>
+      <c r="E23" s="94" t="s">
         <v>119</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="H23" s="56" t="s">
+      <c r="H23" s="73" t="s">
         <v>127</v>
       </c>
-      <c r="I23" s="56" t="s">
+      <c r="I23" s="73" t="s">
         <v>127</v>
       </c>
-      <c r="J23" s="74" t="s">
+      <c r="J23" s="73" t="s">
         <v>146</v>
       </c>
-      <c r="K23" s="60" t="s">
-        <v>149</v>
-      </c>
-      <c r="L23" s="60" t="s">
+      <c r="K23" s="95" t="s">
+        <v>151</v>
+      </c>
+      <c r="L23" s="95" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="68" t="s">
+      <c r="A24" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="69" t="s">
+      <c r="B24" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="70">
-        <v>4</v>
-      </c>
-      <c r="D24" s="70">
-        <v>1</v>
-      </c>
-      <c r="E24" s="70" t="s">
+      <c r="C24" s="69">
+        <v>4</v>
+      </c>
+      <c r="D24" s="69">
+        <v>1</v>
+      </c>
+      <c r="E24" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="F24" s="71" t="s">
+      <c r="F24" s="70" t="s">
         <v>127</v>
       </c>
-      <c r="G24" s="71" t="s">
+      <c r="G24" s="70" t="s">
         <v>127</v>
       </c>
-      <c r="H24" s="71" t="s">
+      <c r="H24" s="70" t="s">
         <v>127</v>
       </c>
-      <c r="I24" s="71" t="s">
+      <c r="I24" s="70" t="s">
         <v>127</v>
       </c>
-      <c r="J24" s="71" t="s">
+      <c r="J24" s="70" t="s">
         <v>127</v>
       </c>
-      <c r="K24" s="72">
+      <c r="K24" s="71">
         <v>0.16666666666666666</v>
       </c>
-      <c r="L24" s="72">
+      <c r="L24" s="71">
         <v>0.125</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Douglas Giordano] - Atualização responsabilidades.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requisitos" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="Incremento 2" sheetId="3" r:id="rId3"/>
     <sheet name="Incremento 3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="152">
   <si>
     <t>ID</t>
   </si>
@@ -472,10 +472,7 @@
     <t>Finalizado</t>
   </si>
   <si>
-    <t xml:space="preserve"> 02:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 03:00</t>
+    <t>Parcialmente Finalizado</t>
   </si>
 </sst>
 </file>
@@ -855,7 +852,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1047,25 +1044,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1077,7 +1075,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1110,17 +1111,37 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1183,7 +1204,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1218,7 +1239,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1430,7 +1451,7 @@
   <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+      <selection activeCell="A43" sqref="A43:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,18 +1468,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="H1" s="77" t="s">
+      <c r="A1" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="H1" s="83" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="77"/>
+      <c r="I1" s="83"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1588,21 +1609,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="79">
-        <v>4</v>
-      </c>
-      <c r="D7" s="79">
-        <v>1</v>
-      </c>
-      <c r="E7" s="79"/>
-      <c r="F7" s="80"/>
-      <c r="H7" s="77" t="s">
+      <c r="B7" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="80">
+        <v>4</v>
+      </c>
+      <c r="D7" s="80">
+        <v>1</v>
+      </c>
+      <c r="E7" s="80"/>
+      <c r="F7" s="81"/>
+      <c r="H7" s="83" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="77"/>
+      <c r="I7" s="83"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1761,8 +1782,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="78"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1810,13 +1831,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="78" t="s">
+      <c r="B16" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="79"/>
-      <c r="D16" s="79"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="80"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="81"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2028,13 +2049,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="78" t="s">
+      <c r="B27" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="80"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="81"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -2098,13 +2119,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="78" t="s">
+      <c r="B31" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="79"/>
-      <c r="D31" s="79"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="80"/>
+      <c r="C31" s="80"/>
+      <c r="D31" s="80"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="81"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2350,13 +2371,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="78" t="s">
+      <c r="B47" s="79" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="79"/>
-      <c r="D47" s="79"/>
-      <c r="E47" s="79"/>
-      <c r="F47" s="80"/>
+      <c r="C47" s="80"/>
+      <c r="D47" s="80"/>
+      <c r="E47" s="80"/>
+      <c r="F47" s="81"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2474,13 +2495,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="78" t="s">
+      <c r="B55" s="79" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="79"/>
-      <c r="D55" s="79"/>
-      <c r="E55" s="79"/>
-      <c r="F55" s="80"/>
+      <c r="C55" s="80"/>
+      <c r="D55" s="80"/>
+      <c r="E55" s="80"/>
+      <c r="F55" s="81"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2548,16 +2569,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B7:F7"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B55:F55"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2586,20 +2607,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
+      <c r="A1" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
       <c r="G1" s="30"/>
-      <c r="I1" s="84" t="s">
+      <c r="I1" s="86" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -2765,17 +2786,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="79">
-        <v>4</v>
-      </c>
-      <c r="D7" s="79">
-        <v>1</v>
-      </c>
-      <c r="E7" s="79"/>
-      <c r="F7" s="80"/>
+      <c r="B7" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="80">
+        <v>4</v>
+      </c>
+      <c r="D7" s="80">
+        <v>1</v>
+      </c>
+      <c r="E7" s="80"/>
+      <c r="F7" s="81"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -2986,11 +3007,11 @@
       <c r="G14" s="35">
         <v>0</v>
       </c>
-      <c r="I14" s="84" t="s">
+      <c r="I14" s="86" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="85"/>
-      <c r="K14" s="85"/>
+      <c r="J14" s="87"/>
+      <c r="K14" s="87"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="41" t="s">
@@ -3086,8 +3107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3106,23 +3127,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="87"/>
+      <c r="A1" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="89"/>
       <c r="I1" s="50"/>
       <c r="J1" s="30"/>
-      <c r="L1" s="84" t="s">
+      <c r="L1" s="86" t="s">
         <v>133</v>
       </c>
-      <c r="M1" s="85"/>
-      <c r="N1" s="85"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -3169,17 +3190,17 @@
       <c r="A3" s="39">
         <v>4</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="91"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="93"/>
       <c r="L3" s="25" t="s">
         <v>118</v>
       </c>
@@ -3535,22 +3556,22 @@
       <c r="A14" s="9">
         <v>5</v>
       </c>
-      <c r="B14" s="88" t="s">
+      <c r="B14" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="88"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="88"/>
-      <c r="H14" s="88"/>
-      <c r="I14" s="88"/>
-      <c r="J14" s="88"/>
-      <c r="L14" s="84" t="s">
+      <c r="C14" s="90"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="90"/>
+      <c r="L14" s="86" t="s">
         <v>102</v>
       </c>
-      <c r="M14" s="85"/>
-      <c r="N14" s="85"/>
+      <c r="M14" s="87"/>
+      <c r="N14" s="87"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
@@ -3639,16 +3660,16 @@
       <c r="N18" s="25"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="82" t="s">
+      <c r="A19" s="84" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="83"/>
-      <c r="C19" s="83"/>
-      <c r="D19" s="83"/>
-      <c r="E19" s="83"/>
-      <c r="F19" s="83"/>
-      <c r="G19" s="83"/>
-      <c r="H19" s="83"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="85"/>
+      <c r="H19" s="85"/>
       <c r="I19" s="51"/>
       <c r="J19" s="30"/>
       <c r="L19" s="29" t="s">
@@ -3727,21 +3748,21 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="79">
-        <v>4</v>
-      </c>
-      <c r="D22" s="79">
-        <v>1</v>
-      </c>
-      <c r="E22" s="79"/>
-      <c r="F22" s="79"/>
-      <c r="G22" s="79"/>
-      <c r="H22" s="80"/>
-      <c r="I22" s="78"/>
-      <c r="J22" s="79"/>
+      <c r="B22" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="80">
+        <v>4</v>
+      </c>
+      <c r="D22" s="80">
+        <v>1</v>
+      </c>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="81"/>
+      <c r="I22" s="79"/>
+      <c r="J22" s="80"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -3818,7 +3839,7 @@
       <c r="F25" s="27"/>
       <c r="G25" s="27"/>
       <c r="H25" s="27" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I25" s="27"/>
       <c r="J25" s="35"/>
@@ -3908,7 +3929,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="HkpizirgCBmsJxAfyUjPKSTIOPqPhtoe6Lx2nL9JGyc5aA/m7tusagY1QRkNkTuqssViaYUKt5eAw8C5nwkYpg==" saltValue="Y9y8ekWlbOPqhkC8OsbfyA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="zOB+cD/a0EhZ8Ac8MOK/wV+Y1XnK0oCZO/P5y0fD5RfEHRxUdMSwvTzgVjHiGxrnkqw3hChTMc6Z21XsXx4BNA==" saltValue="t+zqGU7MKZt4hFB+H9h9dA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="8">
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="L14:N14"/>
@@ -3926,10 +3947,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3950,25 +3971,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="87"/>
+      <c r="A1" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="89"/>
       <c r="K1" s="50"/>
       <c r="L1" s="30"/>
-      <c r="N1" s="84" t="s">
+      <c r="N1" s="86" t="s">
         <v>133</v>
       </c>
-      <c r="O1" s="85"/>
-      <c r="P1" s="85"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -4021,19 +4042,19 @@
       <c r="A3" s="55">
         <v>6</v>
       </c>
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
       <c r="N3" s="54" t="s">
         <v>118</v>
       </c>
@@ -4061,7 +4082,7 @@
         <v>118</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>150</v>
@@ -4078,8 +4099,8 @@
       <c r="K4" s="54">
         <v>3</v>
       </c>
-      <c r="L4" s="46">
-        <v>0.14583333333333334</v>
+      <c r="L4" s="94">
+        <v>3.3</v>
       </c>
       <c r="N4" s="54" t="s">
         <v>117</v>
@@ -4108,7 +4129,7 @@
         <v>118</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>150</v>
@@ -4125,8 +4146,8 @@
       <c r="K5" s="27">
         <v>3</v>
       </c>
-      <c r="L5" s="47">
-        <v>0.125</v>
+      <c r="L5" s="72">
+        <v>3</v>
       </c>
       <c r="N5" s="54" t="s">
         <v>123</v>
@@ -4135,7 +4156,7 @@
         <v>6</v>
       </c>
       <c r="P5" s="54">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -4149,13 +4170,13 @@
         <v>4</v>
       </c>
       <c r="D6" s="27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>117</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>150</v>
@@ -4167,19 +4188,23 @@
         <v>127</v>
       </c>
       <c r="J6" s="64" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="K6" s="64">
         <v>4</v>
       </c>
-      <c r="L6" s="72">
+      <c r="L6" s="95">
         <v>3</v>
       </c>
       <c r="N6" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="O6" s="54"/>
-      <c r="P6" s="54"/>
+      <c r="O6" s="54">
+        <v>7</v>
+      </c>
+      <c r="P6" s="54">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
@@ -4192,13 +4217,13 @@
         <v>4</v>
       </c>
       <c r="D7" s="27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="27" t="s">
         <v>117</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>150</v>
@@ -4209,13 +4234,13 @@
       <c r="I7" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="J7" s="27" t="s">
-        <v>127</v>
+      <c r="J7" s="74" t="s">
+        <v>126</v>
       </c>
       <c r="K7" s="27">
         <v>3</v>
       </c>
-      <c r="L7" s="74">
+      <c r="L7" s="72">
         <v>3</v>
       </c>
       <c r="N7" s="54" t="s">
@@ -4240,7 +4265,7 @@
       <c r="E8" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="7" t="s">
         <v>127</v>
       </c>
       <c r="G8" s="27" t="s">
@@ -4258,7 +4283,7 @@
       <c r="K8" s="27">
         <v>3</v>
       </c>
-      <c r="L8" s="74">
+      <c r="L8" s="72">
         <v>1</v>
       </c>
       <c r="N8" s="54" t="s">
@@ -4267,8 +4292,8 @@
       <c r="O8" s="54">
         <v>8</v>
       </c>
-      <c r="P8" s="96">
-        <v>6.25E-2</v>
+      <c r="P8" s="95">
+        <v>1.3</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -4282,13 +4307,13 @@
         <v>4</v>
       </c>
       <c r="D9" s="27">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E9" s="27" t="s">
         <v>147</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>126</v>
@@ -4305,7 +4330,7 @@
       <c r="K9" s="27">
         <v>2</v>
       </c>
-      <c r="L9" s="74">
+      <c r="L9" s="72">
         <v>1</v>
       </c>
       <c r="N9" s="54" t="s">
@@ -4319,26 +4344,26 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
-        <v>27</v>
+      <c r="A10" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="C10" s="27">
         <v>4</v>
       </c>
       <c r="D10" s="27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="H10" s="65" t="s">
         <v>127</v>
@@ -4349,17 +4374,21 @@
       <c r="J10" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="K10" s="27">
-        <v>3</v>
-      </c>
-      <c r="L10" s="47">
-        <v>0.125</v>
+      <c r="K10" s="14">
+        <v>2</v>
+      </c>
+      <c r="L10" s="104">
+        <v>2</v>
       </c>
       <c r="N10" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="O10" s="54"/>
-      <c r="P10" s="53"/>
+      <c r="O10" s="54">
+        <v>6</v>
+      </c>
+      <c r="P10" s="95">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="33"/>
@@ -4372,18 +4401,18 @@
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
       <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
+      <c r="K11" s="66"/>
       <c r="L11" s="46"/>
       <c r="N11" s="28" t="s">
         <v>135</v>
       </c>
       <c r="O11" s="28">
         <f>SUM(O3:O10)</f>
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P11" s="28">
         <f>SUM(P3:P10)</f>
-        <v>23.5625</v>
+        <v>38.799999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -4397,8 +4426,14 @@
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="46"/>
+      <c r="K12" s="27">
+        <f>SUM(K4:K10)</f>
+        <v>20</v>
+      </c>
+      <c r="L12" s="72">
+        <f>SUM(L4:L10)</f>
+        <v>16.3</v>
+      </c>
       <c r="N12" s="63" t="s">
         <v>143</v>
       </c>
@@ -4422,11 +4457,11 @@
       <c r="O13" s="54"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N14" s="84" t="s">
+      <c r="N14" s="86" t="s">
         <v>102</v>
       </c>
-      <c r="O14" s="85"/>
-      <c r="P14" s="85"/>
+      <c r="O14" s="87"/>
+      <c r="P14" s="87"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
@@ -4501,18 +4536,18 @@
       <c r="P18" s="54"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="82" t="s">
+      <c r="A19" s="84" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="83"/>
-      <c r="C19" s="83"/>
-      <c r="D19" s="83"/>
-      <c r="E19" s="83"/>
-      <c r="F19" s="83"/>
-      <c r="G19" s="83"/>
-      <c r="H19" s="83"/>
-      <c r="I19" s="83"/>
-      <c r="J19" s="83"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="85"/>
+      <c r="H19" s="85"/>
+      <c r="I19" s="85"/>
+      <c r="J19" s="85"/>
       <c r="K19" s="51"/>
       <c r="L19" s="30"/>
       <c r="N19" s="29" t="s">
@@ -4586,25 +4621,25 @@
         <v>123</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="H21" s="75" t="s">
-        <v>127</v>
-      </c>
-      <c r="I21" s="75" t="s">
+      <c r="H21" s="73" t="s">
+        <v>127</v>
+      </c>
+      <c r="I21" s="73" t="s">
         <v>127</v>
       </c>
       <c r="J21" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="K21" s="66">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="L21" s="46">
-        <v>0.125</v>
+      <c r="K21" s="98">
+        <v>3</v>
+      </c>
+      <c r="L21" s="94">
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -4624,63 +4659,63 @@
         <v>123</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="H22" s="75" t="s">
-        <v>127</v>
-      </c>
-      <c r="I22" s="75" t="s">
+      <c r="H22" s="73" t="s">
+        <v>127</v>
+      </c>
+      <c r="I22" s="73" t="s">
         <v>127</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="K22" s="35">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="L22" s="35">
-        <v>8.3333333333333329E-2</v>
+      <c r="K22" s="99">
+        <v>3</v>
+      </c>
+      <c r="L22" s="99">
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="92" t="s">
+      <c r="A23" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="93" t="s">
+      <c r="B23" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="94">
-        <v>4</v>
-      </c>
-      <c r="D23" s="94">
-        <v>1</v>
-      </c>
-      <c r="E23" s="94" t="s">
+      <c r="C23" s="77">
+        <v>4</v>
+      </c>
+      <c r="D23" s="77">
+        <v>1</v>
+      </c>
+      <c r="E23" s="77" t="s">
         <v>119</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="H23" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="I23" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="J23" s="73" t="s">
+        <v>127</v>
+      </c>
+      <c r="H23" s="71" t="s">
+        <v>127</v>
+      </c>
+      <c r="I23" s="71" t="s">
+        <v>127</v>
+      </c>
+      <c r="J23" s="71" t="s">
         <v>146</v>
       </c>
-      <c r="K23" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="L23" s="95" t="s">
-        <v>152</v>
+      <c r="K23" s="100">
+        <v>2</v>
+      </c>
+      <c r="L23" s="100">
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4714,54 +4749,145 @@
       <c r="J24" s="70" t="s">
         <v>127</v>
       </c>
-      <c r="K24" s="71">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="L24" s="71">
-        <v>0.125</v>
+      <c r="K24" s="101">
+        <v>4</v>
+      </c>
+      <c r="L24" s="101">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="57"/>
-      <c r="B25" s="58"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="56"/>
-      <c r="K25" s="59"/>
-      <c r="L25" s="60"/>
+      <c r="A25" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="27">
+        <v>4</v>
+      </c>
+      <c r="D25" s="27">
+        <v>2</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G25" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="H25" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="I25" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="J25" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="K25" s="102">
+        <v>4</v>
+      </c>
+      <c r="L25" s="103">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="35"/>
-    </row>
-    <row r="27" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="41"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="45"/>
+      <c r="A26" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="27">
+        <v>4</v>
+      </c>
+      <c r="D26" s="27">
+        <v>2</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G26" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="H26" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="I26" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="J26" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="K26" s="102">
+        <v>6</v>
+      </c>
+      <c r="L26" s="103">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="27">
+        <v>4</v>
+      </c>
+      <c r="D27" s="27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="H27" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="I27" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="J27" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="K27" s="98">
+        <v>2</v>
+      </c>
+      <c r="L27" s="99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="41"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="97">
+        <v>24</v>
+      </c>
+      <c r="L28" s="96">
+        <f>SUM(L21:L27)</f>
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
[Gean Pereira] - Atualização da planilha.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
@@ -12,12 +12,12 @@
     <sheet name="Incremento 2" sheetId="3" r:id="rId3"/>
     <sheet name="Incremento 3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="151">
   <si>
     <t>ID</t>
   </si>
@@ -443,9 +443,6 @@
   </si>
   <si>
     <t>Status Interface</t>
-  </si>
-  <si>
-    <t>Status Validação</t>
   </si>
   <si>
     <t>Total Planejadas</t>
@@ -1096,10 +1093,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1111,7 +1105,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1204,7 +1201,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1239,7 +1236,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1468,18 +1465,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="H1" s="90" t="s">
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="H1" s="94" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="90"/>
+      <c r="I1" s="94"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1609,21 +1606,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="91" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="92">
-        <v>4</v>
-      </c>
-      <c r="D7" s="92">
+      <c r="B7" s="90" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="91">
+        <v>4</v>
+      </c>
+      <c r="D7" s="91">
         <v>1</v>
       </c>
-      <c r="E7" s="92"/>
-      <c r="F7" s="93"/>
-      <c r="H7" s="90" t="s">
+      <c r="E7" s="91"/>
+      <c r="F7" s="92"/>
+      <c r="H7" s="94" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="90"/>
+      <c r="I7" s="94"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1782,8 +1779,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="94"/>
-      <c r="K13" s="94"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1831,13 +1828,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="91" t="s">
+      <c r="B16" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="92"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="92"/>
-      <c r="F16" s="93"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="91"/>
+      <c r="F16" s="92"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2049,13 +2046,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="91" t="s">
+      <c r="B27" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="92"/>
-      <c r="D27" s="92"/>
-      <c r="E27" s="92"/>
-      <c r="F27" s="93"/>
+      <c r="C27" s="91"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="91"/>
+      <c r="F27" s="92"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -2119,13 +2116,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="91" t="s">
+      <c r="B31" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="92"/>
-      <c r="D31" s="92"/>
-      <c r="E31" s="92"/>
-      <c r="F31" s="93"/>
+      <c r="C31" s="91"/>
+      <c r="D31" s="91"/>
+      <c r="E31" s="91"/>
+      <c r="F31" s="92"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2371,13 +2368,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="91" t="s">
+      <c r="B47" s="90" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="92"/>
-      <c r="D47" s="92"/>
-      <c r="E47" s="92"/>
-      <c r="F47" s="93"/>
+      <c r="C47" s="91"/>
+      <c r="D47" s="91"/>
+      <c r="E47" s="91"/>
+      <c r="F47" s="92"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2495,13 +2492,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="91" t="s">
+      <c r="B55" s="90" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="92"/>
-      <c r="D55" s="92"/>
-      <c r="E55" s="92"/>
-      <c r="F55" s="93"/>
+      <c r="C55" s="91"/>
+      <c r="D55" s="91"/>
+      <c r="E55" s="91"/>
+      <c r="F55" s="92"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2569,16 +2566,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B7:F7"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B55:F55"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2786,17 +2783,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="91" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="92">
-        <v>4</v>
-      </c>
-      <c r="D7" s="92">
+      <c r="B7" s="90" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="91">
+        <v>4</v>
+      </c>
+      <c r="D7" s="91">
         <v>1</v>
       </c>
-      <c r="E7" s="92"/>
-      <c r="F7" s="93"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="92"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -3105,10 +3102,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,16 +3114,17 @@
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="95" t="s">
         <v>1</v>
       </c>
@@ -3136,16 +3134,17 @@
       <c r="E1" s="96"/>
       <c r="F1" s="99"/>
       <c r="G1" s="99"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="30"/>
-      <c r="L1" s="97" t="s">
+      <c r="H1" s="99"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="30"/>
+      <c r="M1" s="97" t="s">
         <v>133</v>
       </c>
-      <c r="M1" s="98"/>
       <c r="N1" s="98"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="98"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
@@ -3165,28 +3164,31 @@
         <v>141</v>
       </c>
       <c r="G2" s="52" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H2" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="I2" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="J2" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="K2" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="M2" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="N2" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="N2" s="28" t="s">
+      <c r="O2" s="28" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="39">
         <v>4</v>
       </c>
@@ -3200,18 +3202,19 @@
       <c r="G3" s="103"/>
       <c r="H3" s="103"/>
       <c r="I3" s="103"/>
-      <c r="J3" s="104"/>
-      <c r="L3" s="25" t="s">
+      <c r="J3" s="103"/>
+      <c r="K3" s="104"/>
+      <c r="M3" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="M3" s="25">
+      <c r="N3" s="25">
         <v>8</v>
       </c>
-      <c r="N3" s="25">
+      <c r="O3" s="25">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
         <v>21</v>
       </c>
@@ -3227,28 +3230,35 @@
       <c r="E4" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
+      <c r="F4" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" s="59" t="s">
+        <v>127</v>
+      </c>
       <c r="H4" s="59" t="s">
         <v>127</v>
       </c>
-      <c r="I4" s="59">
+      <c r="I4" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="J4" s="59">
         <v>2</v>
       </c>
-      <c r="J4" s="61">
+      <c r="K4" s="61">
         <v>3.125E-2</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="M4" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="M4" s="25">
+      <c r="N4" s="25">
         <v>12</v>
       </c>
-      <c r="N4" s="25">
+      <c r="O4" s="25">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>22</v>
       </c>
@@ -3264,26 +3274,33 @@
       <c r="E5" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="I5" s="27">
+      <c r="F5" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H5" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="J5" s="27">
         <v>6</v>
       </c>
-      <c r="J5" s="46"/>
-      <c r="L5" s="25" t="s">
+      <c r="K5" s="46"/>
+      <c r="M5" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="M5" s="25">
+      <c r="N5" s="25">
         <v>8</v>
       </c>
-      <c r="N5" s="25">
+      <c r="O5" s="25">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>25</v>
       </c>
@@ -3299,28 +3316,35 @@
       <c r="E6" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27" t="s">
+      <c r="F6" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H6" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="I6" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="I6" s="27">
-        <v>4</v>
-      </c>
-      <c r="J6" s="47">
+      <c r="J6" s="27">
+        <v>4</v>
+      </c>
+      <c r="K6" s="47">
         <v>0.125</v>
       </c>
-      <c r="L6" s="25" t="s">
+      <c r="M6" s="25" t="s">
         <v>121</v>
-      </c>
-      <c r="M6" s="25">
-        <v>8</v>
       </c>
       <c r="N6" s="25">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>27</v>
       </c>
@@ -3340,18 +3364,19 @@
       <c r="G7" s="27"/>
       <c r="H7" s="27"/>
       <c r="I7" s="27"/>
-      <c r="J7" s="47"/>
-      <c r="L7" s="25" t="s">
+      <c r="J7" s="27"/>
+      <c r="K7" s="47"/>
+      <c r="M7" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="M7" s="25">
+      <c r="N7" s="25">
         <v>8</v>
       </c>
-      <c r="N7" s="25">
+      <c r="O7" s="25">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>29</v>
       </c>
@@ -3367,28 +3392,35 @@
       <c r="E8" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="I8" s="27">
+      <c r="F8" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H8" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="J8" s="27">
         <v>2</v>
       </c>
-      <c r="J8" s="46">
+      <c r="K8" s="46">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="L8" s="25" t="s">
+      <c r="M8" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="M8" s="25">
+      <c r="N8" s="25">
         <v>8</v>
       </c>
-      <c r="N8" s="25">
+      <c r="O8" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>31</v>
       </c>
@@ -3408,18 +3440,19 @@
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
       <c r="I9" s="27"/>
-      <c r="J9" s="46"/>
-      <c r="L9" s="25" t="s">
+      <c r="J9" s="27"/>
+      <c r="K9" s="46"/>
+      <c r="M9" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="M9" s="25">
+      <c r="N9" s="25">
         <v>6</v>
       </c>
-      <c r="N9" s="25">
+      <c r="O9" s="25">
         <v>3.15</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>33</v>
       </c>
@@ -3435,28 +3468,35 @@
       <c r="E10" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="I10" s="27">
-        <v>4</v>
-      </c>
-      <c r="J10" s="46">
+      <c r="F10" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H10" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="J10" s="27">
+        <v>4</v>
+      </c>
+      <c r="K10" s="46">
         <v>0.1875</v>
       </c>
-      <c r="L10" s="25" t="s">
+      <c r="M10" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="M10" s="25">
+      <c r="N10" s="25">
         <v>10</v>
       </c>
-      <c r="N10" s="53">
+      <c r="O10" s="53">
         <v>10.5</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>35</v>
       </c>
@@ -3472,30 +3512,37 @@
       <c r="E11" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="I11" s="27">
+      <c r="F11" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H11" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="J11" s="27">
         <v>5</v>
       </c>
-      <c r="J11" s="46">
+      <c r="K11" s="46">
         <v>0.14583333333333334</v>
       </c>
-      <c r="L11" s="28" t="s">
+      <c r="M11" s="28" t="s">
         <v>135</v>
-      </c>
-      <c r="M11" s="28">
-        <f>SUM(M3:M10)</f>
-        <v>68</v>
       </c>
       <c r="N11" s="28">
         <f>SUM(N3:N10)</f>
+        <v>68</v>
+      </c>
+      <c r="O11" s="28">
+        <f>SUM(O3:O10)</f>
         <v>50.65</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
         <v>37</v>
       </c>
@@ -3511,19 +3558,26 @@
       <c r="E12" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="I12" s="27">
-        <v>4</v>
-      </c>
-      <c r="J12" s="46">
+      <c r="F12" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H12" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="J12" s="27">
+        <v>4</v>
+      </c>
+      <c r="K12" s="46">
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>130</v>
       </c>
@@ -3539,20 +3593,27 @@
       <c r="E13" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="I13" s="27">
-        <v>4</v>
-      </c>
-      <c r="J13" s="46">
+      <c r="F13" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H13" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="J13" s="27">
+        <v>4</v>
+      </c>
+      <c r="K13" s="46">
         <v>0.20833333333333334</v>
       </c>
-      <c r="M13" s="25"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N13" s="25"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>5</v>
       </c>
@@ -3567,13 +3628,14 @@
       <c r="H14" s="101"/>
       <c r="I14" s="101"/>
       <c r="J14" s="101"/>
-      <c r="L14" s="97" t="s">
+      <c r="K14" s="101"/>
+      <c r="M14" s="97" t="s">
         <v>102</v>
       </c>
-      <c r="M14" s="98"/>
       <c r="N14" s="98"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="98"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
         <v>40</v>
       </c>
@@ -3591,24 +3653,25 @@
       </c>
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
-      <c r="H15" s="27" t="s">
+      <c r="H15" s="27"/>
+      <c r="I15" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="I15" s="27">
+      <c r="J15" s="27">
         <v>7</v>
       </c>
-      <c r="J15" s="46">
+      <c r="K15" s="46">
         <v>0.25</v>
       </c>
-      <c r="L15" s="25" t="s">
+      <c r="M15" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="M15" s="25" t="s">
+      <c r="N15" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="N15" s="25"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="25"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
       <c r="B16" s="3"/>
       <c r="C16" s="27"/>
@@ -3618,16 +3681,17 @@
       <c r="G16" s="27"/>
       <c r="H16" s="27"/>
       <c r="I16" s="27"/>
-      <c r="J16" s="48"/>
-      <c r="L16" s="25" t="s">
+      <c r="J16" s="27"/>
+      <c r="K16" s="48"/>
+      <c r="M16" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="M16" s="25">
+      <c r="N16" s="25">
         <v>1</v>
       </c>
-      <c r="N16" s="25"/>
-    </row>
-    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O16" s="25"/>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="41"/>
       <c r="B17" s="42"/>
       <c r="C17" s="43"/>
@@ -3635,31 +3699,32 @@
       <c r="E17" s="43"/>
       <c r="F17" s="27"/>
       <c r="G17" s="27"/>
-      <c r="H17" s="6"/>
+      <c r="H17" s="27"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="49"/>
-      <c r="L17" s="25" t="s">
+      <c r="J17" s="6"/>
+      <c r="K17" s="49"/>
+      <c r="M17" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="M17" s="25">
+      <c r="N17" s="25">
         <v>3</v>
       </c>
-      <c r="N17" s="25"/>
-    </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I18">
-        <f>SUM(I4:I13)+SUM(I15:I17)+SUM(I21)+SUM(I23:I28)</f>
+      <c r="O17" s="25"/>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J18">
+        <f>SUM(J4:J13)+SUM(J15:J17)+SUM(J21)+SUM(J23:J28)</f>
         <v>55</v>
       </c>
-      <c r="L18" s="25" t="s">
+      <c r="M18" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="M18" s="25">
+      <c r="N18" s="25">
         <v>3</v>
       </c>
-      <c r="N18" s="25"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" s="25"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="95" t="s">
         <v>137</v>
       </c>
@@ -3670,17 +3735,18 @@
       <c r="F19" s="96"/>
       <c r="G19" s="96"/>
       <c r="H19" s="96"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="30"/>
-      <c r="L19" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="M19" s="25">
+      <c r="I19" s="96"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="30"/>
+      <c r="M19" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="N19" s="25">
         <v>13</v>
       </c>
-      <c r="N19" s="25"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" s="25"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>0</v>
       </c>
@@ -3698,25 +3764,26 @@
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
-      <c r="H20" s="19" t="s">
+      <c r="H20" s="19"/>
+      <c r="I20" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="I20" s="19" t="s">
+      <c r="J20" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="J20" s="19" t="s">
+      <c r="K20" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="L20" s="28" t="s">
+      <c r="M20" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="M20" s="28">
-        <f>SUM(M16:M19)</f>
+      <c r="N20" s="28">
+        <f>SUM(N16:N19)</f>
         <v>20</v>
       </c>
-      <c r="N20" s="28"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" s="28"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="33">
         <v>0</v>
       </c>
@@ -3732,39 +3799,47 @@
       <c r="E21" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="7" t="s">
+      <c r="F21" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H21" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="I21" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="I21" s="27">
-        <v>4</v>
-      </c>
-      <c r="J21" s="46">
+      <c r="J21" s="27">
+        <v>4</v>
+      </c>
+      <c r="K21" s="46">
         <v>0.20833333333333334</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="91" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="92">
-        <v>4</v>
-      </c>
-      <c r="D22" s="92">
+      <c r="B22" s="90" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="91">
+        <v>4</v>
+      </c>
+      <c r="D22" s="91">
         <v>1</v>
       </c>
-      <c r="E22" s="92"/>
-      <c r="F22" s="92"/>
-      <c r="G22" s="92"/>
-      <c r="H22" s="93"/>
-      <c r="I22" s="91"/>
-      <c r="J22" s="92"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E22" s="91"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="91"/>
+      <c r="H22" s="91"/>
+      <c r="I22" s="92"/>
+      <c r="J22" s="90"/>
+      <c r="K22" s="91"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
         <v>7</v>
       </c>
@@ -3780,19 +3855,26 @@
       <c r="E23" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="7" t="s">
+      <c r="F23" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H23" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="I23" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="I23" s="27">
+      <c r="J23" s="27">
         <v>1</v>
       </c>
-      <c r="J23" s="35">
+      <c r="K23" s="35">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
         <v>9</v>
       </c>
@@ -3808,19 +3890,26 @@
       <c r="E24" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="7" t="s">
+      <c r="F24" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H24" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="I24" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="I24" s="27">
+      <c r="J24" s="27">
         <v>3</v>
       </c>
-      <c r="J24" s="35">
+      <c r="K24" s="35">
         <v>0.1875</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
         <v>11</v>
       </c>
@@ -3836,15 +3925,22 @@
       <c r="E25" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27" t="s">
+      <c r="F25" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H25" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="I25" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="I25" s="27"/>
-      <c r="J25" s="35"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J25" s="27"/>
+      <c r="K25" s="35"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="57" t="s">
         <v>13</v>
       </c>
@@ -3860,19 +3956,26 @@
       <c r="E26" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="F26" s="59"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="56" t="s">
-        <v>127</v>
-      </c>
-      <c r="I26" s="59">
+      <c r="F26" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="G26" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="H26" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="I26" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="J26" s="59">
         <v>3</v>
       </c>
-      <c r="J26" s="60" t="s">
+      <c r="K26" s="60" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
         <v>16</v>
       </c>
@@ -3888,19 +3991,26 @@
       <c r="E27" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="7" t="s">
+      <c r="F27" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H27" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="I27" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="I27" s="27">
+      <c r="J27" s="27">
         <v>2</v>
       </c>
-      <c r="J27" s="35">
+      <c r="K27" s="35">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="41" t="s">
         <v>18</v>
       </c>
@@ -3916,29 +4026,35 @@
       <c r="E28" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="44" t="s">
-        <v>127</v>
-      </c>
-      <c r="I28" s="43">
-        <v>4</v>
-      </c>
-      <c r="J28" s="45">
+      <c r="F28" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H28" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="I28" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="J28" s="43">
+        <v>4</v>
+      </c>
+      <c r="K28" s="45">
         <v>0.125</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="zOB+cD/a0EhZ8Ac8MOK/wV+Y1XnK0oCZO/P5y0fD5RfEHRxUdMSwvTzgVjHiGxrnkqw3hChTMc6Z21XsXx4BNA==" saltValue="t+zqGU7MKZt4hFB+H9h9dA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="8">
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B14:J14"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="A19:I19"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B14:K14"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="J22:K22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3947,10 +4063,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3961,16 +4077,15 @@
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" customWidth="1"/>
     <col min="7" max="8" width="26.42578125" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="95" t="s">
         <v>1</v>
       </c>
@@ -3981,17 +4096,16 @@
       <c r="F1" s="99"/>
       <c r="G1" s="99"/>
       <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="30"/>
-      <c r="N1" s="97" t="s">
+      <c r="I1" s="100"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="30"/>
+      <c r="M1" s="97" t="s">
         <v>133</v>
       </c>
+      <c r="N1" s="98"/>
       <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
@@ -4011,34 +4125,31 @@
         <v>141</v>
       </c>
       <c r="G2" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" s="52" t="s">
         <v>148</v>
       </c>
-      <c r="H2" s="52" t="s">
-        <v>149</v>
-      </c>
       <c r="I2" s="52" t="s">
-        <v>142</v>
-      </c>
-      <c r="J2" s="52" t="s">
         <v>103</v>
       </c>
+      <c r="J2" s="19" t="s">
+        <v>131</v>
+      </c>
       <c r="K2" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="L2" s="19" t="s">
         <v>132</v>
       </c>
+      <c r="M2" s="28" t="s">
+        <v>134</v>
+      </c>
       <c r="N2" s="28" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="O2" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="P2" s="28" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="55">
         <v>6</v>
       </c>
@@ -4054,23 +4165,22 @@
       <c r="I3" s="101"/>
       <c r="J3" s="101"/>
       <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
-      <c r="N3" s="54" t="s">
+      <c r="M3" s="54" t="s">
         <v>118</v>
       </c>
+      <c r="N3" s="54">
+        <v>6</v>
+      </c>
       <c r="O3" s="54">
-        <v>6</v>
-      </c>
-      <c r="P3" s="54">
         <v>6.5</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C4" s="54">
         <v>4</v>
@@ -4085,39 +4195,36 @@
         <v>127</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H4" s="65" t="s">
         <v>127</v>
       </c>
       <c r="I4" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="J4" s="54" t="s">
-        <v>146</v>
-      </c>
-      <c r="K4" s="54">
+        <v>145</v>
+      </c>
+      <c r="J4" s="54">
         <v>3</v>
       </c>
-      <c r="L4" s="78">
+      <c r="K4" s="78">
         <v>3.3</v>
       </c>
-      <c r="N4" s="54" t="s">
+      <c r="M4" s="54" t="s">
         <v>117</v>
       </c>
+      <c r="N4" s="54">
+        <v>7</v>
+      </c>
       <c r="O4" s="54">
-        <v>7</v>
-      </c>
-      <c r="P4" s="54">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C5" s="27">
         <v>4</v>
@@ -4132,34 +4239,31 @@
         <v>127</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H5" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="I5" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="J5" s="62" t="s">
-        <v>146</v>
-      </c>
-      <c r="K5" s="27">
+      <c r="I5" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="J5" s="27">
         <v>3</v>
       </c>
-      <c r="L5" s="72">
+      <c r="K5" s="72">
         <v>3</v>
       </c>
-      <c r="N5" s="54" t="s">
+      <c r="M5" s="54" t="s">
         <v>123</v>
+      </c>
+      <c r="N5" s="54">
+        <v>6</v>
       </c>
       <c r="O5" s="54">
         <v>6</v>
       </c>
-      <c r="P5" s="54">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>42</v>
       </c>
@@ -4179,34 +4283,31 @@
         <v>127</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H6" s="65" t="s">
         <v>127</v>
       </c>
       <c r="I6" s="64" t="s">
-        <v>127</v>
-      </c>
-      <c r="J6" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="K6" s="64">
-        <v>4</v>
-      </c>
-      <c r="L6" s="79">
+      <c r="J6" s="64">
+        <v>4</v>
+      </c>
+      <c r="K6" s="79">
         <v>3</v>
       </c>
-      <c r="N6" s="54" t="s">
+      <c r="M6" s="54" t="s">
         <v>121</v>
       </c>
+      <c r="N6" s="54">
+        <v>7</v>
+      </c>
       <c r="O6" s="54">
-        <v>7</v>
-      </c>
-      <c r="P6" s="54">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>44</v>
       </c>
@@ -4226,30 +4327,27 @@
         <v>127</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H7" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="I7" s="64" t="s">
-        <v>127</v>
-      </c>
-      <c r="J7" s="74" t="s">
+      <c r="I7" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="K7" s="27">
+      <c r="J7" s="27">
         <v>3</v>
       </c>
-      <c r="L7" s="72">
+      <c r="K7" s="72">
         <v>3</v>
       </c>
-      <c r="N7" s="54" t="s">
+      <c r="M7" s="54" t="s">
         <v>122</v>
       </c>
+      <c r="N7" s="54"/>
       <c r="O7" s="54"/>
-      <c r="P7" s="54"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>86</v>
       </c>
@@ -4263,40 +4361,37 @@
         <v>3</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>127</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H8" s="65" t="s">
         <v>127</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="J8" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="K8" s="27">
+        <v>145</v>
+      </c>
+      <c r="J8" s="27">
         <v>3</v>
       </c>
-      <c r="L8" s="72">
+      <c r="K8" s="72">
         <v>1</v>
       </c>
-      <c r="N8" s="54" t="s">
+      <c r="M8" s="54" t="s">
         <v>124</v>
       </c>
-      <c r="O8" s="54">
+      <c r="N8" s="54">
         <v>8</v>
       </c>
-      <c r="P8" s="79">
+      <c r="O8" s="79">
         <v>1.3</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>100</v>
       </c>
@@ -4310,40 +4405,37 @@
         <v>3</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H9" s="65" t="s">
         <v>127</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="J9" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="K9" s="27">
+      <c r="J9" s="27">
         <v>2</v>
       </c>
-      <c r="L9" s="72">
+      <c r="K9" s="72">
         <v>2</v>
       </c>
-      <c r="N9" s="54" t="s">
-        <v>147</v>
+      <c r="M9" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="N9" s="54">
+        <v>4</v>
       </c>
       <c r="O9" s="54">
-        <v>4</v>
-      </c>
-      <c r="P9" s="54">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>58</v>
       </c>
@@ -4369,28 +4461,25 @@
         <v>127</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="J10" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="K10" s="14">
+      <c r="J10" s="14">
         <v>2</v>
       </c>
-      <c r="L10" s="88">
+      <c r="K10" s="88">
         <v>2</v>
       </c>
-      <c r="N10" s="54" t="s">
+      <c r="M10" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="O10" s="54">
+      <c r="N10" s="54">
         <v>6</v>
       </c>
-      <c r="P10" s="79">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O10" s="79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="33"/>
       <c r="B11" s="3"/>
       <c r="C11" s="27"/>
@@ -4400,22 +4489,21 @@
       <c r="G11" s="27"/>
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="46"/>
-      <c r="N11" s="28" t="s">
+      <c r="J11" s="66"/>
+      <c r="K11" s="46"/>
+      <c r="M11" s="28" t="s">
         <v>135</v>
+      </c>
+      <c r="N11" s="28">
+        <f>SUM(N3:N10)</f>
+        <v>44</v>
       </c>
       <c r="O11" s="28">
         <f>SUM(O3:O10)</f>
-        <v>44</v>
-      </c>
-      <c r="P11" s="28">
-        <f>SUM(P3:P10)</f>
         <v>38.799999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="33"/>
       <c r="B12" s="3"/>
       <c r="C12" s="27"/>
@@ -4425,23 +4513,22 @@
       <c r="G12" s="27"/>
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27">
+      <c r="J12" s="27">
+        <f>SUM(J4:J10)</f>
+        <v>20</v>
+      </c>
+      <c r="K12" s="72">
         <f>SUM(K4:K10)</f>
-        <v>20</v>
-      </c>
-      <c r="L12" s="72">
-        <f>SUM(L4:L10)</f>
         <v>17.3</v>
       </c>
-      <c r="N12" s="63" t="s">
-        <v>143</v>
-      </c>
-      <c r="O12" s="63">
+      <c r="M12" s="63" t="s">
+        <v>142</v>
+      </c>
+      <c r="N12" s="63">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="33"/>
       <c r="B13" s="3"/>
       <c r="C13" s="27"/>
@@ -4452,18 +4539,17 @@
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="46"/>
-      <c r="O13" s="54"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N14" s="97" t="s">
+      <c r="K13" s="46"/>
+      <c r="N13" s="54"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M14" s="97" t="s">
         <v>102</v>
       </c>
+      <c r="N14" s="98"/>
       <c r="O14" s="98"/>
-      <c r="P14" s="98"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
       <c r="B15" s="3"/>
       <c r="C15" s="27"/>
@@ -4474,17 +4560,16 @@
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="46"/>
+      <c r="K15" s="46"/>
+      <c r="M15" s="54" t="s">
+        <v>103</v>
+      </c>
       <c r="N15" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="O15" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="P15" s="54"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O15" s="54"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
       <c r="B16" s="3"/>
       <c r="C16" s="27"/>
@@ -4495,17 +4580,16 @@
       <c r="H16" s="27"/>
       <c r="I16" s="27"/>
       <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="48"/>
-      <c r="N16" s="54" t="s">
+      <c r="K16" s="48"/>
+      <c r="M16" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="O16" s="54">
+      <c r="N16" s="54">
         <v>0</v>
       </c>
-      <c r="P16" s="54"/>
-    </row>
-    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O16" s="54"/>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="41"/>
       <c r="B17" s="42"/>
       <c r="C17" s="43"/>
@@ -4516,26 +4600,25 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="49"/>
-      <c r="N17" s="54" t="s">
+      <c r="K17" s="49"/>
+      <c r="M17" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="O17" s="54">
+      <c r="N17" s="54">
         <v>2</v>
       </c>
-      <c r="P17" s="54"/>
-    </row>
-    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N18" s="54" t="s">
+      <c r="O17" s="54"/>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M18" s="54" t="s">
         <v>128</v>
       </c>
-      <c r="O18" s="54">
-        <v>4</v>
-      </c>
-      <c r="P18" s="54"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N18" s="54">
+        <v>4</v>
+      </c>
+      <c r="O18" s="54"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="95" t="s">
         <v>137</v>
       </c>
@@ -4547,18 +4630,17 @@
       <c r="G19" s="96"/>
       <c r="H19" s="96"/>
       <c r="I19" s="96"/>
-      <c r="J19" s="96"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="30"/>
-      <c r="N19" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="O19" s="54">
+      <c r="J19" s="51"/>
+      <c r="K19" s="30"/>
+      <c r="M19" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="N19" s="54">
         <v>5</v>
       </c>
-      <c r="P19" s="54"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O19" s="54"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>0</v>
       </c>
@@ -4578,33 +4660,30 @@
         <v>141</v>
       </c>
       <c r="G20" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="H20" s="52" t="s">
         <v>148</v>
       </c>
-      <c r="H20" s="52" t="s">
-        <v>149</v>
-      </c>
-      <c r="I20" s="52" t="s">
-        <v>142</v>
+      <c r="I20" s="19" t="s">
+        <v>103</v>
       </c>
       <c r="J20" s="19" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="K20" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="L20" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="N20" s="28" t="s">
+      <c r="M20" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="O20" s="28">
-        <f>SUM(O16:O19)</f>
+      <c r="N20" s="28">
+        <f>SUM(N16:N19)</f>
         <v>11</v>
       </c>
-      <c r="P20" s="28"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O20" s="28"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
         <v>29</v>
       </c>
@@ -4624,25 +4703,22 @@
         <v>127</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H21" s="73" t="s">
         <v>127</v>
       </c>
-      <c r="I21" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="J21" s="27" t="s">
+      <c r="I21" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="K21" s="82">
+      <c r="J21" s="82">
         <v>3</v>
       </c>
-      <c r="L21" s="78">
+      <c r="K21" s="78">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
         <v>16</v>
       </c>
@@ -4662,25 +4738,22 @@
         <v>127</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H22" s="73" t="s">
         <v>127</v>
       </c>
-      <c r="I22" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="J22" s="7" t="s">
+      <c r="I22" s="7" t="s">
         <v>126</v>
+      </c>
+      <c r="J22" s="83">
+        <v>3</v>
       </c>
       <c r="K22" s="83">
         <v>3</v>
       </c>
-      <c r="L22" s="83">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="75" t="s">
         <v>13</v>
       </c>
@@ -4706,19 +4779,16 @@
         <v>127</v>
       </c>
       <c r="I23" s="71" t="s">
-        <v>127</v>
-      </c>
-      <c r="J23" s="71" t="s">
-        <v>146</v>
+        <v>145</v>
+      </c>
+      <c r="J23" s="84">
+        <v>2</v>
       </c>
       <c r="K23" s="84">
-        <v>2</v>
-      </c>
-      <c r="L23" s="84">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="67" t="s">
         <v>18</v>
       </c>
@@ -4746,17 +4816,14 @@
       <c r="I24" s="70" t="s">
         <v>127</v>
       </c>
-      <c r="J24" s="70" t="s">
-        <v>127</v>
+      <c r="J24" s="85">
+        <v>4</v>
       </c>
       <c r="K24" s="85">
-        <v>4</v>
-      </c>
-      <c r="L24" s="85">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
         <v>25</v>
       </c>
@@ -4776,25 +4843,22 @@
         <v>127</v>
       </c>
       <c r="G25" s="27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H25" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="I25" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="J25" s="47" t="s">
+      <c r="I25" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="K25" s="86">
-        <v>4</v>
-      </c>
-      <c r="L25" s="87">
+      <c r="J25" s="86">
+        <v>4</v>
+      </c>
+      <c r="K25" s="87">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
         <v>40</v>
       </c>
@@ -4814,25 +4878,22 @@
         <v>127</v>
       </c>
       <c r="G26" s="27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H26" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="I26" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="J26" s="46" t="s">
+      <c r="I26" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="K26" s="86">
+      <c r="J26" s="86">
         <v>6</v>
       </c>
-      <c r="L26" s="87">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K26" s="87">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
         <v>11</v>
       </c>
@@ -4852,25 +4913,22 @@
         <v>127</v>
       </c>
       <c r="G27" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H27" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="I27" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="J27" s="35" t="s">
+      <c r="I27" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="K27" s="82">
+      <c r="J27" s="82">
         <v>2</v>
       </c>
-      <c r="L27" s="83">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K27" s="83">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="41"/>
       <c r="B28" s="42"/>
       <c r="C28" s="43"/>
@@ -4879,23 +4937,22 @@
       <c r="F28" s="43"/>
       <c r="G28" s="43"/>
       <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="81">
+      <c r="I28" s="44"/>
+      <c r="J28" s="81">
         <v>24</v>
       </c>
-      <c r="L28" s="80">
-        <f>SUM(L21:L27)</f>
+      <c r="K28" s="80">
+        <f>SUM(K21:K27)</f>
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="A19:I19"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Pedro Silva] - Atualização da planilha.
</commit_message>
<xml_diff>
--- a/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
+++ b/Priorização de Casos de Uso, Incrementos e Responsabilidades.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
@@ -12,7 +12,7 @@
     <sheet name="Incremento 2" sheetId="3" r:id="rId3"/>
     <sheet name="Incremento 3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -1093,7 +1093,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1105,10 +1108,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1201,7 +1201,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1236,7 +1236,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1465,18 +1465,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="H1" s="94" t="s">
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="H1" s="90" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="94"/>
+      <c r="I1" s="90"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1606,21 +1606,21 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="90" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="91">
-        <v>4</v>
-      </c>
-      <c r="D7" s="91">
+      <c r="B7" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="92">
+        <v>4</v>
+      </c>
+      <c r="D7" s="92">
         <v>1</v>
       </c>
-      <c r="E7" s="91"/>
-      <c r="F7" s="92"/>
-      <c r="H7" s="94" t="s">
+      <c r="E7" s="92"/>
+      <c r="F7" s="93"/>
+      <c r="H7" s="90" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="94"/>
+      <c r="I7" s="90"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -1779,8 +1779,8 @@
       <c r="F13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="89"/>
-      <c r="K13" s="89"/>
+      <c r="J13" s="94"/>
+      <c r="K13" s="94"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1828,13 +1828,13 @@
       <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="90" t="s">
+      <c r="B16" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="91"/>
-      <c r="D16" s="91"/>
-      <c r="E16" s="91"/>
-      <c r="F16" s="92"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="93"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2046,13 +2046,13 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="90" t="s">
+      <c r="B27" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="91"/>
-      <c r="D27" s="91"/>
-      <c r="E27" s="91"/>
-      <c r="F27" s="92"/>
+      <c r="C27" s="92"/>
+      <c r="D27" s="92"/>
+      <c r="E27" s="92"/>
+      <c r="F27" s="93"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -2116,13 +2116,13 @@
       <c r="A31" s="9">
         <v>6</v>
       </c>
-      <c r="B31" s="90" t="s">
+      <c r="B31" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="91"/>
-      <c r="D31" s="91"/>
-      <c r="E31" s="91"/>
-      <c r="F31" s="92"/>
+      <c r="C31" s="92"/>
+      <c r="D31" s="92"/>
+      <c r="E31" s="92"/>
+      <c r="F31" s="93"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -2368,13 +2368,13 @@
       <c r="A47" s="9">
         <v>7</v>
       </c>
-      <c r="B47" s="90" t="s">
+      <c r="B47" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="91"/>
-      <c r="D47" s="91"/>
-      <c r="E47" s="91"/>
-      <c r="F47" s="92"/>
+      <c r="C47" s="92"/>
+      <c r="D47" s="92"/>
+      <c r="E47" s="92"/>
+      <c r="F47" s="93"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2492,13 +2492,13 @@
       <c r="A55" s="9">
         <v>8</v>
       </c>
-      <c r="B55" s="90" t="s">
+      <c r="B55" s="91" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="91"/>
-      <c r="D55" s="91"/>
-      <c r="E55" s="91"/>
-      <c r="F55" s="92"/>
+      <c r="C55" s="92"/>
+      <c r="D55" s="92"/>
+      <c r="E55" s="92"/>
+      <c r="F55" s="93"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -2566,16 +2566,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B55:F55"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B7:F7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B55:F55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2783,17 +2783,17 @@
       <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="90" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="91">
-        <v>4</v>
-      </c>
-      <c r="D7" s="91">
+      <c r="B7" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="92">
+        <v>4</v>
+      </c>
+      <c r="D7" s="92">
         <v>1</v>
       </c>
-      <c r="E7" s="91"/>
-      <c r="F7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="93"/>
       <c r="G7" s="40"/>
       <c r="I7" s="25" t="s">
         <v>122</v>
@@ -3822,22 +3822,22 @@
       <c r="A22" s="39">
         <v>3</v>
       </c>
-      <c r="B22" s="90" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="91">
-        <v>4</v>
-      </c>
-      <c r="D22" s="91">
+      <c r="B22" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="92">
+        <v>4</v>
+      </c>
+      <c r="D22" s="92">
         <v>1</v>
       </c>
-      <c r="E22" s="91"/>
-      <c r="F22" s="91"/>
-      <c r="G22" s="91"/>
-      <c r="H22" s="91"/>
-      <c r="I22" s="92"/>
-      <c r="J22" s="90"/>
-      <c r="K22" s="91"/>
+      <c r="E22" s="92"/>
+      <c r="F22" s="92"/>
+      <c r="G22" s="92"/>
+      <c r="H22" s="92"/>
+      <c r="I22" s="93"/>
+      <c r="J22" s="91"/>
+      <c r="K22" s="92"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -4065,8 +4065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4476,7 +4476,7 @@
         <v>6</v>
       </c>
       <c r="O10" s="79">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -4500,7 +4500,7 @@
       </c>
       <c r="O11" s="28">
         <f>SUM(O3:O10)</f>
-        <v>38.799999999999997</v>
+        <v>44.8</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -4889,8 +4889,8 @@
       <c r="J26" s="86">
         <v>6</v>
       </c>
-      <c r="K26" s="87">
-        <v>4</v>
+      <c r="K26" s="84">
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -4943,7 +4943,7 @@
       </c>
       <c r="K28" s="80">
         <f>SUM(K21:K27)</f>
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>